<commit_message>
updated excel con numericas
</commit_message>
<xml_diff>
--- a/mmp_info.xlsx
+++ b/mmp_info.xlsx
@@ -1,37 +1,49 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alinaoganesyan/Desktop/Master Data Science/Entregables/Trabajos/Repositorio entregable 2/Entregable_MMP/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\DataScience\Material didáctico\Ejercicios\Modelo_supervisado\Entregable_MMP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30224843-EF78-8940-AB35-D06D2DB9F6D0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A28B2DB-1739-42D4-B105-1DF8D71A5C48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28820" windowHeight="17500" xr2:uid="{16D500F6-5AD7-764E-8C39-1ED26FBE09BA}"/>
+    <workbookView xWindow="23880" yWindow="-7695" windowWidth="29040" windowHeight="15840" xr2:uid="{16D500F6-5AD7-764E-8C39-1ED26FBE09BA}"/>
   </bookViews>
   <sheets>
     <sheet name="INFO" sheetId="1" r:id="rId1"/>
-    <sheet name="Checklist" sheetId="3" r:id="rId2"/>
-    <sheet name="STATS" sheetId="2" r:id="rId3"/>
-    <sheet name="OBJECT" sheetId="4" r:id="rId4"/>
+    <sheet name="Hoja1" sheetId="5" r:id="rId2"/>
+    <sheet name="Checklist" sheetId="3" r:id="rId3"/>
+    <sheet name="STATS" sheetId="2" r:id="rId4"/>
+    <sheet name="OBJECT" sheetId="4" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">INFO!$A$1:$T$85</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="398">
   <si>
     <t>TIPO DATOS</t>
   </si>
@@ -1195,6 +1207,69 @@
   </si>
   <si>
     <t xml:space="preserve">Casi totas las 500K variables pertenecen a Retail. Eliminar por no aportar información? </t>
+  </si>
+  <si>
+    <t>Tiene 0.98 de correlación con Census_OS_OSInstallLanguageIdentifier</t>
+  </si>
+  <si>
+    <t>Tiene 0.98 de correlación con Census_OS_UIL Local identifier. ELIMINAR POR CORRELACION Y NULOS</t>
+  </si>
+  <si>
+    <t>Se correlaciona 0.93 con Census OSBuildNumber. Nosquedamos este ya que después de la distriución del violin plot vemos que la cantidad de registros por cada valor del target se distribuye mejor o más uniforme en la amplitud delk OsBuild.</t>
+  </si>
+  <si>
+    <t>Se correlaciona con OsBuild en 0.93. Eliminamos ya que vemos un comportamiento distinto en la distribución de registros extremos.</t>
+  </si>
+  <si>
+    <t>Se correlaciona -0.88 con SxSPassiveMode, se podría considerar eliminar aunque mejor no, porque no es tan alto. Los valores se concentran en 7 y 0. Los demas se podrían agrupar. El valor de 35 es claramente un outlier</t>
+  </si>
+  <si>
+    <t>Eliminar. Bool con todos los valores 0 excepto 1 valor (=1). Debido a la distribución del violin plot, solo un valor negativo de in beta te dice que está infectado x malware, por lo que no tiene sentido mantenerla.</t>
+  </si>
+  <si>
+    <t>Consultar a miguel si vale la pena mantener las categorias o agruparlas en others</t>
+  </si>
+  <si>
+    <t>Consultar a miguel como leer violinplots de bool vs bool o que visualizacion hacer</t>
+  </si>
+  <si>
+    <t>Como es ID de software, no pensamos que el valor numérico aporte valor al algoritmo (no tiene orden intrísneco) por lo tanto agrupamos según el num de ocurrencias desde 330000 hasta 1000 y después Others con los de menos ocurrencias.</t>
+  </si>
+  <si>
+    <t>Cambiar a categorica, crear others y crear NaN (No identificado)</t>
+  </si>
+  <si>
+    <t>Cambiar a categorica, NaN no identificado</t>
+  </si>
+  <si>
+    <t>* La gran mayoría de valores es cero y el target está equitativamente distribuido. El violin plot indica la distribución de datos en la variable continua. La rayida blanca es la mediana. El rectangulo gris te indica rango interquartílico, es decir Q1, Q2=mediana, Q3. Entre Q1-Q2 se agrupa la misma cantidad de datos que entre Q2 y Q3. Por lo tanto, cuanto más grande sea la rayita gris entre el extremo y mediana, querrá decir que hay mas dispersion entre los datos.. Si la rayita entre Q2 y extremo inferior es más corta, querrá que los datos estan menos dispersos, más concentrados.</t>
+  </si>
+  <si>
+    <t>Transformar a categórica AVPRODUCTINSTALLED_1</t>
+  </si>
+  <si>
+    <t>Transformar a categórica AVPRODUCTENABLED_1</t>
+  </si>
+  <si>
+    <t>Parece que esta equitativamente distriuida en la var tagret, que la gram mayoria de HasTpm se concentra en True(1).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transformar a categórica </t>
+  </si>
+  <si>
+    <t>ELiMINAR</t>
+  </si>
+  <si>
+    <t>Transformar a categórica (cortar por 1000 para hacer other en ocurrencia), la variable según target está equitativamente distribuida</t>
+  </si>
+  <si>
+    <t>Transformar a categorica (corte en 100)</t>
+  </si>
+  <si>
+    <t>Eliminar ya que tenemos el geolocalizador. los virus no se mueven limitados a city, además se entiende que en un país, la capital concentra más la digitalización , movimiento de virus y antivirus, por lo que es descriptiva la ciudad del país y se considera menos relevante.</t>
+  </si>
+  <si>
+    <t>Transformar a categórica o Eliminar</t>
   </si>
 </sst>
 </file>
@@ -1346,7 +1421,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1359,6 +1434,99 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>227771</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>132731</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8EEA819E-8C76-53BE-F29C-80DB037E0E16}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="304800" y="1181100"/>
+          <a:ext cx="6628571" cy="4952381"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>752475</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>218304</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>189919</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A09E677-0755-F505-B337-50E36CA8771B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7458075" y="1343025"/>
+          <a:ext cx="6171429" cy="4647619"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1680,30 +1848,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1355D624-ACBD-7B41-A30E-75FD1558C62F}">
   <dimension ref="A1:S85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F73" sqref="F73"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="85.1640625" style="7" customWidth="1"/>
-    <col min="2" max="2" width="18.33203125" style="7" customWidth="1"/>
+    <col min="1" max="1" width="85.125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="18.375" style="7" customWidth="1"/>
     <col min="3" max="3" width="46" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="13.1640625" style="7" customWidth="1"/>
-    <col min="7" max="7" width="14.1640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="61.33203125" style="7" customWidth="1"/>
+    <col min="4" max="6" width="13.125" style="7" customWidth="1"/>
+    <col min="7" max="7" width="14.125" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="61.375" style="7" customWidth="1"/>
     <col min="9" max="9" width="20" style="7" customWidth="1"/>
-    <col min="10" max="10" width="10.83203125" style="7"/>
-    <col min="11" max="11" width="16.83203125" style="15" customWidth="1"/>
-    <col min="12" max="12" width="19.33203125" style="16" customWidth="1"/>
-    <col min="13" max="13" width="22.83203125" style="7" customWidth="1"/>
-    <col min="14" max="18" width="10.83203125" style="7"/>
-    <col min="19" max="19" width="87.83203125" style="7" customWidth="1"/>
-    <col min="20" max="16384" width="10.83203125" style="7"/>
+    <col min="10" max="10" width="10.875" style="7"/>
+    <col min="11" max="11" width="16.875" style="15" customWidth="1"/>
+    <col min="12" max="12" width="19.375" style="16" customWidth="1"/>
+    <col min="13" max="13" width="22.875" style="7" customWidth="1"/>
+    <col min="14" max="18" width="10.875" style="7"/>
+    <col min="19" max="19" width="87.875" style="7" customWidth="1"/>
+    <col min="20" max="16384" width="10.875" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="13" customFormat="1" ht="17">
+    <row r="1" spans="1:19" s="13" customFormat="1" ht="15.75">
       <c r="A1" s="6" t="s">
         <v>211</v>
       </c>
@@ -1759,7 +1927,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="51">
+    <row r="2" spans="1:19" ht="30">
       <c r="A2" s="7" t="s">
         <v>212</v>
       </c>
@@ -1825,12 +1993,12 @@
         <f>VLOOKUP(C2,STATS!$A$1:$I$55,9,0)</f>
         <v>8921471000000</v>
       </c>
-      <c r="S2" s="7" t="e">
-        <f ca="1">_xlfn.CONCAT("- ","&lt;b&gt;",C2,": ","&lt;/b&gt;",A2,".  ")</f>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" ht="68">
+      <c r="S2" s="7" t="str">
+        <f>_xlfn.CONCAT("- ","&lt;b&gt;",C2,": ","&lt;/b&gt;",A2,".  ")</f>
+        <v xml:space="preserve">- &lt;b&gt;Unnamed: 0: &lt;/b&gt;index.  </v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="60">
       <c r="A3" s="7" t="s">
         <v>218</v>
       </c>
@@ -1894,12 +2062,12 @@
         <f>VLOOKUP(C3,STATS!$A$1:$I$55,9,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="S3" s="7" t="e">
-        <f t="shared" ref="S3:S66" ca="1" si="1">_xlfn.CONCAT("- ","&lt;b&gt;",C3,": ","&lt;/b&gt;",A3,".  ")</f>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" ht="102">
+      <c r="S3" s="7" t="str">
+        <f t="shared" ref="S3:S66" si="1">_xlfn.CONCAT("- ","&lt;b&gt;",C3,": ","&lt;/b&gt;",A3,".  ")</f>
+        <v xml:space="preserve">- &lt;b&gt;MachineIdentifier: &lt;/b&gt;Individual machine ID.  </v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="90">
       <c r="B4" s="7" t="s">
         <v>95</v>
       </c>
@@ -1961,11 +2129,11 @@
         <v>#N/A</v>
       </c>
       <c r="S4" s="7" t="e">
-        <f ca="1">_xlfn.CONCAT("- ","&lt;b&gt;",C4,": ","&lt;/b&gt;",#REF!,".  ")</f>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" ht="68">
+        <f>_xlfn.CONCAT("- ","&lt;b&gt;",C4,": ","&lt;/b&gt;",#REF!,".  ")</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="60">
       <c r="A5" s="7" t="s">
         <v>219</v>
       </c>
@@ -2029,12 +2197,12 @@
         <f>VLOOKUP(C5,STATS!$A$1:$I$55,9,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="S5" s="7" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" ht="51">
+      <c r="S5" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">- &lt;b&gt;EngineVersion: &lt;/b&gt;Defender state information e.g. 1.1.12603.0.  </v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="30">
       <c r="A6" s="7" t="s">
         <v>220</v>
       </c>
@@ -2098,12 +2266,12 @@
         <f>VLOOKUP(C6,STATS!$A$1:$I$55,9,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="S6" s="7" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" ht="34">
+      <c r="S6" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">- &lt;b&gt;AppVersion: &lt;/b&gt;Defender state information e.g. 4.9.10586.0.  </v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="30">
       <c r="A7" s="7" t="s">
         <v>221</v>
       </c>
@@ -2167,12 +2335,12 @@
         <f>VLOOKUP(C7,STATS!$A$1:$I$55,9,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="S7" s="7" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" ht="34">
+      <c r="S7" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">- &lt;b&gt;AvSigVersion: &lt;/b&gt;Defender state information e.g. 1.217.1014.0.  </v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="60">
       <c r="A8" s="7" t="s">
         <v>222</v>
       </c>
@@ -2192,7 +2360,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G8" s="14"/>
+      <c r="G8" s="14" t="s">
+        <v>350</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>382</v>
+      </c>
       <c r="I8" s="7" t="e">
         <f>VLOOKUP(C8,OBJECT!A:C,3,FALSE)</f>
         <v>#N/A</v>
@@ -2233,12 +2406,12 @@
         <f>VLOOKUP(C8,STATS!$A$1:$I$55,9,0)</f>
         <v>1000000</v>
       </c>
-      <c r="S8" s="7" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" ht="17">
+      <c r="S8" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">- &lt;b&gt;IsBeta: &lt;/b&gt;Defender state information e.g. false.  </v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="105">
       <c r="A9" s="7" t="s">
         <v>306</v>
       </c>
@@ -2258,7 +2431,12 @@
         <f t="shared" si="0"/>
         <v>3.6640000000000002E-3</v>
       </c>
-      <c r="G9" s="14"/>
+      <c r="G9" s="14" t="s">
+        <v>383</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>381</v>
+      </c>
       <c r="I9" s="7" t="e">
         <f>VLOOKUP(C9,OBJECT!A:C,3,FALSE)</f>
         <v>#N/A</v>
@@ -2299,12 +2477,12 @@
         <f>VLOOKUP(C9,STATS!$A$1:$I$55,9,0)</f>
         <v>35000000</v>
       </c>
-      <c r="S9" s="7" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" ht="51">
+      <c r="S9" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">- &lt;b&gt;RtpStateBitfield: &lt;/b&gt;RTP state: Realtime protection state (Enabled or Disabled).  </v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="150">
       <c r="A10" s="7" t="s">
         <v>307</v>
       </c>
@@ -2324,7 +2502,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G10" s="14"/>
+      <c r="G10" s="14" t="s">
+        <v>384</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>388</v>
+      </c>
       <c r="I10" s="7" t="e">
         <f>VLOOKUP(C10,OBJECT!A:C,3,FALSE)</f>
         <v>#N/A</v>
@@ -2365,12 +2548,12 @@
         <f>VLOOKUP(C10,STATS!$A$1:$I$55,9,0)</f>
         <v>1000000</v>
       </c>
-      <c r="S10" s="7" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" ht="17">
+      <c r="S10" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">- &lt;b&gt;IsSxsPassiveMode: &lt;/b&gt;active/passive mode of operation for Windows Defender. If another third party primary antivirus exists on the system, the Defender enters Passive mode. Passive mode obviously offers reduced functionality.  </v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="15.75">
       <c r="A11" s="7" t="s">
         <v>224</v>
       </c>
@@ -2436,12 +2619,12 @@
         <f>VLOOKUP(C11,STATS!$A$1:$I$55,9,0)</f>
         <v>3209000000</v>
       </c>
-      <c r="S11" s="7" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" ht="17">
+      <c r="S11" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">- &lt;b&gt;DefaultBrowsersIdentifier: &lt;/b&gt;ID for the machine's default browser.  </v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" ht="75">
       <c r="A12" s="7" t="s">
         <v>225</v>
       </c>
@@ -2461,7 +2644,12 @@
         <f t="shared" si="0"/>
         <v>3.8760000000000001E-3</v>
       </c>
-      <c r="G12" s="14"/>
+      <c r="G12" s="14" t="s">
+        <v>386</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>385</v>
+      </c>
       <c r="I12" s="7" t="e">
         <f>VLOOKUP(C12,OBJECT!A:C,3,FALSE)</f>
         <v>#N/A</v>
@@ -2502,12 +2690,12 @@
         <f>VLOOKUP(C12,STATS!$A$1:$I$55,9,0)</f>
         <v>70492000000</v>
       </c>
-      <c r="S12" s="7" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" ht="17">
+      <c r="S12" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">- &lt;b&gt;AVProductStatesIdentifier: &lt;/b&gt;ID for the specific configuration of a user's antivirus software.  </v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" ht="60">
       <c r="A13" s="7" t="s">
         <v>309</v>
       </c>
@@ -2527,7 +2715,12 @@
         <f t="shared" si="0"/>
         <v>3.8760000000000001E-3</v>
       </c>
-      <c r="G13" s="14"/>
+      <c r="G13" s="14" t="s">
+        <v>387</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>389</v>
+      </c>
       <c r="I13" s="7" t="e">
         <f>VLOOKUP(C13,OBJECT!A:C,3,FALSE)</f>
         <v>#N/A</v>
@@ -2568,12 +2761,12 @@
         <f>VLOOKUP(C13,STATS!$A$1:$I$55,9,0)</f>
         <v>5000000</v>
       </c>
-      <c r="S13" s="7" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" ht="17">
+      <c r="S13" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">- &lt;b&gt;AVProductsInstalled: &lt;/b&gt;Active anti-virus of the total installed.  </v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" ht="60">
       <c r="A14" s="7" t="s">
         <v>308</v>
       </c>
@@ -2593,7 +2786,12 @@
         <f t="shared" si="0"/>
         <v>3.8760000000000001E-3</v>
       </c>
-      <c r="G14" s="14"/>
+      <c r="G14" s="14" t="s">
+        <v>387</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>390</v>
+      </c>
       <c r="I14" s="7" t="e">
         <f>VLOOKUP(C14,OBJECT!A:C,3,FALSE)</f>
         <v>#N/A</v>
@@ -2634,12 +2832,12 @@
         <f>VLOOKUP(C14,STATS!$A$1:$I$55,9,0)</f>
         <v>4000000</v>
       </c>
-      <c r="S14" s="7" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" ht="17">
+      <c r="S14" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">- &lt;b&gt;AVProductsEnabled: &lt;/b&gt;Of the installed antiviruses, those that are active.  </v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" ht="30">
       <c r="A15" s="7" t="s">
         <v>226</v>
       </c>
@@ -2660,6 +2858,9 @@
         <v>0</v>
       </c>
       <c r="G15" s="14"/>
+      <c r="H15" s="7" t="s">
+        <v>391</v>
+      </c>
       <c r="I15" s="7" t="e">
         <f>VLOOKUP(C15,OBJECT!A:C,3,FALSE)</f>
         <v>#N/A</v>
@@ -2700,12 +2901,12 @@
         <f>VLOOKUP(C15,STATS!$A$1:$I$55,9,0)</f>
         <v>1000000</v>
       </c>
-      <c r="S15" s="7" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" ht="17">
+      <c r="S15" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">- &lt;b&gt;HasTpm: &lt;/b&gt;True if machine has tpm.  </v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" ht="75">
       <c r="A16" s="7" t="s">
         <v>227</v>
       </c>
@@ -2725,7 +2926,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G16" s="14"/>
+      <c r="G16" s="14" t="s">
+        <v>350</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>396</v>
+      </c>
       <c r="I16" s="7" t="e">
         <f>VLOOKUP(C16,OBJECT!A:C,3,FALSE)</f>
         <v>#N/A</v>
@@ -2766,12 +2972,12 @@
         <f>VLOOKUP(C16,STATS!$A$1:$I$55,9,0)</f>
         <v>222000000</v>
       </c>
-      <c r="S16" s="7" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" ht="17">
+      <c r="S16" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">- &lt;b&gt;CountryIdentifier: &lt;/b&gt;ID for the country the machine is located in.  </v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" ht="75">
       <c r="A17" s="7" t="s">
         <v>228</v>
       </c>
@@ -2791,7 +2997,12 @@
         <f t="shared" si="0"/>
         <v>3.6479999999999999E-2</v>
       </c>
-      <c r="G17" s="14"/>
+      <c r="G17" s="14" t="s">
+        <v>393</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>396</v>
+      </c>
       <c r="I17" s="7" t="e">
         <f>VLOOKUP(C17,OBJECT!A:C,3,FALSE)</f>
         <v>#N/A</v>
@@ -2832,12 +3043,12 @@
         <f>VLOOKUP(C17,STATS!$A$1:$I$55,9,0)</f>
         <v>167958000000</v>
       </c>
-      <c r="S17" s="7" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" ht="34">
+      <c r="S17" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">- &lt;b&gt;CityIdentifier: &lt;/b&gt;ID for the city the machine is located in.  </v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" ht="60">
       <c r="A18" s="7" t="s">
         <v>229</v>
       </c>
@@ -2857,7 +3068,12 @@
         <f t="shared" si="0"/>
         <v>0.30912600000000001</v>
       </c>
-      <c r="G18" s="14"/>
+      <c r="G18" s="14" t="s">
+        <v>387</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>394</v>
+      </c>
       <c r="I18" s="7" t="e">
         <f>VLOOKUP(C18,OBJECT!A:C,3,FALSE)</f>
         <v>#N/A</v>
@@ -2898,12 +3114,12 @@
         <f>VLOOKUP(C18,STATS!$A$1:$I$55,9,0)</f>
         <v>52000000</v>
       </c>
-      <c r="S18" s="7" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19" ht="17">
+      <c r="S18" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">- &lt;b&gt;OrganizationIdentifier: &lt;/b&gt;ID for the organization the machine belongs in, organization ID is mapped to both specific companies and broad industries.  </v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" ht="45">
       <c r="A19" s="7" t="s">
         <v>230</v>
       </c>
@@ -2923,7 +3139,12 @@
         <f t="shared" si="0"/>
         <v>3.1999999999999999E-5</v>
       </c>
-      <c r="G19" s="14"/>
+      <c r="G19" s="14" t="s">
+        <v>395</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>392</v>
+      </c>
       <c r="I19" s="7" t="e">
         <f>VLOOKUP(C19,OBJECT!A:C,3,FALSE)</f>
         <v>#N/A</v>
@@ -2964,12 +3185,12 @@
         <f>VLOOKUP(C19,STATS!$A$1:$I$55,9,0)</f>
         <v>296000000</v>
       </c>
-      <c r="S19" s="7" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19" ht="17">
+      <c r="S19" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">- &lt;b&gt;GeoNameIdentifier: &lt;/b&gt;ID for the geographic region a machine is located in.  </v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" ht="45">
       <c r="A20" s="7" t="s">
         <v>231</v>
       </c>
@@ -2989,7 +3210,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G20" s="14"/>
+      <c r="G20" s="14" t="s">
+        <v>395</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>397</v>
+      </c>
       <c r="I20" s="7" t="e">
         <f>VLOOKUP(C20,OBJECT!A:C,3,FALSE)</f>
         <v>#N/A</v>
@@ -3030,12 +3256,12 @@
         <f>VLOOKUP(C20,STATS!$A$1:$I$55,9,0)</f>
         <v>283000000</v>
       </c>
-      <c r="S20" s="7" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19" ht="68">
+      <c r="S20" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">- &lt;b&gt;LocaleEnglishNameIdentifier: &lt;/b&gt;English name of Locale ID of the current user.  </v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" ht="45">
       <c r="A21" s="7" t="s">
         <v>232</v>
       </c>
@@ -3099,12 +3325,12 @@
         <f>VLOOKUP(C21,STATS!$A$1:$I$55,9,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="S21" s="7" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="22" spans="1:19" ht="102">
+      <c r="S21" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">- &lt;b&gt;Platform: &lt;/b&gt;Calculates platform name (of OS related properties and processor property).  </v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" ht="90">
       <c r="A22" s="7" t="s">
         <v>233</v>
       </c>
@@ -3168,12 +3394,12 @@
         <f>VLOOKUP(C22,STATS!$A$1:$I$55,9,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="S22" s="7" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="23" spans="1:19" ht="51">
+      <c r="S22" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">- &lt;b&gt;Processor: &lt;/b&gt;This is the process architecture of the installed operating system.  </v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" ht="45">
       <c r="A23" s="7" t="s">
         <v>234</v>
       </c>
@@ -3237,12 +3463,12 @@
         <f>VLOOKUP(C23,STATS!$A$1:$I$55,9,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="S23" s="7" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="24" spans="1:19" ht="17">
+      <c r="S23" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">- &lt;b&gt;OsVer: &lt;/b&gt;Version of the current operating system.  </v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" ht="60">
       <c r="A24" s="7" t="s">
         <v>235</v>
       </c>
@@ -3263,6 +3489,9 @@
         <v>0</v>
       </c>
       <c r="G24" s="14"/>
+      <c r="H24" s="7" t="s">
+        <v>379</v>
+      </c>
       <c r="I24" s="7" t="e">
         <f>VLOOKUP(C24,OBJECT!A:C,3,FALSE)</f>
         <v>#N/A</v>
@@ -3303,12 +3532,12 @@
         <f>VLOOKUP(C24,STATS!$A$1:$I$55,9,0)</f>
         <v>18242000000</v>
       </c>
-      <c r="S24" s="7" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="25" spans="1:19" ht="17">
+      <c r="S24" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">- &lt;b&gt;OsBuild: &lt;/b&gt;Build of the current operating system.  </v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" ht="15.75">
       <c r="A25" s="7" t="s">
         <v>236</v>
       </c>
@@ -3369,12 +3598,12 @@
         <f>VLOOKUP(C25,STATS!$A$1:$I$55,9,0)</f>
         <v>784000000</v>
       </c>
-      <c r="S25" s="7" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="26" spans="1:19" ht="85">
+      <c r="S25" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">- &lt;b&gt;OsSuite: &lt;/b&gt;Product suite mask for the current operating system..  </v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" ht="60">
       <c r="A26" s="7" t="s">
         <v>237</v>
       </c>
@@ -3438,12 +3667,12 @@
         <f>VLOOKUP(C26,STATS!$A$1:$I$55,9,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="S26" s="7" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="27" spans="1:19" ht="85">
+      <c r="S26" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">- &lt;b&gt;OsPlatformSubRelease: &lt;/b&gt;Returns the OS Platform sub.  </v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" ht="75">
       <c r="A27" s="7" t="s">
         <v>238</v>
       </c>
@@ -3507,12 +3736,12 @@
         <f>VLOOKUP(C27,STATS!$A$1:$I$55,9,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="S27" s="7" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="28" spans="1:19" ht="90">
+      <c r="S27" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">- &lt;b&gt;OsBuildLab: &lt;/b&gt;Build lab that generated the current OS. Example: 9600.17630.amd64fre.winblue_r7.150109.  </v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" ht="82.5">
       <c r="A28" s="7" t="s">
         <v>277</v>
       </c>
@@ -3576,12 +3805,12 @@
         <f>VLOOKUP(C28,STATS!$A$1:$I$55,9,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="S28" s="7" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="29" spans="1:19" ht="34">
+      <c r="S28" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">- &lt;b&gt;SkuEdition: &lt;/b&gt;The goal of this feature is to use the Product Type defined in the MSDN (Microsoft Developer Network) to map to a SKU (Stock Keeping Unit).  </v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" ht="30">
       <c r="A29" s="7" t="s">
         <v>239</v>
       </c>
@@ -3642,12 +3871,12 @@
         <f>VLOOKUP(C29,STATS!$A$1:$I$55,9,0)</f>
         <v>1000000</v>
       </c>
-      <c r="S29" s="7" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="30" spans="1:19" ht="34">
+      <c r="S29" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">- &lt;b&gt;IsProtected: &lt;/b&gt;This is a calculated field derived from the Spynet Report's AV Products field. Returns: a. TRUE if there is at least one active and up.  </v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" ht="30">
       <c r="A30" s="7" t="s">
         <v>240</v>
       </c>
@@ -3708,12 +3937,12 @@
         <f>VLOOKUP(C30,STATS!$A$1:$I$55,9,0)</f>
         <v>1000000</v>
       </c>
-      <c r="S30" s="7" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="31" spans="1:19" ht="17">
+      <c r="S30" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">- &lt;b&gt;AutoSampleOptIn: &lt;/b&gt;This is the SubmitSamplesConsent value passed in from the service, available on CAMP 9+.  </v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" ht="15.75">
       <c r="A31" s="7" t="s">
         <v>241</v>
       </c>
@@ -3779,12 +4008,12 @@
         <f>VLOOKUP(C31,STATS!$A$1:$I$55,9,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="S31" s="7" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="32" spans="1:19" ht="34">
+      <c r="S31" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">- &lt;b&gt;PuaMode: &lt;/b&gt;Pua Enabled mode from the service.  </v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" ht="30">
       <c r="A32" s="7" t="s">
         <v>242</v>
       </c>
@@ -3845,12 +4074,12 @@
         <f>VLOOKUP(C32,STATS!$A$1:$I$55,9,0)</f>
         <v>1000000</v>
       </c>
-      <c r="S32" s="7" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="33" spans="1:19" ht="17">
+      <c r="S32" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">- &lt;b&gt;SMode: &lt;/b&gt;This field is set to true when the device is known to be in 'S Mode', as in, Windows 10 S mode, where only Microsoft Store apps can be installed.  </v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" ht="15.75">
       <c r="A33" s="7" t="s">
         <v>310</v>
       </c>
@@ -3911,12 +4140,12 @@
         <f>VLOOKUP(C33,STATS!$A$1:$I$55,9,0)</f>
         <v>429000000</v>
       </c>
-      <c r="S33" s="7" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="34" spans="1:19" ht="136">
+      <c r="S33" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">- &lt;b&gt;IeVerIdentifier: &lt;/b&gt;Retrieves which version of Internet Explorer is running on this device.  </v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" ht="121.5">
       <c r="A34" s="7" t="s">
         <v>243</v>
       </c>
@@ -3982,12 +4211,12 @@
         <f>VLOOKUP(C34,STATS!$A$1:$I$55,9,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="S34" s="7" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="35" spans="1:19" ht="34">
+      <c r="S34" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">- &lt;b&gt;SmartScreen: &lt;/b&gt;This is the SmartScreen enabled string value from registry. This is obtained by checking in order, HKLM\SOFTWARE\Policies\Microsoft\Windows\System\SmartScreenEnabled and HKLM\SOFTWARE\Microsoft\Windows\CurrentVersion\Explorer\SmartScreenEnabled. If the value exists but is blank, the value "ExistsNotSet" is sent in telemetry..  </v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" ht="30">
       <c r="A35" s="7" t="s">
         <v>244</v>
       </c>
@@ -4048,12 +4277,12 @@
         <f>VLOOKUP(C35,STATS!$A$1:$I$55,9,0)</f>
         <v>1000000</v>
       </c>
-      <c r="S35" s="7" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="36" spans="1:19" ht="51">
+      <c r="S35" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">- &lt;b&gt;Firewall: &lt;/b&gt;This attribute is true (1) for Windows 8.1 and above if windows firewall is enabled, as reported by the service..  </v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" ht="45">
       <c r="A36" s="7" t="s">
         <v>245</v>
       </c>
@@ -4114,12 +4343,12 @@
         <f>VLOOKUP(C36,STATS!$A$1:$I$55,9,0)</f>
         <v>6357062000000</v>
       </c>
-      <c r="S36" s="7" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="37" spans="1:19" ht="85">
+      <c r="S36" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">- &lt;b&gt;UacLuaenable: &lt;/b&gt;This attribute reports whether or not the "administrator in Admin Approval Mode" user type is disabled or enabled in UAC. The value reported is obtained by reading the regkey HKLM\SOFTWARE\Microsoft\Windows\CurrentVersion\Policies\System\EnableLUA..  </v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" ht="75">
       <c r="A37" s="7" t="s">
         <v>246</v>
       </c>
@@ -4183,12 +4412,12 @@
         <f>VLOOKUP(C37,STATS!$A$1:$I$55,9,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="S37" s="7" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="38" spans="1:19" ht="68">
+      <c r="S37" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">- &lt;b&gt;Census_MDC2FormFactor: &lt;/b&gt;A grouping based on a combination of Device Census level hardware characteristics. The logic used to define Form Factor is rooted in business and industry standards and aligns with how people think about their device. (Examples: Smartphone, Small Tablet, All in One, Convertible...).  </v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" ht="60">
       <c r="A38" s="7" t="s">
         <v>247</v>
       </c>
@@ -4252,12 +4481,12 @@
         <f>VLOOKUP(C38,STATS!$A$1:$I$55,9,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="S38" s="7" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="39" spans="1:19" ht="17">
+      <c r="S38" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">- &lt;b&gt;Census_DeviceFamily: &lt;/b&gt;AKA DeviceClass. Indicates the type of device that an edition of the OS is intended for. Example values: Windows.Desktop, Windows.Mobile, and iOS.Phone.  </v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" ht="15.75">
       <c r="A39" s="7" t="s">
         <v>223</v>
       </c>
@@ -4318,12 +4547,12 @@
         <f>VLOOKUP(C39,STATS!$A$1:$I$55,9,0)</f>
         <v>6143000000</v>
       </c>
-      <c r="S39" s="7" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="40" spans="1:19" ht="34">
+      <c r="S39" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">- &lt;b&gt;Census_OEMNameIdentifier: &lt;/b&gt;NA.  </v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" ht="15.75">
       <c r="A40" s="7" t="s">
         <v>223</v>
       </c>
@@ -4384,12 +4613,12 @@
         <f>VLOOKUP(C40,STATS!$A$1:$I$55,9,0)</f>
         <v>345493000000</v>
       </c>
-      <c r="S40" s="7" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="41" spans="1:19" ht="17">
+      <c r="S40" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">- &lt;b&gt;Census_OEMModelIdentifier: &lt;/b&gt;NA.  </v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" ht="15.75">
       <c r="A41" s="7" t="s">
         <v>248</v>
       </c>
@@ -4450,12 +4679,12 @@
         <f>VLOOKUP(C41,STATS!$A$1:$I$55,9,0)</f>
         <v>88000000</v>
       </c>
-      <c r="S41" s="7" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="42" spans="1:19" ht="17">
+      <c r="S41" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">- &lt;b&gt;Census_ProcessorCoreCount: &lt;/b&gt;Number of logical cores in the processor.  </v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" ht="15.75">
       <c r="A42" s="7" t="s">
         <v>223</v>
       </c>
@@ -4516,12 +4745,12 @@
         <f>VLOOKUP(C42,STATS!$A$1:$I$55,9,0)</f>
         <v>10000000</v>
       </c>
-      <c r="S42" s="7" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="43" spans="1:19" ht="17">
+      <c r="S42" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">- &lt;b&gt;Census_ProcessorManufacturerIdentifier: &lt;/b&gt;NA.  </v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" ht="15.75">
       <c r="A43" s="7" t="s">
         <v>223</v>
       </c>
@@ -4582,12 +4811,12 @@
         <f>VLOOKUP(C43,STATS!$A$1:$I$55,9,0)</f>
         <v>4472000000</v>
       </c>
-      <c r="S43" s="7" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="44" spans="1:19" ht="34">
+      <c r="S43" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">- &lt;b&gt;Census_ProcessorModelIdentifier: &lt;/b&gt;NA.  </v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" ht="30">
       <c r="A44" s="7" t="s">
         <v>249</v>
       </c>
@@ -4653,12 +4882,12 @@
         <f>VLOOKUP(C44,STATS!$A$1:$I$55,9,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="S44" s="7" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="45" spans="1:19" ht="34">
+      <c r="S44" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">- &lt;b&gt;Census_ProcessorClass: &lt;/b&gt;A classification of processors into high/medium/low. Initially used for Pricing Level SKU. No longer maintained and updated.  </v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" ht="15.75">
       <c r="A45" s="7" t="s">
         <v>215</v>
       </c>
@@ -4719,12 +4948,12 @@
         <f>VLOOKUP(C45,STATS!$A$1:$I$55,9,0)</f>
         <v>47687670000000</v>
       </c>
-      <c r="S45" s="7" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="46" spans="1:19" ht="51">
+      <c r="S45" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">- &lt;b&gt;Census_PrimaryDiskTotalCapacity: &lt;/b&gt;Amount of disk space on primary disk of the machine in MB.  </v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" ht="45">
       <c r="A46" s="7" t="s">
         <v>216</v>
       </c>
@@ -4788,12 +5017,12 @@
         <f>VLOOKUP(C46,STATS!$A$1:$I$55,9,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="S46" s="7" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="47" spans="1:19" ht="34">
+      <c r="S46" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">- &lt;b&gt;Census_PrimaryDiskTypeName: &lt;/b&gt;Friendly name of Primary Disk Type .  </v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" ht="15.75">
       <c r="A47" s="7" t="s">
         <v>217</v>
       </c>
@@ -4854,12 +5083,12 @@
         <f>VLOOKUP(C47,STATS!$A$1:$I$55,9,0)</f>
         <v>47687100000000</v>
       </c>
-      <c r="S47" s="7" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="48" spans="1:19" ht="34">
+      <c r="S47" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">- &lt;b&gt;Census_SystemVolumeTotalCapacity: &lt;/b&gt;The size of the partition that the System volume is installed on in MB.  </v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" ht="30">
       <c r="A48" s="7" t="s">
         <v>250</v>
       </c>
@@ -4920,12 +5149,12 @@
         <f>VLOOKUP(C48,STATS!$A$1:$I$55,9,0)</f>
         <v>1000000</v>
       </c>
-      <c r="S48" s="7" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="49" spans="1:19" ht="17">
+      <c r="S48" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">- &lt;b&gt;Census_HasOpticalDiskDrive: &lt;/b&gt;True indicates that the machine has an optical disk drive (CD/DVD).  </v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" ht="15.75">
       <c r="A49" s="7" t="s">
         <v>251</v>
       </c>
@@ -4986,12 +5215,12 @@
         <f>VLOOKUP(C49,STATS!$A$1:$I$55,9,0)</f>
         <v>393216000000</v>
       </c>
-      <c r="S49" s="7" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="50" spans="1:19" ht="51">
+      <c r="S49" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">- &lt;b&gt;Census_TotalPhysicalRAM: &lt;/b&gt;Retrieves the physical RAM in MB.  </v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" ht="45">
       <c r="A50" s="7" t="s">
         <v>252</v>
       </c>
@@ -5055,12 +5284,12 @@
         <f>VLOOKUP(C50,STATS!$A$1:$I$55,9,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="S50" s="7" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="51" spans="1:19" ht="34">
+      <c r="S50" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">- &lt;b&gt;Census_ChassisTypeName: &lt;/b&gt;Retrieves a numeric representation of what type of chassis the machine has. A value of 0 means xx.  </v>
+      </c>
+    </row>
+    <row r="51" spans="1:19" ht="31.5">
       <c r="A51" s="7" t="s">
         <v>253</v>
       </c>
@@ -5121,12 +5350,12 @@
         <f>VLOOKUP(C51,STATS!$A$1:$I$55,9,0)</f>
         <v>142000000</v>
       </c>
-      <c r="S51" s="7" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="52" spans="1:19" ht="34">
+      <c r="S51" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">- &lt;b&gt;Census_InternalPrimaryDiagonalDisplaySizeInInches: &lt;/b&gt;Retrieves the physical diagonal length in inches of the primary display.  </v>
+      </c>
+    </row>
+    <row r="52" spans="1:19" ht="31.5">
       <c r="A52" s="7" t="s">
         <v>254</v>
       </c>
@@ -5187,12 +5416,12 @@
         <f>VLOOKUP(C52,STATS!$A$1:$I$55,9,0)</f>
         <v>11520000000</v>
       </c>
-      <c r="S52" s="7" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="53" spans="1:19" ht="34">
+      <c r="S52" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">- &lt;b&gt;Census_InternalPrimaryDisplayResolutionHorizontal: &lt;/b&gt;Retrieves the number of pixels in the horizontal direction of the internal display..  </v>
+      </c>
+    </row>
+    <row r="53" spans="1:19" ht="31.5">
       <c r="A53" s="7" t="s">
         <v>255</v>
       </c>
@@ -5253,12 +5482,12 @@
         <f>VLOOKUP(C53,STATS!$A$1:$I$55,9,0)</f>
         <v>4320000000</v>
       </c>
-      <c r="S53" s="7" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="54" spans="1:19" ht="51">
+      <c r="S53" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">- &lt;b&gt;Census_InternalPrimaryDisplayResolutionVertical: &lt;/b&gt;Retrieves the number of pixels in the vertical direction of the internal display.  </v>
+      </c>
+    </row>
+    <row r="54" spans="1:19" ht="45">
       <c r="A54" s="7" t="s">
         <v>214</v>
       </c>
@@ -5322,12 +5551,12 @@
         <f>VLOOKUP(C54,STATS!$A$1:$I$55,9,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="S54" s="7" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="55" spans="1:19" ht="68">
+      <c r="S54" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">- &lt;b&gt;Census_PowerPlatformRoleName: &lt;/b&gt;Indicates the OEM preferred power management profile. This value helps identify the basic form factor of the device.  </v>
+      </c>
+    </row>
+    <row r="55" spans="1:19" ht="60">
       <c r="A55" s="7" t="s">
         <v>223</v>
       </c>
@@ -5391,12 +5620,12 @@
         <f>VLOOKUP(C55,STATS!$A$1:$I$55,9,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="S55" s="7" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="56" spans="1:19" ht="17">
+      <c r="S55" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">- &lt;b&gt;Census_InternalBatteryType: &lt;/b&gt;NA.  </v>
+      </c>
+    </row>
+    <row r="56" spans="1:19" ht="15.75">
       <c r="A56" s="7" t="s">
         <v>223</v>
       </c>
@@ -5457,12 +5686,12 @@
         <f>VLOOKUP(C56,STATS!$A$1:$I$55,9,0)</f>
         <v>4294967000000000</v>
       </c>
-      <c r="S56" s="7" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="57" spans="1:19" ht="34">
+      <c r="S56" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">- &lt;b&gt;Census_InternalBatteryNumberOfCharges: &lt;/b&gt;NA.  </v>
+      </c>
+    </row>
+    <row r="57" spans="1:19" ht="30">
       <c r="A57" s="7" t="s">
         <v>256</v>
       </c>
@@ -5526,12 +5755,12 @@
         <f>VLOOKUP(C57,STATS!$A$1:$I$55,9,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="S57" s="7" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="58" spans="1:19" ht="85">
+      <c r="S57" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">- &lt;b&gt;Census_OSVersion: &lt;/b&gt;Numeric OS version Example .  </v>
+      </c>
+    </row>
+    <row r="58" spans="1:19" ht="75">
       <c r="A58" s="7" t="s">
         <v>257</v>
       </c>
@@ -5595,12 +5824,12 @@
         <f>VLOOKUP(C58,STATS!$A$1:$I$55,9,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="S58" s="7" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="59" spans="1:19" ht="85">
+      <c r="S58" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">- &lt;b&gt;Census_OSArchitecture: &lt;/b&gt;Architecture on which the OS is based. Derived from OSVersionFull. Example .  </v>
+      </c>
+    </row>
+    <row r="59" spans="1:19" ht="75">
       <c r="A59" s="7" t="s">
         <v>258</v>
       </c>
@@ -5664,12 +5893,12 @@
         <f>VLOOKUP(C59,STATS!$A$1:$I$55,9,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="S59" s="7" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="60" spans="1:19" ht="17">
+      <c r="S59" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">- &lt;b&gt;Census_OSBranch: &lt;/b&gt;Branch of the OS extracted from the OsVersionFull. Example .  </v>
+      </c>
+    </row>
+    <row r="60" spans="1:19" ht="30">
       <c r="A60" s="7" t="s">
         <v>259</v>
       </c>
@@ -5690,6 +5919,9 @@
         <v>0</v>
       </c>
       <c r="G60" s="14"/>
+      <c r="H60" s="7" t="s">
+        <v>380</v>
+      </c>
       <c r="I60" s="7" t="e">
         <f>VLOOKUP(C60,OBJECT!A:C,3,FALSE)</f>
         <v>#N/A</v>
@@ -5730,12 +5962,12 @@
         <f>VLOOKUP(C60,STATS!$A$1:$I$55,9,0)</f>
         <v>18242000000</v>
       </c>
-      <c r="S60" s="7" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="61" spans="1:19" ht="17">
+      <c r="S60" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">- &lt;b&gt;Census_OSBuildNumber: &lt;/b&gt;OS Build number extracted from the OsVersionFull. Example .  </v>
+      </c>
+    </row>
+    <row r="61" spans="1:19" ht="15.75">
       <c r="A61" s="7" t="s">
         <v>260</v>
       </c>
@@ -5796,12 +6028,12 @@
         <f>VLOOKUP(C61,STATS!$A$1:$I$55,9,0)</f>
         <v>19069000000</v>
       </c>
-      <c r="S61" s="7" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="62" spans="1:19" ht="68">
+      <c r="S61" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">- &lt;b&gt;Census_OSBuildRevision: &lt;/b&gt;OS Build revision extracted from the OsVersionFull. Example .  </v>
+      </c>
+    </row>
+    <row r="62" spans="1:19" ht="60">
       <c r="A62" s="7" t="s">
         <v>261</v>
       </c>
@@ -5865,12 +6097,12 @@
         <f>VLOOKUP(C62,STATS!$A$1:$I$55,9,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="S62" s="7" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="63" spans="1:19" ht="51">
+      <c r="S62" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">- &lt;b&gt;Census_OSEdition: &lt;/b&gt;Edition of the current OS. Sourced from HKLM\Software\Microsoft\Windows NT\CurrentVersion@EditionID in registry. Example: Enterprise.  </v>
+      </c>
+    </row>
+    <row r="63" spans="1:19" ht="45">
       <c r="A63" s="7" t="s">
         <v>262</v>
       </c>
@@ -5934,12 +6166,12 @@
         <f>VLOOKUP(C63,STATS!$A$1:$I$55,9,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="S63" s="7" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="64" spans="1:19" ht="51">
+      <c r="S63" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">- &lt;b&gt;Census_OSSkuName: &lt;/b&gt;OS edition friendly name (currently Windows only).  </v>
+      </c>
+    </row>
+    <row r="64" spans="1:19" ht="45">
       <c r="A64" s="7" t="s">
         <v>263</v>
       </c>
@@ -6003,12 +6235,12 @@
         <f>VLOOKUP(C64,STATS!$A$1:$I$55,9,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="S64" s="7" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="65" spans="1:19" ht="17">
+      <c r="S64" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">- &lt;b&gt;Census_OSInstallTypeName: &lt;/b&gt;Friendly description of what install was used on the machine i.e. clean.  </v>
+      </c>
+    </row>
+    <row r="65" spans="1:19" ht="30">
       <c r="A65" s="7" t="s">
         <v>223</v>
       </c>
@@ -6028,7 +6260,12 @@
         <f t="shared" si="0"/>
         <v>6.6639999999999998E-3</v>
       </c>
-      <c r="G65" s="14"/>
+      <c r="G65" s="14" t="s">
+        <v>350</v>
+      </c>
+      <c r="H65" s="7" t="s">
+        <v>378</v>
+      </c>
       <c r="I65" s="7" t="e">
         <f>VLOOKUP(C65,OBJECT!A:C,3,FALSE)</f>
         <v>#N/A</v>
@@ -6069,12 +6306,12 @@
         <f>VLOOKUP(C65,STATS!$A$1:$I$55,9,0)</f>
         <v>39000000</v>
       </c>
-      <c r="S65" s="7" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="66" spans="1:19" ht="17">
+      <c r="S65" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">- &lt;b&gt;Census_OSInstallLanguageIdentifier: &lt;/b&gt;NA.  </v>
+      </c>
+    </row>
+    <row r="66" spans="1:19" ht="30">
       <c r="A66" s="7" t="s">
         <v>223</v>
       </c>
@@ -6095,6 +6332,9 @@
         <v>0</v>
       </c>
       <c r="G66" s="14"/>
+      <c r="H66" s="7" t="s">
+        <v>377</v>
+      </c>
       <c r="I66" s="7" t="e">
         <f>VLOOKUP(C66,OBJECT!A:C,3,FALSE)</f>
         <v>#N/A</v>
@@ -6135,12 +6375,12 @@
         <f>VLOOKUP(C66,STATS!$A$1:$I$55,9,0)</f>
         <v>162000000</v>
       </c>
-      <c r="S66" s="7" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="67" spans="1:19" ht="68">
+      <c r="S66" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">- &lt;b&gt;Census_OSUILocaleIdentifier: &lt;/b&gt;NA.  </v>
+      </c>
+    </row>
+    <row r="67" spans="1:19" ht="60">
       <c r="A67" s="7" t="s">
         <v>264</v>
       </c>
@@ -6204,12 +6444,12 @@
         <f>VLOOKUP(C67,STATS!$A$1:$I$55,9,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="S67" s="7" t="e">
-        <f t="shared" ref="S67:S85" ca="1" si="3">_xlfn.CONCAT("- ","&lt;b&gt;",C67,": ","&lt;/b&gt;",A67,".  ")</f>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="68" spans="1:19" ht="34">
+      <c r="S67" s="7" t="str">
+        <f t="shared" ref="S67:S85" si="3">_xlfn.CONCAT("- ","&lt;b&gt;",C67,": ","&lt;/b&gt;",A67,".  ")</f>
+        <v xml:space="preserve">- &lt;b&gt;Census_OSWUAutoUpdateOptionsName: &lt;/b&gt;Friendly name of the WindowsUpdate auto.  </v>
+      </c>
+    </row>
+    <row r="68" spans="1:19" ht="30">
       <c r="A68" s="7" t="s">
         <v>265</v>
       </c>
@@ -6270,12 +6510,12 @@
         <f>VLOOKUP(C68,STATS!$A$1:$I$55,9,0)</f>
         <v>1000000</v>
       </c>
-      <c r="S68" s="7" t="e">
-        <f t="shared" ca="1" si="3"/>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="69" spans="1:19" ht="34">
+      <c r="S68" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">- &lt;b&gt;Census_IsPortableOperatingSystem: &lt;/b&gt;Indicates whether OS is booted up and running via Windows.  </v>
+      </c>
+    </row>
+    <row r="69" spans="1:19" ht="30">
       <c r="A69" s="7" t="s">
         <v>266</v>
       </c>
@@ -6339,12 +6579,12 @@
         <f>VLOOKUP(C69,STATS!$A$1:$I$55,9,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="S69" s="7" t="e">
-        <f t="shared" ca="1" si="3"/>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="70" spans="1:19" ht="51">
+      <c r="S69" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">- &lt;b&gt;Census_GenuineStateName: &lt;/b&gt;Friendly name of OSGenuineStateID. 0 = Genuine.  </v>
+      </c>
+    </row>
+    <row r="70" spans="1:19" ht="30">
       <c r="A70" s="7" t="s">
         <v>267</v>
       </c>
@@ -6408,12 +6648,12 @@
         <f>VLOOKUP(C70,STATS!$A$1:$I$55,9,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="S70" s="7" t="e">
-        <f t="shared" ca="1" si="3"/>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="71" spans="1:19" ht="51">
+      <c r="S70" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">- &lt;b&gt;Census_ActivationChannel: &lt;/b&gt;Retail license key or Volume license key for a machine..  </v>
+      </c>
+    </row>
+    <row r="71" spans="1:19" ht="45">
       <c r="A71" s="7" t="s">
         <v>311</v>
       </c>
@@ -6479,12 +6719,12 @@
         <f>VLOOKUP(C71,STATS!$A$1:$I$55,9,0)</f>
         <v>1000000</v>
       </c>
-      <c r="S71" s="7" t="e">
-        <f t="shared" ca="1" si="3"/>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="72" spans="1:19" ht="34">
+      <c r="S71" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">- &lt;b&gt;Census_IsFlightingInternal: &lt;/b&gt;Flighting' in Windows Defender context means making new development features available as soon as possible, during the development cycle. This does not refer to a public release. The 'internal' most likely means the Window Insider community.  </v>
+      </c>
+    </row>
+    <row r="72" spans="1:19" ht="30">
       <c r="A72" s="7" t="s">
         <v>268</v>
       </c>
@@ -6545,12 +6785,12 @@
         <f>VLOOKUP(C72,STATS!$A$1:$I$55,9,0)</f>
         <v>1000000</v>
       </c>
-      <c r="S72" s="7" t="e">
-        <f t="shared" ca="1" si="3"/>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="73" spans="1:19" ht="51">
+      <c r="S72" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">- &lt;b&gt;Census_IsFlightsDisabled: &lt;/b&gt;Indicates if the machine is participating in flighting..  </v>
+      </c>
+    </row>
+    <row r="73" spans="1:19" ht="45">
       <c r="A73" s="7" t="s">
         <v>269</v>
       </c>
@@ -6614,12 +6854,12 @@
         <f>VLOOKUP(C73,STATS!$A$1:$I$55,9,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="S73" s="7" t="e">
-        <f t="shared" ca="1" si="3"/>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="74" spans="1:19" ht="34">
+      <c r="S73" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">- &lt;b&gt;Census_FlightRing: &lt;/b&gt;The ring that the device user would like to receive flights for. This might be different from the ring of the OS which is currently installed if the user changes the ring after getting a flight from a different ring..  </v>
+      </c>
+    </row>
+    <row r="74" spans="1:19" ht="30">
       <c r="A74" s="7" t="s">
         <v>223</v>
       </c>
@@ -6680,12 +6920,12 @@
         <f>VLOOKUP(C74,STATS!$A$1:$I$55,9,0)</f>
         <v>1000000</v>
       </c>
-      <c r="S74" s="7" t="e">
-        <f t="shared" ca="1" si="3"/>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="75" spans="1:19" ht="17">
+      <c r="S74" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">- &lt;b&gt;Census_ThresholdOptIn: &lt;/b&gt;NA.  </v>
+      </c>
+    </row>
+    <row r="75" spans="1:19" ht="15.75">
       <c r="A75" s="7" t="s">
         <v>223</v>
       </c>
@@ -6746,12 +6986,12 @@
         <f>VLOOKUP(C75,STATS!$A$1:$I$55,9,0)</f>
         <v>1084000000</v>
       </c>
-      <c r="S75" s="7" t="e">
-        <f t="shared" ca="1" si="3"/>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="76" spans="1:19" ht="17">
+      <c r="S75" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">- &lt;b&gt;Census_FirmwareManufacturerIdentifier: &lt;/b&gt;NA.  </v>
+      </c>
+    </row>
+    <row r="76" spans="1:19" ht="15.75">
       <c r="A76" s="7" t="s">
         <v>223</v>
       </c>
@@ -6812,12 +7052,12 @@
         <f>VLOOKUP(C76,STATS!$A$1:$I$55,9,0)</f>
         <v>72091000000</v>
       </c>
-      <c r="S76" s="7" t="e">
-        <f t="shared" ca="1" si="3"/>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="77" spans="1:19" ht="34">
+      <c r="S76" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">- &lt;b&gt;Census_FirmwareVersionIdentifier: &lt;/b&gt;NA.  </v>
+      </c>
+    </row>
+    <row r="77" spans="1:19" ht="30">
       <c r="A77" s="7" t="s">
         <v>276</v>
       </c>
@@ -6878,12 +7118,12 @@
         <f>VLOOKUP(C77,STATS!$A$1:$I$55,9,0)</f>
         <v>1000000</v>
       </c>
-      <c r="S77" s="7" t="e">
-        <f t="shared" ca="1" si="3"/>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="78" spans="1:19" ht="34">
+      <c r="S77" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">- &lt;b&gt;Census_IsSecureBootEnabled: &lt;/b&gt;Indicates if Secure Boot mode is enabled. Secure Boot is a security measure to protect against malware during early system startup..  </v>
+      </c>
+    </row>
+    <row r="78" spans="1:19" ht="30">
       <c r="A78" s="7" t="s">
         <v>275</v>
       </c>
@@ -6949,12 +7189,12 @@
         <f>VLOOKUP(C78,STATS!$A$1:$I$55,9,0)</f>
         <v>0.000000e+00</v>
       </c>
-      <c r="S78" s="7" t="e">
-        <f t="shared" ca="1" si="3"/>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="79" spans="1:19" ht="34">
+      <c r="S78" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">- &lt;b&gt;Census_IsWIMBootEnabled: &lt;/b&gt;wimboot is a boot loader for Windows Imaging Format .wim files. It enables you to boot into a Windows PE (WinPE) deployment or recovery environment..  </v>
+      </c>
+    </row>
+    <row r="79" spans="1:19" ht="30">
       <c r="A79" s="7" t="s">
         <v>270</v>
       </c>
@@ -7015,12 +7255,12 @@
         <f>VLOOKUP(C79,STATS!$A$1:$I$55,9,0)</f>
         <v>1000000</v>
       </c>
-      <c r="S79" s="7" t="e">
-        <f t="shared" ca="1" si="3"/>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="80" spans="1:19" ht="34">
+      <c r="S79" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">- &lt;b&gt;Census_IsVirtualDevice: &lt;/b&gt;Identifies a Virtual Machine (machine learning model).  </v>
+      </c>
+    </row>
+    <row r="80" spans="1:19" ht="30">
       <c r="A80" s="7" t="s">
         <v>271</v>
       </c>
@@ -7081,12 +7321,12 @@
         <f>VLOOKUP(C80,STATS!$A$1:$I$55,9,0)</f>
         <v>1000000</v>
       </c>
-      <c r="S80" s="7" t="e">
-        <f t="shared" ca="1" si="3"/>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="81" spans="1:19" ht="34">
+      <c r="S80" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">- &lt;b&gt;Census_IsTouchEnabled: &lt;/b&gt;Is this a touch device ?.  </v>
+      </c>
+    </row>
+    <row r="81" spans="1:19" ht="30">
       <c r="A81" s="7" t="s">
         <v>272</v>
       </c>
@@ -7147,12 +7387,12 @@
         <f>VLOOKUP(C81,STATS!$A$1:$I$55,9,0)</f>
         <v>1000000</v>
       </c>
-      <c r="S81" s="7" t="e">
-        <f t="shared" ca="1" si="3"/>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="82" spans="1:19" ht="34">
+      <c r="S81" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">- &lt;b&gt;Census_IsPenCapable: &lt;/b&gt;Is the device capable of pen input ?.  </v>
+      </c>
+    </row>
+    <row r="82" spans="1:19" ht="31.5">
       <c r="A82" s="7" t="s">
         <v>273</v>
       </c>
@@ -7213,12 +7453,12 @@
         <f>VLOOKUP(C82,STATS!$A$1:$I$55,9,0)</f>
         <v>1000000</v>
       </c>
-      <c r="S82" s="7" t="e">
-        <f t="shared" ca="1" si="3"/>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="83" spans="1:19" ht="17">
+      <c r="S82" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">- &lt;b&gt;Census_IsAlwaysOnAlwaysConnectedCapable: &lt;/b&gt;Retreives information about whether the battery enables the device to be AlwaysOnAlwaysConnected.  </v>
+      </c>
+    </row>
+    <row r="83" spans="1:19" ht="30">
       <c r="A83" s="7" t="s">
         <v>274</v>
       </c>
@@ -7279,12 +7519,12 @@
         <f>VLOOKUP(C83,STATS!$A$1:$I$55,9,0)</f>
         <v>1000000</v>
       </c>
-      <c r="S83" s="7" t="e">
-        <f t="shared" ca="1" si="3"/>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="84" spans="1:19" ht="17">
+      <c r="S83" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">- &lt;b&gt;Wdft_IsGamer: &lt;/b&gt;Indicates whether the device is a gamer device or not based on its hardware combination..  </v>
+      </c>
+    </row>
+    <row r="84" spans="1:19" ht="15.75">
       <c r="A84" s="7" t="s">
         <v>312</v>
       </c>
@@ -7345,12 +7585,12 @@
         <f>VLOOKUP(C84,STATS!$A$1:$I$55,9,0)</f>
         <v>15000000</v>
       </c>
-      <c r="S84" s="7" t="e">
-        <f t="shared" ca="1" si="3"/>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="85" spans="1:19" ht="17">
+      <c r="S84" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">- &lt;b&gt;Wdft_RegionIdentifier: &lt;/b&gt;Region id code.  </v>
+      </c>
+    </row>
+    <row r="85" spans="1:19" ht="15.75">
       <c r="A85" s="10" t="s">
         <v>213</v>
       </c>
@@ -7414,9 +7654,9 @@
         <f>VLOOKUP(C85,STATS!$A$1:$I$55,9,0)</f>
         <v>1000000</v>
       </c>
-      <c r="S85" s="7" t="e">
-        <f t="shared" ca="1" si="3"/>
-        <v>#NAME?</v>
+      <c r="S85" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">- &lt;b&gt;HasDetections: &lt;/b&gt;indicates that Malware was detected on the machine.  </v>
       </c>
     </row>
   </sheetData>
@@ -7427,18 +7667,33 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C71567D1-A77B-4416-8352-A30CB3D12592}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63F36F59-B644-4A4B-A18E-D4BF69C056EB}">
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="20.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="43" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -7565,7 +7820,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D5B25CC-CABB-DE4A-98FC-468330853C12}">
   <dimension ref="A1:I55"/>
   <sheetViews>
@@ -7573,13 +7828,13 @@
       <selection activeCell="C74" sqref="C74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="51.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="51.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.875" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -9184,7 +9439,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51A459D5-AB12-FD47-8576-BFB8DC08FAD4}">
   <dimension ref="A1:E31"/>
   <sheetViews>
@@ -9192,10 +9447,10 @@
       <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="39.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">

</xml_diff>

<commit_message>
updated excel of numeric categories complete
</commit_message>
<xml_diff>
--- a/mmp_info.xlsx
+++ b/mmp_info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\DataScience\Material didáctico\Ejercicios\Modelo_supervisado\Entregable_MMP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{735E15F6-69E3-4CF2-B9B7-78828DD0314C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4840A020-0EB8-4E19-B5C3-304C846056F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="23880" yWindow="-7695" windowWidth="29040" windowHeight="15840" xr2:uid="{16D500F6-5AD7-764E-8C39-1ED26FBE09BA}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="776" uniqueCount="442">
   <si>
     <t>TIPO DATOS</t>
   </si>
@@ -1209,9 +1209,6 @@
     <t xml:space="preserve">Casi totas las 500K variables pertenecen a Retail. Eliminar por no aportar información? </t>
   </si>
   <si>
-    <t>Tiene 0.98 de correlación con Census_OS_OSInstallLanguageIdentifier</t>
-  </si>
-  <si>
     <t>Tiene 0.98 de correlación con Census_OS_UIL Local identifier. ELIMINAR POR CORRELACION Y NULOS</t>
   </si>
   <si>
@@ -1270,6 +1267,141 @@
   </si>
   <si>
     <t>Transformar a categórica o Eliminar</t>
+  </si>
+  <si>
+    <t>Cambiar a categórica. NaN como no dientidicado</t>
+  </si>
+  <si>
+    <t>Distribución categórica. Cambio a categoria con OHE</t>
+  </si>
+  <si>
+    <t>Poner -1 o algun valor extremo a NaN</t>
+  </si>
+  <si>
+    <t>Pasar NaN a un valor random. Debería ser bool</t>
+  </si>
+  <si>
+    <t>Pasar NaN a un valor random. Debería ser bool. La mayoría de Census es 0, pero cuando es 1, se comporta de forma diferencial sobre la infección.</t>
+  </si>
+  <si>
+    <t>Distribución bastante equiparable.</t>
+  </si>
+  <si>
+    <t>Debería ser bool. Suele ser census cero. Se comporta diferente sobre HasDetections dependiendo de si es Census 1 o 0</t>
+  </si>
+  <si>
+    <t>Convertir NaN a valor random, por ejemplo -1</t>
+  </si>
+  <si>
+    <t>Debería ser bool. Hay más cantidad de 1 en Has detection cuando el census es cero</t>
+  </si>
+  <si>
+    <t>es bool. Comportamiento similar para el target.</t>
+  </si>
+  <si>
+    <t>FreqE</t>
+  </si>
+  <si>
+    <t>Es un identificador con números, debería ser categórico ya que no tiene ningún orden. Hay muchos valores así que FreqE</t>
+  </si>
+  <si>
+    <t>Comportamiento similar con respecto al target. Es bool pero la mayoría son NaN</t>
+  </si>
+  <si>
+    <t>Transformar NaN a un valor random, pe -1</t>
+  </si>
+  <si>
+    <t>Hay solo 7 valores 1(True), los demás son cero y NaN. Quizás conviene convertir los NaN a un valor random p.e. -1</t>
+  </si>
+  <si>
+    <t>Transformar NaN a valor -1 o qualquier random, solo tiene 7 Trues… quizás eliminar ya que podría aprender?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bool, la ayoria son False o cero. </t>
+  </si>
+  <si>
+    <t>OHE</t>
+  </si>
+  <si>
+    <t>Tiene 0.98 de correlación con Census_OS_OSInstallLanguageIdentifier, Es un identificador, por lo tanto, una variable categórica. OHE para transformar los números que son menos de 100</t>
+  </si>
+  <si>
+    <t>Freq Encoding</t>
+  </si>
+  <si>
+    <t>Es  OS Build revision extracted from the OsVersionFull. Example - OsBuildRevision = 1000 or 16458. Que quiere decir esto? Es redundante?</t>
+  </si>
+  <si>
+    <t>No creo que el numero de recargas de la batería aporte mucha información sobre el número de cargas de la batería aporte info sobre la infección de malware. Sin embargio puede contener información de la cantidad de uso del pc. Entiendo que es una variable que tiene sentido que sea numérica, indicando el número de veces, por lo que el modelo cortará por donde lo crea conveniente.</t>
+  </si>
+  <si>
+    <t>Parece que se comporta de forma diferencial respecto al target. Osniste en el numero de pixels. Llega a tener muchos valores así que al ser numeral el modelo ya determinará donde hacer los cortes.</t>
+  </si>
+  <si>
+    <t>Es igual a las de abajo?</t>
+  </si>
+  <si>
+    <t>Substituir NAN con un valor random.</t>
+  </si>
+  <si>
+    <t>Se comporta de forma muy diferencial respecto al target. RAM en MB. Numerica contínua, va de 0 a 400000.</t>
+  </si>
+  <si>
+    <t>Bool. Distribucion bastante similar con respecto al target</t>
+  </si>
+  <si>
+    <t>Numérica, se comporta de forma diferencial respecto al target. Existen NaN</t>
+  </si>
+  <si>
+    <t>Substituir NaN con valor random, negativo?</t>
+  </si>
+  <si>
+    <t>Se comporta dde forma diferencial con respecto al target. Es numeral (int)</t>
+  </si>
+  <si>
+    <t>Categórica, FrequEncoding</t>
+  </si>
+  <si>
+    <t>FreqEncoding</t>
+  </si>
+  <si>
+    <t>Categórica, OHE, NaN con valor random No identificado</t>
+  </si>
+  <si>
+    <t>OHE, Convertir NaN a no identificado</t>
+  </si>
+  <si>
+    <t>Numérica, convertir NaN a un valor random</t>
+  </si>
+  <si>
+    <t>Convertir NaN a un valor random -1</t>
+  </si>
+  <si>
+    <t>Es identificador, convertir a Categórica, FreqEncoding</t>
+  </si>
+  <si>
+    <t>Parece que hay un outlier 6357062.00. No entiendo muy bien que es este valor. Tiene NaN, quizá se podría hacer categoría otros para incluirlo.</t>
+  </si>
+  <si>
+    <t>NaN=-1</t>
+  </si>
+  <si>
+    <t>Poner valor random a NaN. Se comportan de forma parecida respecto al target.</t>
+  </si>
+  <si>
+    <t>Es identificador, convertir a Categórica, FreqEncoding, NaN pasar a valor random</t>
+  </si>
+  <si>
+    <t>Poner valor random a NaN. La mayoría son ceros, solo hay 206 True de 469950 False</t>
+  </si>
+  <si>
+    <t>Poner valor random a NaN. La mayoría son ceros, solo hay 14 True de 499986False</t>
+  </si>
+  <si>
+    <t>Se comportan de forma diferencial. Hay NaN</t>
+  </si>
+  <si>
+    <t>Es categórica, pasar valor a categórico con OHE</t>
   </si>
 </sst>
 </file>
@@ -1848,9 +1980,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1355D624-ACBD-7B41-A30E-75FD1558C62F}">
   <dimension ref="A1:S85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15"/>
@@ -2364,7 +2496,7 @@
         <v>350</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="I8" s="7" t="e">
         <f>VLOOKUP(C8,OBJECT!A:C,3,FALSE)</f>
@@ -2432,10 +2564,10 @@
         <v>3.6640000000000002E-3</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="I9" s="7" t="e">
         <f>VLOOKUP(C9,OBJECT!A:C,3,FALSE)</f>
@@ -2503,10 +2635,10 @@
         <v>0</v>
       </c>
       <c r="G10" s="14" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="I10" s="7" t="e">
         <f>VLOOKUP(C10,OBJECT!A:C,3,FALSE)</f>
@@ -2645,10 +2777,10 @@
         <v>3.8760000000000001E-3</v>
       </c>
       <c r="G12" s="14" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="I12" s="7" t="e">
         <f>VLOOKUP(C12,OBJECT!A:C,3,FALSE)</f>
@@ -2716,10 +2848,10 @@
         <v>3.8760000000000001E-3</v>
       </c>
       <c r="G13" s="14" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="I13" s="7" t="e">
         <f>VLOOKUP(C13,OBJECT!A:C,3,FALSE)</f>
@@ -2787,10 +2919,10 @@
         <v>3.8760000000000001E-3</v>
       </c>
       <c r="G14" s="14" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="I14" s="7" t="e">
         <f>VLOOKUP(C14,OBJECT!A:C,3,FALSE)</f>
@@ -2859,7 +2991,7 @@
       </c>
       <c r="G15" s="14"/>
       <c r="H15" s="7" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="I15" s="7" t="e">
         <f>VLOOKUP(C15,OBJECT!A:C,3,FALSE)</f>
@@ -2930,7 +3062,7 @@
         <v>350</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="I16" s="7" t="e">
         <f>VLOOKUP(C16,OBJECT!A:C,3,FALSE)</f>
@@ -2998,10 +3130,10 @@
         <v>3.6479999999999999E-2</v>
       </c>
       <c r="G17" s="14" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="I17" s="7" t="e">
         <f>VLOOKUP(C17,OBJECT!A:C,3,FALSE)</f>
@@ -3069,10 +3201,10 @@
         <v>0.30912600000000001</v>
       </c>
       <c r="G18" s="14" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="I18" s="7" t="e">
         <f>VLOOKUP(C18,OBJECT!A:C,3,FALSE)</f>
@@ -3140,10 +3272,10 @@
         <v>3.1999999999999999E-5</v>
       </c>
       <c r="G19" s="14" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="I19" s="7" t="e">
         <f>VLOOKUP(C19,OBJECT!A:C,3,FALSE)</f>
@@ -3211,10 +3343,10 @@
         <v>0</v>
       </c>
       <c r="G20" s="14" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="I20" s="7" t="e">
         <f>VLOOKUP(C20,OBJECT!A:C,3,FALSE)</f>
@@ -3490,7 +3622,7 @@
       </c>
       <c r="G24" s="14"/>
       <c r="H24" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="I24" s="7" t="e">
         <f>VLOOKUP(C24,OBJECT!A:C,3,FALSE)</f>
@@ -3557,7 +3689,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G25" s="14"/>
+      <c r="G25" s="14" t="s">
+        <v>414</v>
+      </c>
+      <c r="H25" s="7" t="s">
+        <v>441</v>
+      </c>
       <c r="I25" s="7" t="e">
         <f>VLOOKUP(C25,OBJECT!A:C,3,FALSE)</f>
         <v>#N/A</v>
@@ -3830,7 +3967,12 @@
         <f t="shared" si="0"/>
         <v>3.852E-3</v>
       </c>
-      <c r="G29" s="14"/>
+      <c r="G29" s="14" t="s">
+        <v>435</v>
+      </c>
+      <c r="H29" s="7" t="s">
+        <v>440</v>
+      </c>
       <c r="I29" s="7" t="e">
         <f>VLOOKUP(C29,OBJECT!A:C,3,FALSE)</f>
         <v>#N/A</v>
@@ -3897,6 +4039,9 @@
         <v>0</v>
       </c>
       <c r="G30" s="14"/>
+      <c r="H30" s="7" t="s">
+        <v>439</v>
+      </c>
       <c r="I30" s="7" t="e">
         <f>VLOOKUP(C30,OBJECT!A:C,3,FALSE)</f>
         <v>#N/A</v>
@@ -4033,7 +4178,12 @@
         <f t="shared" si="0"/>
         <v>5.9695999999999999E-2</v>
       </c>
-      <c r="G32" s="14"/>
+      <c r="G32" s="14" t="s">
+        <v>435</v>
+      </c>
+      <c r="H32" s="7" t="s">
+        <v>438</v>
+      </c>
       <c r="I32" s="7" t="e">
         <f>VLOOKUP(C32,OBJECT!A:C,3,FALSE)</f>
         <v>#N/A</v>
@@ -4079,7 +4229,7 @@
         <v xml:space="preserve">- &lt;b&gt;SMode: &lt;/b&gt;This field is set to true when the device is known to be in 'S Mode', as in, Windows 10 S mode, where only Microsoft Store apps can be installed.  </v>
       </c>
     </row>
-    <row r="33" spans="1:19" ht="15.75">
+    <row r="33" spans="1:19" ht="30">
       <c r="A33" s="7" t="s">
         <v>310</v>
       </c>
@@ -4099,7 +4249,12 @@
         <f t="shared" si="0"/>
         <v>6.4180000000000001E-3</v>
       </c>
-      <c r="G33" s="14"/>
+      <c r="G33" s="14" t="s">
+        <v>416</v>
+      </c>
+      <c r="H33" s="7" t="s">
+        <v>437</v>
+      </c>
       <c r="I33" s="7" t="e">
         <f>VLOOKUP(C33,OBJECT!A:C,3,FALSE)</f>
         <v>#N/A</v>
@@ -4236,7 +4391,12 @@
         <f t="shared" si="0"/>
         <v>1.0324E-2</v>
       </c>
-      <c r="G35" s="14"/>
+      <c r="G35" s="14" t="s">
+        <v>435</v>
+      </c>
+      <c r="H35" s="7" t="s">
+        <v>436</v>
+      </c>
       <c r="I35" s="7" t="e">
         <f>VLOOKUP(C35,OBJECT!A:C,3,FALSE)</f>
         <v>#N/A</v>
@@ -4303,6 +4463,9 @@
         <v>1.2459999999999999E-3</v>
       </c>
       <c r="G36" s="14"/>
+      <c r="H36" s="7" t="s">
+        <v>434</v>
+      </c>
       <c r="I36" s="7" t="e">
         <f>VLOOKUP(C36,OBJECT!A:C,3,FALSE)</f>
         <v>#N/A</v>
@@ -4506,7 +4669,12 @@
         <f t="shared" si="0"/>
         <v>1.0762000000000001E-2</v>
       </c>
-      <c r="G39" s="14"/>
+      <c r="G39" s="14" t="s">
+        <v>416</v>
+      </c>
+      <c r="H39" s="7" t="s">
+        <v>433</v>
+      </c>
       <c r="I39" s="7" t="e">
         <f>VLOOKUP(C39,OBJECT!A:C,3,FALSE)</f>
         <v>#N/A</v>
@@ -4572,7 +4740,12 @@
         <f t="shared" si="0"/>
         <v>1.1528E-2</v>
       </c>
-      <c r="G40" s="14"/>
+      <c r="G40" s="14" t="s">
+        <v>416</v>
+      </c>
+      <c r="H40" s="7" t="s">
+        <v>433</v>
+      </c>
       <c r="I40" s="7" t="e">
         <f>VLOOKUP(C40,OBJECT!A:C,3,FALSE)</f>
         <v>#N/A</v>
@@ -4618,7 +4791,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_OEMModelIdentifier: &lt;/b&gt;NA.  </v>
       </c>
     </row>
-    <row r="41" spans="1:19" ht="15.75">
+    <row r="41" spans="1:19" ht="45">
       <c r="A41" s="7" t="s">
         <v>248</v>
       </c>
@@ -4638,7 +4811,12 @@
         <f t="shared" si="0"/>
         <v>4.6940000000000003E-3</v>
       </c>
-      <c r="G41" s="14"/>
+      <c r="G41" s="14" t="s">
+        <v>432</v>
+      </c>
+      <c r="H41" s="7" t="s">
+        <v>431</v>
+      </c>
       <c r="I41" s="7" t="e">
         <f>VLOOKUP(C41,OBJECT!A:C,3,FALSE)</f>
         <v>#N/A</v>
@@ -4684,7 +4862,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_ProcessorCoreCount: &lt;/b&gt;Number of logical cores in the processor.  </v>
       </c>
     </row>
-    <row r="42" spans="1:19" ht="15.75">
+    <row r="42" spans="1:19" ht="60">
       <c r="A42" s="7" t="s">
         <v>223</v>
       </c>
@@ -4704,7 +4882,12 @@
         <f t="shared" si="0"/>
         <v>4.6940000000000003E-3</v>
       </c>
-      <c r="G42" s="14"/>
+      <c r="G42" s="14" t="s">
+        <v>430</v>
+      </c>
+      <c r="H42" s="7" t="s">
+        <v>429</v>
+      </c>
       <c r="I42" s="7" t="e">
         <f>VLOOKUP(C42,OBJECT!A:C,3,FALSE)</f>
         <v>#N/A</v>
@@ -4770,7 +4953,12 @@
         <f t="shared" si="0"/>
         <v>4.6979999999999999E-3</v>
       </c>
-      <c r="G43" s="14"/>
+      <c r="G43" s="14" t="s">
+        <v>428</v>
+      </c>
+      <c r="H43" s="7" t="s">
+        <v>427</v>
+      </c>
       <c r="I43" s="7" t="e">
         <f>VLOOKUP(C43,OBJECT!A:C,3,FALSE)</f>
         <v>#N/A</v>
@@ -4887,7 +5075,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_ProcessorClass: &lt;/b&gt;A classification of processors into high/medium/low. Initially used for Pricing Level SKU. No longer maintained and updated.  </v>
       </c>
     </row>
-    <row r="45" spans="1:19" ht="15.75">
+    <row r="45" spans="1:19" ht="30">
       <c r="A45" s="7" t="s">
         <v>215</v>
       </c>
@@ -4908,6 +5096,9 @@
         <v>5.9519999999999998E-3</v>
       </c>
       <c r="G45" s="14"/>
+      <c r="H45" s="7" t="s">
+        <v>426</v>
+      </c>
       <c r="I45" s="7" t="e">
         <f>VLOOKUP(C45,OBJECT!A:C,3,FALSE)</f>
         <v>#N/A</v>
@@ -5022,7 +5213,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_PrimaryDiskTypeName: &lt;/b&gt;Friendly name of Primary Disk Type .  </v>
       </c>
     </row>
-    <row r="47" spans="1:19" ht="15.75">
+    <row r="47" spans="1:19" ht="60">
       <c r="A47" s="7" t="s">
         <v>217</v>
       </c>
@@ -5042,7 +5233,12 @@
         <f t="shared" si="0"/>
         <v>5.9519999999999998E-3</v>
       </c>
-      <c r="G47" s="14"/>
+      <c r="G47" s="14" t="s">
+        <v>425</v>
+      </c>
+      <c r="H47" s="7" t="s">
+        <v>424</v>
+      </c>
       <c r="I47" s="7" t="e">
         <f>VLOOKUP(C47,OBJECT!A:C,3,FALSE)</f>
         <v>#N/A</v>
@@ -5109,6 +5305,9 @@
         <v>0</v>
       </c>
       <c r="G48" s="14"/>
+      <c r="H48" s="7" t="s">
+        <v>423</v>
+      </c>
       <c r="I48" s="7" t="e">
         <f>VLOOKUP(C48,OBJECT!A:C,3,FALSE)</f>
         <v>#N/A</v>
@@ -5154,7 +5353,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_HasOpticalDiskDrive: &lt;/b&gt;True indicates that the machine has an optical disk drive (CD/DVD).  </v>
       </c>
     </row>
-    <row r="49" spans="1:19" ht="15.75">
+    <row r="49" spans="1:19" ht="45">
       <c r="A49" s="7" t="s">
         <v>251</v>
       </c>
@@ -5174,7 +5373,12 @@
         <f t="shared" si="0"/>
         <v>9.1120000000000003E-3</v>
       </c>
-      <c r="G49" s="14"/>
+      <c r="G49" s="14" t="s">
+        <v>421</v>
+      </c>
+      <c r="H49" s="7" t="s">
+        <v>422</v>
+      </c>
       <c r="I49" s="7" t="e">
         <f>VLOOKUP(C49,OBJECT!A:C,3,FALSE)</f>
         <v>#N/A</v>
@@ -5289,7 +5493,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_ChassisTypeName: &lt;/b&gt;Retrieves a numeric representation of what type of chassis the machine has. A value of 0 means xx.  </v>
       </c>
     </row>
-    <row r="51" spans="1:19" ht="31.5">
+    <row r="51" spans="1:19" ht="60">
       <c r="A51" s="7" t="s">
         <v>253</v>
       </c>
@@ -5309,7 +5513,12 @@
         <f t="shared" si="0"/>
         <v>5.3080000000000002E-3</v>
       </c>
-      <c r="G51" s="14"/>
+      <c r="G51" s="14" t="s">
+        <v>420</v>
+      </c>
+      <c r="H51" s="7" t="s">
+        <v>419</v>
+      </c>
       <c r="I51" s="7" t="e">
         <f>VLOOKUP(C51,OBJECT!A:C,3,FALSE)</f>
         <v>#N/A</v>
@@ -5355,7 +5564,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_InternalPrimaryDiagonalDisplaySizeInInches: &lt;/b&gt;Retrieves the physical diagonal length in inches of the primary display.  </v>
       </c>
     </row>
-    <row r="52" spans="1:19" ht="31.5">
+    <row r="52" spans="1:19" ht="60">
       <c r="A52" s="7" t="s">
         <v>254</v>
       </c>
@@ -5376,6 +5585,9 @@
         <v>5.3E-3</v>
       </c>
       <c r="G52" s="14"/>
+      <c r="H52" s="7" t="s">
+        <v>419</v>
+      </c>
       <c r="I52" s="7" t="e">
         <f>VLOOKUP(C52,OBJECT!A:C,3,FALSE)</f>
         <v>#N/A</v>
@@ -5421,7 +5633,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_InternalPrimaryDisplayResolutionHorizontal: &lt;/b&gt;Retrieves the number of pixels in the horizontal direction of the internal display..  </v>
       </c>
     </row>
-    <row r="53" spans="1:19" ht="31.5">
+    <row r="53" spans="1:19" ht="60">
       <c r="A53" s="7" t="s">
         <v>255</v>
       </c>
@@ -5442,6 +5654,9 @@
         <v>5.3E-3</v>
       </c>
       <c r="G53" s="14"/>
+      <c r="H53" s="7" t="s">
+        <v>419</v>
+      </c>
       <c r="I53" s="7" t="e">
         <f>VLOOKUP(C53,OBJECT!A:C,3,FALSE)</f>
         <v>#N/A</v>
@@ -5625,7 +5840,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_InternalBatteryType: &lt;/b&gt;NA.  </v>
       </c>
     </row>
-    <row r="56" spans="1:19" ht="15.75">
+    <row r="56" spans="1:19" ht="105">
       <c r="A56" s="7" t="s">
         <v>223</v>
       </c>
@@ -5646,6 +5861,9 @@
         <v>3.0075999999999999E-2</v>
       </c>
       <c r="G56" s="14"/>
+      <c r="H56" s="7" t="s">
+        <v>418</v>
+      </c>
       <c r="I56" s="7" t="e">
         <f>VLOOKUP(C56,OBJECT!A:C,3,FALSE)</f>
         <v>#N/A</v>
@@ -5920,7 +6138,7 @@
       </c>
       <c r="G60" s="14"/>
       <c r="H60" s="7" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="I60" s="7" t="e">
         <f>VLOOKUP(C60,OBJECT!A:C,3,FALSE)</f>
@@ -5967,7 +6185,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_OSBuildNumber: &lt;/b&gt;OS Build number extracted from the OsVersionFull. Example .  </v>
       </c>
     </row>
-    <row r="61" spans="1:19" ht="15.75">
+    <row r="61" spans="1:19" ht="45">
       <c r="A61" s="7" t="s">
         <v>260</v>
       </c>
@@ -5987,7 +6205,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G61" s="14"/>
+      <c r="G61" s="14" t="s">
+        <v>416</v>
+      </c>
+      <c r="H61" s="7" t="s">
+        <v>417</v>
+      </c>
       <c r="I61" s="7" t="e">
         <f>VLOOKUP(C61,OBJECT!A:C,3,FALSE)</f>
         <v>#N/A</v>
@@ -6264,7 +6487,7 @@
         <v>350</v>
       </c>
       <c r="H65" s="7" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="I65" s="7" t="e">
         <f>VLOOKUP(C65,OBJECT!A:C,3,FALSE)</f>
@@ -6311,7 +6534,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_OSInstallLanguageIdentifier: &lt;/b&gt;NA.  </v>
       </c>
     </row>
-    <row r="66" spans="1:19" ht="30">
+    <row r="66" spans="1:19" ht="60">
       <c r="A66" s="7" t="s">
         <v>223</v>
       </c>
@@ -6331,9 +6554,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G66" s="14"/>
+      <c r="G66" s="14" t="s">
+        <v>414</v>
+      </c>
       <c r="H66" s="7" t="s">
-        <v>377</v>
+        <v>415</v>
       </c>
       <c r="I66" s="7" t="e">
         <f>VLOOKUP(C66,OBJECT!A:C,3,FALSE)</f>
@@ -6470,6 +6695,9 @@
         <v>0</v>
       </c>
       <c r="G68" s="14"/>
+      <c r="H68" s="7" t="s">
+        <v>413</v>
+      </c>
       <c r="I68" s="7" t="e">
         <f>VLOOKUP(C68,OBJECT!A:C,3,FALSE)</f>
         <v>#N/A</v>
@@ -6584,7 +6812,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_GenuineStateName: &lt;/b&gt;Friendly name of OSGenuineStateID. 0 = Genuine.  </v>
       </c>
     </row>
-    <row r="70" spans="1:19" ht="30">
+    <row r="70" spans="1:19" ht="45">
       <c r="A70" s="7" t="s">
         <v>267</v>
       </c>
@@ -6724,7 +6952,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_IsFlightingInternal: &lt;/b&gt;Flighting' in Windows Defender context means making new development features available as soon as possible, during the development cycle. This does not refer to a public release. The 'internal' most likely means the Window Insider community.  </v>
       </c>
     </row>
-    <row r="72" spans="1:19" ht="30">
+    <row r="72" spans="1:19" ht="135">
       <c r="A72" s="7" t="s">
         <v>268</v>
       </c>
@@ -6744,7 +6972,12 @@
         <f t="shared" si="2"/>
         <v>1.7866E-2</v>
       </c>
-      <c r="G72" s="14"/>
+      <c r="G72" s="14" t="s">
+        <v>412</v>
+      </c>
+      <c r="H72" s="7" t="s">
+        <v>411</v>
+      </c>
       <c r="I72" s="7" t="e">
         <f>VLOOKUP(C72,OBJECT!A:C,3,FALSE)</f>
         <v>#N/A</v>
@@ -6859,7 +7092,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_FlightRing: &lt;/b&gt;The ring that the device user would like to receive flights for. This might be different from the ring of the OS which is currently installed if the user changes the ring after getting a flight from a different ring..  </v>
       </c>
     </row>
-    <row r="74" spans="1:19" ht="30">
+    <row r="74" spans="1:19" ht="45">
       <c r="A74" s="7" t="s">
         <v>223</v>
       </c>
@@ -6879,7 +7112,12 @@
         <f t="shared" si="2"/>
         <v>0.636208</v>
       </c>
-      <c r="G74" s="14"/>
+      <c r="G74" s="14" t="s">
+        <v>410</v>
+      </c>
+      <c r="H74" s="7" t="s">
+        <v>409</v>
+      </c>
       <c r="I74" s="7" t="e">
         <f>VLOOKUP(C74,OBJECT!A:C,3,FALSE)</f>
         <v>#N/A</v>
@@ -6925,7 +7163,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_ThresholdOptIn: &lt;/b&gt;NA.  </v>
       </c>
     </row>
-    <row r="75" spans="1:19" ht="15.75">
+    <row r="75" spans="1:19" ht="30">
       <c r="A75" s="7" t="s">
         <v>223</v>
       </c>
@@ -6945,7 +7183,12 @@
         <f t="shared" si="2"/>
         <v>2.0698000000000001E-2</v>
       </c>
-      <c r="G75" s="14"/>
+      <c r="G75" s="14" t="s">
+        <v>407</v>
+      </c>
+      <c r="H75" s="7" t="s">
+        <v>408</v>
+      </c>
       <c r="I75" s="7" t="e">
         <f>VLOOKUP(C75,OBJECT!A:C,3,FALSE)</f>
         <v>#N/A</v>
@@ -6991,7 +7234,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_FirmwareManufacturerIdentifier: &lt;/b&gt;NA.  </v>
       </c>
     </row>
-    <row r="76" spans="1:19" ht="15.75">
+    <row r="76" spans="1:19" ht="30">
       <c r="A76" s="7" t="s">
         <v>223</v>
       </c>
@@ -7011,7 +7254,12 @@
         <f t="shared" si="2"/>
         <v>1.8121999999999999E-2</v>
       </c>
-      <c r="G76" s="14"/>
+      <c r="G76" s="14" t="s">
+        <v>407</v>
+      </c>
+      <c r="H76" s="7" t="s">
+        <v>408</v>
+      </c>
       <c r="I76" s="7" t="e">
         <f>VLOOKUP(C76,OBJECT!A:C,3,FALSE)</f>
         <v>#N/A</v>
@@ -7078,6 +7326,9 @@
         <v>0</v>
       </c>
       <c r="G77" s="14"/>
+      <c r="H77" s="7" t="s">
+        <v>406</v>
+      </c>
       <c r="I77" s="7" t="e">
         <f>VLOOKUP(C77,OBJECT!A:C,3,FALSE)</f>
         <v>#N/A</v>
@@ -7123,7 +7374,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_IsSecureBootEnabled: &lt;/b&gt;Indicates if Secure Boot mode is enabled. Secure Boot is a security measure to protect against malware during early system startup..  </v>
       </c>
     </row>
-    <row r="78" spans="1:19" ht="30">
+    <row r="78" spans="1:19" ht="45">
       <c r="A78" s="7" t="s">
         <v>275</v>
       </c>
@@ -7194,7 +7445,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_IsWIMBootEnabled: &lt;/b&gt;wimboot is a boot loader for Windows Imaging Format .wim files. It enables you to boot into a Windows PE (WinPE) deployment or recovery environment..  </v>
       </c>
     </row>
-    <row r="79" spans="1:19" ht="30">
+    <row r="79" spans="1:19" ht="60">
       <c r="A79" s="7" t="s">
         <v>270</v>
       </c>
@@ -7214,7 +7465,12 @@
         <f t="shared" si="2"/>
         <v>1.802E-3</v>
       </c>
-      <c r="G79" s="14"/>
+      <c r="G79" s="14" t="s">
+        <v>404</v>
+      </c>
+      <c r="H79" s="7" t="s">
+        <v>405</v>
+      </c>
       <c r="I79" s="7" t="e">
         <f>VLOOKUP(C79,OBJECT!A:C,3,FALSE)</f>
         <v>#N/A</v>
@@ -7281,6 +7537,9 @@
         <v>0</v>
       </c>
       <c r="G80" s="14"/>
+      <c r="H80" s="7" t="s">
+        <v>403</v>
+      </c>
       <c r="I80" s="7" t="e">
         <f>VLOOKUP(C80,OBJECT!A:C,3,FALSE)</f>
         <v>#N/A</v>
@@ -7347,6 +7606,9 @@
         <v>0</v>
       </c>
       <c r="G81" s="14"/>
+      <c r="H81" s="7" t="s">
+        <v>402</v>
+      </c>
       <c r="I81" s="7" t="e">
         <f>VLOOKUP(C81,OBJECT!A:C,3,FALSE)</f>
         <v>#N/A</v>
@@ -7392,7 +7654,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_IsPenCapable: &lt;/b&gt;Is the device capable of pen input ?.  </v>
       </c>
     </row>
-    <row r="82" spans="1:19" ht="31.5">
+    <row r="82" spans="1:19" ht="45">
       <c r="A82" s="7" t="s">
         <v>273</v>
       </c>
@@ -7412,7 +7674,12 @@
         <f t="shared" si="2"/>
         <v>8.0800000000000004E-3</v>
       </c>
-      <c r="G82" s="14"/>
+      <c r="G82" s="14" t="s">
+        <v>399</v>
+      </c>
+      <c r="H82" s="7" t="s">
+        <v>401</v>
+      </c>
       <c r="I82" s="7" t="e">
         <f>VLOOKUP(C82,OBJECT!A:C,3,FALSE)</f>
         <v>#N/A</v>
@@ -7458,7 +7725,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_IsAlwaysOnAlwaysConnectedCapable: &lt;/b&gt;Retreives information about whether the battery enables the device to be AlwaysOnAlwaysConnected.  </v>
       </c>
     </row>
-    <row r="83" spans="1:19" ht="30">
+    <row r="83" spans="1:19" ht="45">
       <c r="A83" s="7" t="s">
         <v>274</v>
       </c>
@@ -7478,7 +7745,12 @@
         <f t="shared" si="2"/>
         <v>3.39E-2</v>
       </c>
-      <c r="G83" s="14"/>
+      <c r="G83" s="14" t="s">
+        <v>399</v>
+      </c>
+      <c r="H83" s="7" t="s">
+        <v>400</v>
+      </c>
       <c r="I83" s="7" t="e">
         <f>VLOOKUP(C83,OBJECT!A:C,3,FALSE)</f>
         <v>#N/A</v>
@@ -7524,7 +7796,7 @@
         <v xml:space="preserve">- &lt;b&gt;Wdft_IsGamer: &lt;/b&gt;Indicates whether the device is a gamer device or not based on its hardware combination..  </v>
       </c>
     </row>
-    <row r="84" spans="1:19" ht="15.75">
+    <row r="84" spans="1:19" ht="60">
       <c r="A84" s="7" t="s">
         <v>312</v>
       </c>
@@ -7544,7 +7816,12 @@
         <f t="shared" si="2"/>
         <v>3.39E-2</v>
       </c>
-      <c r="G84" s="14"/>
+      <c r="G84" s="14" t="s">
+        <v>397</v>
+      </c>
+      <c r="H84" s="7" t="s">
+        <v>398</v>
+      </c>
       <c r="I84" s="7" t="e">
         <f>VLOOKUP(C84,OBJECT!A:C,3,FALSE)</f>
         <v>#N/A</v>

</xml_diff>

<commit_message>
última revisión de categóricas
</commit_message>
<xml_diff>
--- a/mmp_info.xlsx
+++ b/mmp_info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\DataScience\Material didáctico\Ejercicios\Modelo_supervisado\Entregable_MMP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alinaoganesyan/Desktop/Master Data Science/Entregables/Trabajos/Repositorio entregable 2/Entregable_MMP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4840A020-0EB8-4E19-B5C3-304C846056F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9293642-DF77-B54D-A126-CD5D887A7777}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23880" yWindow="-7695" windowWidth="29040" windowHeight="15840" xr2:uid="{16D500F6-5AD7-764E-8C39-1ED26FBE09BA}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{16D500F6-5AD7-764E-8C39-1ED26FBE09BA}"/>
   </bookViews>
   <sheets>
     <sheet name="INFO" sheetId="1" r:id="rId1"/>
@@ -22,21 +22,10 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">INFO!$A$1:$T$85</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -1284,9 +1273,6 @@
     <t>Pasar NaN a un valor random. Debería ser bool. La mayoría de Census es 0, pero cuando es 1, se comporta de forma diferencial sobre la infección.</t>
   </si>
   <si>
-    <t>Distribución bastante equiparable.</t>
-  </si>
-  <si>
     <t>Debería ser bool. Suele ser census cero. Se comporta diferente sobre HasDetections dependiendo de si es Census 1 o 0</t>
   </si>
   <si>
@@ -1296,9 +1282,6 @@
     <t>Debería ser bool. Hay más cantidad de 1 en Has detection cuando el census es cero</t>
   </si>
   <si>
-    <t>es bool. Comportamiento similar para el target.</t>
-  </si>
-  <si>
     <t>FreqE</t>
   </si>
   <si>
@@ -1311,9 +1294,6 @@
     <t>Transformar NaN a un valor random, pe -1</t>
   </si>
   <si>
-    <t>Hay solo 7 valores 1(True), los demás son cero y NaN. Quizás conviene convertir los NaN a un valor random p.e. -1</t>
-  </si>
-  <si>
     <t>Transformar NaN a valor -1 o qualquier random, solo tiene 7 Trues… quizás eliminar ya que podría aprender?</t>
   </si>
   <si>
@@ -1332,9 +1312,6 @@
     <t>Es  OS Build revision extracted from the OsVersionFull. Example - OsBuildRevision = 1000 or 16458. Que quiere decir esto? Es redundante?</t>
   </si>
   <si>
-    <t>No creo que el numero de recargas de la batería aporte mucha información sobre el número de cargas de la batería aporte info sobre la infección de malware. Sin embargio puede contener información de la cantidad de uso del pc. Entiendo que es una variable que tiene sentido que sea numérica, indicando el número de veces, por lo que el modelo cortará por donde lo crea conveniente.</t>
-  </si>
-  <si>
     <t>Parece que se comporta de forma diferencial respecto al target. Osniste en el numero de pixels. Llega a tener muchos valores así que al ser numeral el modelo ya determinará donde hacer los cortes.</t>
   </si>
   <si>
@@ -1371,18 +1348,12 @@
     <t>OHE, Convertir NaN a no identificado</t>
   </si>
   <si>
-    <t>Numérica, convertir NaN a un valor random</t>
-  </si>
-  <si>
     <t>Convertir NaN a un valor random -1</t>
   </si>
   <si>
     <t>Es identificador, convertir a Categórica, FreqEncoding</t>
   </si>
   <si>
-    <t>Parece que hay un outlier 6357062.00. No entiendo muy bien que es este valor. Tiene NaN, quizá se podría hacer categoría otros para incluirlo.</t>
-  </si>
-  <si>
     <t>NaN=-1</t>
   </si>
   <si>
@@ -1392,16 +1363,37 @@
     <t>Es identificador, convertir a Categórica, FreqEncoding, NaN pasar a valor random</t>
   </si>
   <si>
-    <t>Poner valor random a NaN. La mayoría son ceros, solo hay 206 True de 469950 False</t>
-  </si>
-  <si>
-    <t>Poner valor random a NaN. La mayoría son ceros, solo hay 14 True de 499986False</t>
-  </si>
-  <si>
-    <t>Se comportan de forma diferencial. Hay NaN</t>
-  </si>
-  <si>
     <t>Es categórica, pasar valor a categórico con OHE</t>
+  </si>
+  <si>
+    <t>Poner valor random a NaN. La mayoría son ceros, solo hay 206 True de 469950 False
+Fijarnos si significan algo las diferencias en el target</t>
+  </si>
+  <si>
+    <t>La mayoría son ceros, solo hay 14 True de 499986False</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se comportan de forma diferencial. Hay NaN Poner valor random a NaN. </t>
+  </si>
+  <si>
+    <t>Parece que hay un outlier 6357062.00. No entiendo muy bien que es este valor. Tiene NaN, quizá se podría hacer categoría otros para incluirlo.
+Reviar las diferencias respeto al target</t>
+  </si>
+  <si>
+    <t>Numérica, convertir NaN a un valor random
+Revisar las diferencias respecto al target</t>
+  </si>
+  <si>
+    <t>No creo que el numero de recargas de la batería aporte mucha información sobre la infección de malware. Sin embargio puede contener información de la cantidad de uso del pc. Entiendo que es una variable que tiene sentido que sea numérica, indicando el número de veces, por lo que el modelo cortará por donde lo crea conveniente.</t>
+  </si>
+  <si>
+    <t>Hay solo 7 valores 1(True), los demás son cero y NaN. Quizás conviene convertir los NaN a un valor random p.e. -1. Revisar diferencias en el target</t>
+  </si>
+  <si>
+    <t>es bool. Comportamiento similar para el target. Variable muy equitativamente distribuida</t>
+  </si>
+  <si>
+    <t>Debería ser bool. Predomina el 0. Distribución bastante equiparable del target</t>
   </si>
 </sst>
 </file>
@@ -1553,7 +1545,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1981,29 +1973,29 @@
   <dimension ref="A1:S85"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G26" sqref="G26"/>
+      <pane ySplit="1" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H82" sqref="H82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="85.125" style="7" customWidth="1"/>
-    <col min="2" max="2" width="18.375" style="7" customWidth="1"/>
+    <col min="1" max="1" width="85.1640625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" style="7" customWidth="1"/>
     <col min="3" max="3" width="46" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="13.125" style="7" customWidth="1"/>
-    <col min="7" max="7" width="14.125" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="61.375" style="7" customWidth="1"/>
+    <col min="4" max="6" width="13.1640625" style="7" customWidth="1"/>
+    <col min="7" max="7" width="14.1640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="61.33203125" style="7" customWidth="1"/>
     <col min="9" max="9" width="20" style="7" customWidth="1"/>
-    <col min="10" max="10" width="10.875" style="7"/>
-    <col min="11" max="11" width="16.875" style="15" customWidth="1"/>
-    <col min="12" max="12" width="19.375" style="16" customWidth="1"/>
-    <col min="13" max="13" width="22.875" style="7" customWidth="1"/>
-    <col min="14" max="18" width="10.875" style="7"/>
-    <col min="19" max="19" width="87.875" style="7" customWidth="1"/>
-    <col min="20" max="16384" width="10.875" style="7"/>
+    <col min="10" max="10" width="10.83203125" style="7"/>
+    <col min="11" max="11" width="16.83203125" style="15" customWidth="1"/>
+    <col min="12" max="12" width="19.33203125" style="16" customWidth="1"/>
+    <col min="13" max="13" width="22.83203125" style="7" customWidth="1"/>
+    <col min="14" max="18" width="10.83203125" style="7"/>
+    <col min="19" max="19" width="87.83203125" style="7" customWidth="1"/>
+    <col min="20" max="16384" width="10.83203125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="13" customFormat="1" ht="15.75">
+    <row r="1" spans="1:19" s="13" customFormat="1" ht="17">
       <c r="A1" s="6" t="s">
         <v>211</v>
       </c>
@@ -2059,7 +2051,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="30">
+    <row r="2" spans="1:19" ht="51">
       <c r="A2" s="7" t="s">
         <v>212</v>
       </c>
@@ -2130,7 +2122,7 @@
         <v xml:space="preserve">- &lt;b&gt;Unnamed: 0: &lt;/b&gt;index.  </v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="60">
+    <row r="3" spans="1:19" ht="68">
       <c r="A3" s="7" t="s">
         <v>218</v>
       </c>
@@ -2199,7 +2191,7 @@
         <v xml:space="preserve">- &lt;b&gt;MachineIdentifier: &lt;/b&gt;Individual machine ID.  </v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="90">
+    <row r="4" spans="1:19" ht="119">
       <c r="B4" s="7" t="s">
         <v>95</v>
       </c>
@@ -2265,7 +2257,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="60">
+    <row r="5" spans="1:19" ht="68">
       <c r="A5" s="7" t="s">
         <v>219</v>
       </c>
@@ -2334,7 +2326,7 @@
         <v xml:space="preserve">- &lt;b&gt;EngineVersion: &lt;/b&gt;Defender state information e.g. 1.1.12603.0.  </v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="30">
+    <row r="6" spans="1:19" ht="51">
       <c r="A6" s="7" t="s">
         <v>220</v>
       </c>
@@ -2403,7 +2395,7 @@
         <v xml:space="preserve">- &lt;b&gt;AppVersion: &lt;/b&gt;Defender state information e.g. 4.9.10586.0.  </v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="30">
+    <row r="7" spans="1:19" ht="34">
       <c r="A7" s="7" t="s">
         <v>221</v>
       </c>
@@ -2472,7 +2464,7 @@
         <v xml:space="preserve">- &lt;b&gt;AvSigVersion: &lt;/b&gt;Defender state information e.g. 1.217.1014.0.  </v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="60">
+    <row r="8" spans="1:19" ht="68">
       <c r="A8" s="7" t="s">
         <v>222</v>
       </c>
@@ -2543,7 +2535,7 @@
         <v xml:space="preserve">- &lt;b&gt;IsBeta: &lt;/b&gt;Defender state information e.g. false.  </v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="105">
+    <row r="9" spans="1:19" ht="119">
       <c r="A9" s="7" t="s">
         <v>306</v>
       </c>
@@ -2614,7 +2606,7 @@
         <v xml:space="preserve">- &lt;b&gt;RtpStateBitfield: &lt;/b&gt;RTP state: Realtime protection state (Enabled or Disabled).  </v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="150">
+    <row r="10" spans="1:19" ht="170">
       <c r="A10" s="7" t="s">
         <v>307</v>
       </c>
@@ -2685,7 +2677,7 @@
         <v xml:space="preserve">- &lt;b&gt;IsSxsPassiveMode: &lt;/b&gt;active/passive mode of operation for Windows Defender. If another third party primary antivirus exists on the system, the Defender enters Passive mode. Passive mode obviously offers reduced functionality.  </v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="15.75">
+    <row r="11" spans="1:19" ht="17">
       <c r="A11" s="7" t="s">
         <v>224</v>
       </c>
@@ -2756,7 +2748,7 @@
         <v xml:space="preserve">- &lt;b&gt;DefaultBrowsersIdentifier: &lt;/b&gt;ID for the machine's default browser.  </v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="75">
+    <row r="12" spans="1:19" ht="102">
       <c r="A12" s="7" t="s">
         <v>225</v>
       </c>
@@ -2827,7 +2819,7 @@
         <v xml:space="preserve">- &lt;b&gt;AVProductStatesIdentifier: &lt;/b&gt;ID for the specific configuration of a user's antivirus software.  </v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="60">
+    <row r="13" spans="1:19" ht="68">
       <c r="A13" s="7" t="s">
         <v>309</v>
       </c>
@@ -2898,7 +2890,7 @@
         <v xml:space="preserve">- &lt;b&gt;AVProductsInstalled: &lt;/b&gt;Active anti-virus of the total installed.  </v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="60">
+    <row r="14" spans="1:19" ht="68">
       <c r="A14" s="7" t="s">
         <v>308</v>
       </c>
@@ -2969,7 +2961,7 @@
         <v xml:space="preserve">- &lt;b&gt;AVProductsEnabled: &lt;/b&gt;Of the installed antiviruses, those that are active.  </v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="30">
+    <row r="15" spans="1:19" ht="34">
       <c r="A15" s="7" t="s">
         <v>226</v>
       </c>
@@ -3038,7 +3030,7 @@
         <v xml:space="preserve">- &lt;b&gt;HasTpm: &lt;/b&gt;True if machine has tpm.  </v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="75">
+    <row r="16" spans="1:19" ht="85">
       <c r="A16" s="7" t="s">
         <v>227</v>
       </c>
@@ -3109,7 +3101,7 @@
         <v xml:space="preserve">- &lt;b&gt;CountryIdentifier: &lt;/b&gt;ID for the country the machine is located in.  </v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="75">
+    <row r="17" spans="1:19" ht="85">
       <c r="A17" s="7" t="s">
         <v>228</v>
       </c>
@@ -3180,7 +3172,7 @@
         <v xml:space="preserve">- &lt;b&gt;CityIdentifier: &lt;/b&gt;ID for the city the machine is located in.  </v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="60">
+    <row r="18" spans="1:19" ht="68">
       <c r="A18" s="7" t="s">
         <v>229</v>
       </c>
@@ -3251,7 +3243,7 @@
         <v xml:space="preserve">- &lt;b&gt;OrganizationIdentifier: &lt;/b&gt;ID for the organization the machine belongs in, organization ID is mapped to both specific companies and broad industries.  </v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="45">
+    <row r="19" spans="1:19" ht="51">
       <c r="A19" s="7" t="s">
         <v>230</v>
       </c>
@@ -3322,7 +3314,7 @@
         <v xml:space="preserve">- &lt;b&gt;GeoNameIdentifier: &lt;/b&gt;ID for the geographic region a machine is located in.  </v>
       </c>
     </row>
-    <row r="20" spans="1:19" ht="45">
+    <row r="20" spans="1:19" ht="51">
       <c r="A20" s="7" t="s">
         <v>231</v>
       </c>
@@ -3393,7 +3385,7 @@
         <v xml:space="preserve">- &lt;b&gt;LocaleEnglishNameIdentifier: &lt;/b&gt;English name of Locale ID of the current user.  </v>
       </c>
     </row>
-    <row r="21" spans="1:19" ht="45">
+    <row r="21" spans="1:19" ht="68">
       <c r="A21" s="7" t="s">
         <v>232</v>
       </c>
@@ -3462,7 +3454,7 @@
         <v xml:space="preserve">- &lt;b&gt;Platform: &lt;/b&gt;Calculates platform name (of OS related properties and processor property).  </v>
       </c>
     </row>
-    <row r="22" spans="1:19" ht="90">
+    <row r="22" spans="1:19" ht="102">
       <c r="A22" s="7" t="s">
         <v>233</v>
       </c>
@@ -3531,7 +3523,7 @@
         <v xml:space="preserve">- &lt;b&gt;Processor: &lt;/b&gt;This is the process architecture of the installed operating system.  </v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="45">
+    <row r="23" spans="1:19" ht="51">
       <c r="A23" s="7" t="s">
         <v>234</v>
       </c>
@@ -3600,7 +3592,7 @@
         <v xml:space="preserve">- &lt;b&gt;OsVer: &lt;/b&gt;Version of the current operating system.  </v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="60">
+    <row r="24" spans="1:19" ht="68">
       <c r="A24" s="7" t="s">
         <v>235</v>
       </c>
@@ -3669,7 +3661,7 @@
         <v xml:space="preserve">- &lt;b&gt;OsBuild: &lt;/b&gt;Build of the current operating system.  </v>
       </c>
     </row>
-    <row r="25" spans="1:19" ht="15.75">
+    <row r="25" spans="1:19" ht="17">
       <c r="A25" s="7" t="s">
         <v>236</v>
       </c>
@@ -3690,10 +3682,10 @@
         <v>0</v>
       </c>
       <c r="G25" s="14" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>441</v>
+        <v>432</v>
       </c>
       <c r="I25" s="7" t="e">
         <f>VLOOKUP(C25,OBJECT!A:C,3,FALSE)</f>
@@ -3740,7 +3732,7 @@
         <v xml:space="preserve">- &lt;b&gt;OsSuite: &lt;/b&gt;Product suite mask for the current operating system..  </v>
       </c>
     </row>
-    <row r="26" spans="1:19" ht="60">
+    <row r="26" spans="1:19" ht="85">
       <c r="A26" s="7" t="s">
         <v>237</v>
       </c>
@@ -3809,7 +3801,7 @@
         <v xml:space="preserve">- &lt;b&gt;OsPlatformSubRelease: &lt;/b&gt;Returns the OS Platform sub.  </v>
       </c>
     </row>
-    <row r="27" spans="1:19" ht="75">
+    <row r="27" spans="1:19" ht="85">
       <c r="A27" s="7" t="s">
         <v>238</v>
       </c>
@@ -3878,7 +3870,7 @@
         <v xml:space="preserve">- &lt;b&gt;OsBuildLab: &lt;/b&gt;Build lab that generated the current OS. Example: 9600.17630.amd64fre.winblue_r7.150109.  </v>
       </c>
     </row>
-    <row r="28" spans="1:19" ht="82.5">
+    <row r="28" spans="1:19" ht="90">
       <c r="A28" s="7" t="s">
         <v>277</v>
       </c>
@@ -3947,7 +3939,7 @@
         <v xml:space="preserve">- &lt;b&gt;SkuEdition: &lt;/b&gt;The goal of this feature is to use the Product Type defined in the MSDN (Microsoft Developer Network) to map to a SKU (Stock Keeping Unit).  </v>
       </c>
     </row>
-    <row r="29" spans="1:19" ht="30">
+    <row r="29" spans="1:19" ht="34">
       <c r="A29" s="7" t="s">
         <v>239</v>
       </c>
@@ -3968,10 +3960,10 @@
         <v>3.852E-3</v>
       </c>
       <c r="G29" s="14" t="s">
+        <v>429</v>
+      </c>
+      <c r="H29" s="7" t="s">
         <v>435</v>
-      </c>
-      <c r="H29" s="7" t="s">
-        <v>440</v>
       </c>
       <c r="I29" s="7" t="e">
         <f>VLOOKUP(C29,OBJECT!A:C,3,FALSE)</f>
@@ -4018,7 +4010,7 @@
         <v xml:space="preserve">- &lt;b&gt;IsProtected: &lt;/b&gt;This is a calculated field derived from the Spynet Report's AV Products field. Returns: a. TRUE if there is at least one active and up.  </v>
       </c>
     </row>
-    <row r="30" spans="1:19" ht="30">
+    <row r="30" spans="1:19" ht="34">
       <c r="A30" s="7" t="s">
         <v>240</v>
       </c>
@@ -4040,7 +4032,7 @@
       </c>
       <c r="G30" s="14"/>
       <c r="H30" s="7" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="I30" s="7" t="e">
         <f>VLOOKUP(C30,OBJECT!A:C,3,FALSE)</f>
@@ -4087,7 +4079,7 @@
         <v xml:space="preserve">- &lt;b&gt;AutoSampleOptIn: &lt;/b&gt;This is the SubmitSamplesConsent value passed in from the service, available on CAMP 9+.  </v>
       </c>
     </row>
-    <row r="31" spans="1:19" ht="15.75">
+    <row r="31" spans="1:19" ht="17">
       <c r="A31" s="7" t="s">
         <v>241</v>
       </c>
@@ -4158,7 +4150,7 @@
         <v xml:space="preserve">- &lt;b&gt;PuaMode: &lt;/b&gt;Pua Enabled mode from the service.  </v>
       </c>
     </row>
-    <row r="32" spans="1:19" ht="30">
+    <row r="32" spans="1:19" ht="51">
       <c r="A32" s="7" t="s">
         <v>242</v>
       </c>
@@ -4179,10 +4171,10 @@
         <v>5.9695999999999999E-2</v>
       </c>
       <c r="G32" s="14" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
       <c r="H32" s="7" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="I32" s="7" t="e">
         <f>VLOOKUP(C32,OBJECT!A:C,3,FALSE)</f>
@@ -4229,7 +4221,7 @@
         <v xml:space="preserve">- &lt;b&gt;SMode: &lt;/b&gt;This field is set to true when the device is known to be in 'S Mode', as in, Windows 10 S mode, where only Microsoft Store apps can be installed.  </v>
       </c>
     </row>
-    <row r="33" spans="1:19" ht="30">
+    <row r="33" spans="1:19" ht="34">
       <c r="A33" s="7" t="s">
         <v>310</v>
       </c>
@@ -4250,10 +4242,10 @@
         <v>6.4180000000000001E-3</v>
       </c>
       <c r="G33" s="14" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="H33" s="7" t="s">
-        <v>437</v>
+        <v>431</v>
       </c>
       <c r="I33" s="7" t="e">
         <f>VLOOKUP(C33,OBJECT!A:C,3,FALSE)</f>
@@ -4300,7 +4292,7 @@
         <v xml:space="preserve">- &lt;b&gt;IeVerIdentifier: &lt;/b&gt;Retrieves which version of Internet Explorer is running on this device.  </v>
       </c>
     </row>
-    <row r="34" spans="1:19" ht="121.5">
+    <row r="34" spans="1:19" ht="136">
       <c r="A34" s="7" t="s">
         <v>243</v>
       </c>
@@ -4371,7 +4363,7 @@
         <v xml:space="preserve">- &lt;b&gt;SmartScreen: &lt;/b&gt;This is the SmartScreen enabled string value from registry. This is obtained by checking in order, HKLM\SOFTWARE\Policies\Microsoft\Windows\System\SmartScreenEnabled and HKLM\SOFTWARE\Microsoft\Windows\CurrentVersion\Explorer\SmartScreenEnabled. If the value exists but is blank, the value "ExistsNotSet" is sent in telemetry..  </v>
       </c>
     </row>
-    <row r="35" spans="1:19" ht="30">
+    <row r="35" spans="1:19" ht="34">
       <c r="A35" s="7" t="s">
         <v>244</v>
       </c>
@@ -4392,10 +4384,10 @@
         <v>1.0324E-2</v>
       </c>
       <c r="G35" s="14" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
       <c r="H35" s="7" t="s">
-        <v>436</v>
+        <v>430</v>
       </c>
       <c r="I35" s="7" t="e">
         <f>VLOOKUP(C35,OBJECT!A:C,3,FALSE)</f>
@@ -4442,7 +4434,7 @@
         <v xml:space="preserve">- &lt;b&gt;Firewall: &lt;/b&gt;This attribute is true (1) for Windows 8.1 and above if windows firewall is enabled, as reported by the service..  </v>
       </c>
     </row>
-    <row r="36" spans="1:19" ht="45">
+    <row r="36" spans="1:19" ht="68">
       <c r="A36" s="7" t="s">
         <v>245</v>
       </c>
@@ -4464,7 +4456,7 @@
       </c>
       <c r="G36" s="14"/>
       <c r="H36" s="7" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="I36" s="7" t="e">
         <f>VLOOKUP(C36,OBJECT!A:C,3,FALSE)</f>
@@ -4511,7 +4503,7 @@
         <v xml:space="preserve">- &lt;b&gt;UacLuaenable: &lt;/b&gt;This attribute reports whether or not the "administrator in Admin Approval Mode" user type is disabled or enabled in UAC. The value reported is obtained by reading the regkey HKLM\SOFTWARE\Microsoft\Windows\CurrentVersion\Policies\System\EnableLUA..  </v>
       </c>
     </row>
-    <row r="37" spans="1:19" ht="75">
+    <row r="37" spans="1:19" ht="85">
       <c r="A37" s="7" t="s">
         <v>246</v>
       </c>
@@ -4580,7 +4572,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_MDC2FormFactor: &lt;/b&gt;A grouping based on a combination of Device Census level hardware characteristics. The logic used to define Form Factor is rooted in business and industry standards and aligns with how people think about their device. (Examples: Smartphone, Small Tablet, All in One, Convertible...).  </v>
       </c>
     </row>
-    <row r="38" spans="1:19" ht="60">
+    <row r="38" spans="1:19" ht="68">
       <c r="A38" s="7" t="s">
         <v>247</v>
       </c>
@@ -4649,7 +4641,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_DeviceFamily: &lt;/b&gt;AKA DeviceClass. Indicates the type of device that an edition of the OS is intended for. Example values: Windows.Desktop, Windows.Mobile, and iOS.Phone.  </v>
       </c>
     </row>
-    <row r="39" spans="1:19" ht="15.75">
+    <row r="39" spans="1:19" ht="34">
       <c r="A39" s="7" t="s">
         <v>223</v>
       </c>
@@ -4670,10 +4662,10 @@
         <v>1.0762000000000001E-2</v>
       </c>
       <c r="G39" s="14" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="H39" s="7" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="I39" s="7" t="e">
         <f>VLOOKUP(C39,OBJECT!A:C,3,FALSE)</f>
@@ -4720,7 +4712,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_OEMNameIdentifier: &lt;/b&gt;NA.  </v>
       </c>
     </row>
-    <row r="40" spans="1:19" ht="15.75">
+    <row r="40" spans="1:19" ht="34">
       <c r="A40" s="7" t="s">
         <v>223</v>
       </c>
@@ -4741,10 +4733,10 @@
         <v>1.1528E-2</v>
       </c>
       <c r="G40" s="14" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="H40" s="7" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="I40" s="7" t="e">
         <f>VLOOKUP(C40,OBJECT!A:C,3,FALSE)</f>
@@ -4791,7 +4783,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_OEMModelIdentifier: &lt;/b&gt;NA.  </v>
       </c>
     </row>
-    <row r="41" spans="1:19" ht="45">
+    <row r="41" spans="1:19" ht="68">
       <c r="A41" s="7" t="s">
         <v>248</v>
       </c>
@@ -4812,10 +4804,10 @@
         <v>4.6940000000000003E-3</v>
       </c>
       <c r="G41" s="14" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="H41" s="7" t="s">
-        <v>431</v>
+        <v>437</v>
       </c>
       <c r="I41" s="7" t="e">
         <f>VLOOKUP(C41,OBJECT!A:C,3,FALSE)</f>
@@ -4862,7 +4854,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_ProcessorCoreCount: &lt;/b&gt;Number of logical cores in the processor.  </v>
       </c>
     </row>
-    <row r="42" spans="1:19" ht="60">
+    <row r="42" spans="1:19" ht="68">
       <c r="A42" s="7" t="s">
         <v>223</v>
       </c>
@@ -4883,10 +4875,10 @@
         <v>4.6940000000000003E-3</v>
       </c>
       <c r="G42" s="14" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="H42" s="7" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="I42" s="7" t="e">
         <f>VLOOKUP(C42,OBJECT!A:C,3,FALSE)</f>
@@ -4933,7 +4925,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_ProcessorManufacturerIdentifier: &lt;/b&gt;NA.  </v>
       </c>
     </row>
-    <row r="43" spans="1:19" ht="15.75">
+    <row r="43" spans="1:19" ht="17">
       <c r="A43" s="7" t="s">
         <v>223</v>
       </c>
@@ -4954,10 +4946,10 @@
         <v>4.6979999999999999E-3</v>
       </c>
       <c r="G43" s="14" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="H43" s="7" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="I43" s="7" t="e">
         <f>VLOOKUP(C43,OBJECT!A:C,3,FALSE)</f>
@@ -5004,7 +4996,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_ProcessorModelIdentifier: &lt;/b&gt;NA.  </v>
       </c>
     </row>
-    <row r="44" spans="1:19" ht="30">
+    <row r="44" spans="1:19" ht="34">
       <c r="A44" s="7" t="s">
         <v>249</v>
       </c>
@@ -5075,7 +5067,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_ProcessorClass: &lt;/b&gt;A classification of processors into high/medium/low. Initially used for Pricing Level SKU. No longer maintained and updated.  </v>
       </c>
     </row>
-    <row r="45" spans="1:19" ht="30">
+    <row r="45" spans="1:19" ht="34">
       <c r="A45" s="7" t="s">
         <v>215</v>
       </c>
@@ -5097,7 +5089,7 @@
       </c>
       <c r="G45" s="14"/>
       <c r="H45" s="7" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="I45" s="7" t="e">
         <f>VLOOKUP(C45,OBJECT!A:C,3,FALSE)</f>
@@ -5144,7 +5136,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_PrimaryDiskTotalCapacity: &lt;/b&gt;Amount of disk space on primary disk of the machine in MB.  </v>
       </c>
     </row>
-    <row r="46" spans="1:19" ht="45">
+    <row r="46" spans="1:19" ht="51">
       <c r="A46" s="7" t="s">
         <v>216</v>
       </c>
@@ -5213,7 +5205,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_PrimaryDiskTypeName: &lt;/b&gt;Friendly name of Primary Disk Type .  </v>
       </c>
     </row>
-    <row r="47" spans="1:19" ht="60">
+    <row r="47" spans="1:19" ht="68">
       <c r="A47" s="7" t="s">
         <v>217</v>
       </c>
@@ -5234,10 +5226,10 @@
         <v>5.9519999999999998E-3</v>
       </c>
       <c r="G47" s="14" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="H47" s="7" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="I47" s="7" t="e">
         <f>VLOOKUP(C47,OBJECT!A:C,3,FALSE)</f>
@@ -5284,7 +5276,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_SystemVolumeTotalCapacity: &lt;/b&gt;The size of the partition that the System volume is installed on in MB.  </v>
       </c>
     </row>
-    <row r="48" spans="1:19" ht="30">
+    <row r="48" spans="1:19" ht="34">
       <c r="A48" s="7" t="s">
         <v>250</v>
       </c>
@@ -5306,7 +5298,7 @@
       </c>
       <c r="G48" s="14"/>
       <c r="H48" s="7" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="I48" s="7" t="e">
         <f>VLOOKUP(C48,OBJECT!A:C,3,FALSE)</f>
@@ -5353,7 +5345,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_HasOpticalDiskDrive: &lt;/b&gt;True indicates that the machine has an optical disk drive (CD/DVD).  </v>
       </c>
     </row>
-    <row r="49" spans="1:19" ht="45">
+    <row r="49" spans="1:19" ht="51">
       <c r="A49" s="7" t="s">
         <v>251</v>
       </c>
@@ -5374,10 +5366,10 @@
         <v>9.1120000000000003E-3</v>
       </c>
       <c r="G49" s="14" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="H49" s="7" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="I49" s="7" t="e">
         <f>VLOOKUP(C49,OBJECT!A:C,3,FALSE)</f>
@@ -5424,7 +5416,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_TotalPhysicalRAM: &lt;/b&gt;Retrieves the physical RAM in MB.  </v>
       </c>
     </row>
-    <row r="50" spans="1:19" ht="45">
+    <row r="50" spans="1:19" ht="51">
       <c r="A50" s="7" t="s">
         <v>252</v>
       </c>
@@ -5493,7 +5485,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_ChassisTypeName: &lt;/b&gt;Retrieves a numeric representation of what type of chassis the machine has. A value of 0 means xx.  </v>
       </c>
     </row>
-    <row r="51" spans="1:19" ht="60">
+    <row r="51" spans="1:19" ht="68">
       <c r="A51" s="7" t="s">
         <v>253</v>
       </c>
@@ -5514,10 +5506,10 @@
         <v>5.3080000000000002E-3</v>
       </c>
       <c r="G51" s="14" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="H51" s="7" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="I51" s="7" t="e">
         <f>VLOOKUP(C51,OBJECT!A:C,3,FALSE)</f>
@@ -5564,7 +5556,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_InternalPrimaryDiagonalDisplaySizeInInches: &lt;/b&gt;Retrieves the physical diagonal length in inches of the primary display.  </v>
       </c>
     </row>
-    <row r="52" spans="1:19" ht="60">
+    <row r="52" spans="1:19" ht="68">
       <c r="A52" s="7" t="s">
         <v>254</v>
       </c>
@@ -5586,7 +5578,7 @@
       </c>
       <c r="G52" s="14"/>
       <c r="H52" s="7" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="I52" s="7" t="e">
         <f>VLOOKUP(C52,OBJECT!A:C,3,FALSE)</f>
@@ -5633,7 +5625,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_InternalPrimaryDisplayResolutionHorizontal: &lt;/b&gt;Retrieves the number of pixels in the horizontal direction of the internal display..  </v>
       </c>
     </row>
-    <row r="53" spans="1:19" ht="60">
+    <row r="53" spans="1:19" ht="68">
       <c r="A53" s="7" t="s">
         <v>255</v>
       </c>
@@ -5655,7 +5647,7 @@
       </c>
       <c r="G53" s="14"/>
       <c r="H53" s="7" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="I53" s="7" t="e">
         <f>VLOOKUP(C53,OBJECT!A:C,3,FALSE)</f>
@@ -5702,7 +5694,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_InternalPrimaryDisplayResolutionVertical: &lt;/b&gt;Retrieves the number of pixels in the vertical direction of the internal display.  </v>
       </c>
     </row>
-    <row r="54" spans="1:19" ht="45">
+    <row r="54" spans="1:19" ht="51">
       <c r="A54" s="7" t="s">
         <v>214</v>
       </c>
@@ -5771,7 +5763,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_PowerPlatformRoleName: &lt;/b&gt;Indicates the OEM preferred power management profile. This value helps identify the basic form factor of the device.  </v>
       </c>
     </row>
-    <row r="55" spans="1:19" ht="60">
+    <row r="55" spans="1:19" ht="68">
       <c r="A55" s="7" t="s">
         <v>223</v>
       </c>
@@ -5840,7 +5832,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_InternalBatteryType: &lt;/b&gt;NA.  </v>
       </c>
     </row>
-    <row r="56" spans="1:19" ht="105">
+    <row r="56" spans="1:19" ht="102">
       <c r="A56" s="7" t="s">
         <v>223</v>
       </c>
@@ -5862,7 +5854,7 @@
       </c>
       <c r="G56" s="14"/>
       <c r="H56" s="7" t="s">
-        <v>418</v>
+        <v>438</v>
       </c>
       <c r="I56" s="7" t="e">
         <f>VLOOKUP(C56,OBJECT!A:C,3,FALSE)</f>
@@ -5909,7 +5901,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_InternalBatteryNumberOfCharges: &lt;/b&gt;NA.  </v>
       </c>
     </row>
-    <row r="57" spans="1:19" ht="30">
+    <row r="57" spans="1:19" ht="34">
       <c r="A57" s="7" t="s">
         <v>256</v>
       </c>
@@ -5978,7 +5970,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_OSVersion: &lt;/b&gt;Numeric OS version Example .  </v>
       </c>
     </row>
-    <row r="58" spans="1:19" ht="75">
+    <row r="58" spans="1:19" ht="85">
       <c r="A58" s="7" t="s">
         <v>257</v>
       </c>
@@ -6047,7 +6039,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_OSArchitecture: &lt;/b&gt;Architecture on which the OS is based. Derived from OSVersionFull. Example .  </v>
       </c>
     </row>
-    <row r="59" spans="1:19" ht="75">
+    <row r="59" spans="1:19" ht="85">
       <c r="A59" s="7" t="s">
         <v>258</v>
       </c>
@@ -6116,7 +6108,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_OSBranch: &lt;/b&gt;Branch of the OS extracted from the OsVersionFull. Example .  </v>
       </c>
     </row>
-    <row r="60" spans="1:19" ht="30">
+    <row r="60" spans="1:19" ht="51">
       <c r="A60" s="7" t="s">
         <v>259</v>
       </c>
@@ -6185,7 +6177,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_OSBuildNumber: &lt;/b&gt;OS Build number extracted from the OsVersionFull. Example .  </v>
       </c>
     </row>
-    <row r="61" spans="1:19" ht="45">
+    <row r="61" spans="1:19" ht="51">
       <c r="A61" s="7" t="s">
         <v>260</v>
       </c>
@@ -6206,10 +6198,10 @@
         <v>0</v>
       </c>
       <c r="G61" s="14" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="H61" s="7" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="I61" s="7" t="e">
         <f>VLOOKUP(C61,OBJECT!A:C,3,FALSE)</f>
@@ -6256,7 +6248,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_OSBuildRevision: &lt;/b&gt;OS Build revision extracted from the OsVersionFull. Example .  </v>
       </c>
     </row>
-    <row r="62" spans="1:19" ht="60">
+    <row r="62" spans="1:19" ht="68">
       <c r="A62" s="7" t="s">
         <v>261</v>
       </c>
@@ -6325,7 +6317,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_OSEdition: &lt;/b&gt;Edition of the current OS. Sourced from HKLM\Software\Microsoft\Windows NT\CurrentVersion@EditionID in registry. Example: Enterprise.  </v>
       </c>
     </row>
-    <row r="63" spans="1:19" ht="45">
+    <row r="63" spans="1:19" ht="51">
       <c r="A63" s="7" t="s">
         <v>262</v>
       </c>
@@ -6394,7 +6386,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_OSSkuName: &lt;/b&gt;OS edition friendly name (currently Windows only).  </v>
       </c>
     </row>
-    <row r="64" spans="1:19" ht="45">
+    <row r="64" spans="1:19" ht="51">
       <c r="A64" s="7" t="s">
         <v>263</v>
       </c>
@@ -6463,7 +6455,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_OSInstallTypeName: &lt;/b&gt;Friendly description of what install was used on the machine i.e. clean.  </v>
       </c>
     </row>
-    <row r="65" spans="1:19" ht="30">
+    <row r="65" spans="1:19" ht="34">
       <c r="A65" s="7" t="s">
         <v>223</v>
       </c>
@@ -6534,7 +6526,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_OSInstallLanguageIdentifier: &lt;/b&gt;NA.  </v>
       </c>
     </row>
-    <row r="66" spans="1:19" ht="60">
+    <row r="66" spans="1:19" ht="68">
       <c r="A66" s="7" t="s">
         <v>223</v>
       </c>
@@ -6555,10 +6547,10 @@
         <v>0</v>
       </c>
       <c r="G66" s="14" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="H66" s="7" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="I66" s="7" t="e">
         <f>VLOOKUP(C66,OBJECT!A:C,3,FALSE)</f>
@@ -6605,7 +6597,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_OSUILocaleIdentifier: &lt;/b&gt;NA.  </v>
       </c>
     </row>
-    <row r="67" spans="1:19" ht="60">
+    <row r="67" spans="1:19" ht="68">
       <c r="A67" s="7" t="s">
         <v>264</v>
       </c>
@@ -6674,7 +6666,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_OSWUAutoUpdateOptionsName: &lt;/b&gt;Friendly name of the WindowsUpdate auto.  </v>
       </c>
     </row>
-    <row r="68" spans="1:19" ht="30">
+    <row r="68" spans="1:19" ht="34">
       <c r="A68" s="7" t="s">
         <v>265</v>
       </c>
@@ -6696,7 +6688,7 @@
       </c>
       <c r="G68" s="14"/>
       <c r="H68" s="7" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="I68" s="7" t="e">
         <f>VLOOKUP(C68,OBJECT!A:C,3,FALSE)</f>
@@ -6743,7 +6735,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_IsPortableOperatingSystem: &lt;/b&gt;Indicates whether OS is booted up and running via Windows.  </v>
       </c>
     </row>
-    <row r="69" spans="1:19" ht="30">
+    <row r="69" spans="1:19" ht="34">
       <c r="A69" s="7" t="s">
         <v>266</v>
       </c>
@@ -6812,7 +6804,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_GenuineStateName: &lt;/b&gt;Friendly name of OSGenuineStateID. 0 = Genuine.  </v>
       </c>
     </row>
-    <row r="70" spans="1:19" ht="45">
+    <row r="70" spans="1:19" ht="51">
       <c r="A70" s="7" t="s">
         <v>267</v>
       </c>
@@ -6881,7 +6873,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_ActivationChannel: &lt;/b&gt;Retail license key or Volume license key for a machine..  </v>
       </c>
     </row>
-    <row r="71" spans="1:19" ht="45">
+    <row r="71" spans="1:19" ht="68">
       <c r="A71" s="7" t="s">
         <v>311</v>
       </c>
@@ -6952,7 +6944,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_IsFlightingInternal: &lt;/b&gt;Flighting' in Windows Defender context means making new development features available as soon as possible, during the development cycle. This does not refer to a public release. The 'internal' most likely means the Window Insider community.  </v>
       </c>
     </row>
-    <row r="72" spans="1:19" ht="135">
+    <row r="72" spans="1:19" ht="170">
       <c r="A72" s="7" t="s">
         <v>268</v>
       </c>
@@ -6973,10 +6965,10 @@
         <v>1.7866E-2</v>
       </c>
       <c r="G72" s="14" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="H72" s="7" t="s">
-        <v>411</v>
+        <v>439</v>
       </c>
       <c r="I72" s="7" t="e">
         <f>VLOOKUP(C72,OBJECT!A:C,3,FALSE)</f>
@@ -7023,7 +7015,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_IsFlightsDisabled: &lt;/b&gt;Indicates if the machine is participating in flighting..  </v>
       </c>
     </row>
-    <row r="73" spans="1:19" ht="45">
+    <row r="73" spans="1:19" ht="51">
       <c r="A73" s="7" t="s">
         <v>269</v>
       </c>
@@ -7092,7 +7084,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_FlightRing: &lt;/b&gt;The ring that the device user would like to receive flights for. This might be different from the ring of the OS which is currently installed if the user changes the ring after getting a flight from a different ring..  </v>
       </c>
     </row>
-    <row r="74" spans="1:19" ht="45">
+    <row r="74" spans="1:19" ht="68">
       <c r="A74" s="7" t="s">
         <v>223</v>
       </c>
@@ -7113,10 +7105,10 @@
         <v>0.636208</v>
       </c>
       <c r="G74" s="14" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="H74" s="7" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="I74" s="7" t="e">
         <f>VLOOKUP(C74,OBJECT!A:C,3,FALSE)</f>
@@ -7163,7 +7155,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_ThresholdOptIn: &lt;/b&gt;NA.  </v>
       </c>
     </row>
-    <row r="75" spans="1:19" ht="30">
+    <row r="75" spans="1:19" ht="34">
       <c r="A75" s="7" t="s">
         <v>223</v>
       </c>
@@ -7184,10 +7176,10 @@
         <v>2.0698000000000001E-2</v>
       </c>
       <c r="G75" s="14" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="H75" s="7" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="I75" s="7" t="e">
         <f>VLOOKUP(C75,OBJECT!A:C,3,FALSE)</f>
@@ -7234,7 +7226,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_FirmwareManufacturerIdentifier: &lt;/b&gt;NA.  </v>
       </c>
     </row>
-    <row r="76" spans="1:19" ht="30">
+    <row r="76" spans="1:19" ht="34">
       <c r="A76" s="7" t="s">
         <v>223</v>
       </c>
@@ -7255,10 +7247,10 @@
         <v>1.8121999999999999E-2</v>
       </c>
       <c r="G76" s="14" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="H76" s="7" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="I76" s="7" t="e">
         <f>VLOOKUP(C76,OBJECT!A:C,3,FALSE)</f>
@@ -7305,7 +7297,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_FirmwareVersionIdentifier: &lt;/b&gt;NA.  </v>
       </c>
     </row>
-    <row r="77" spans="1:19" ht="30">
+    <row r="77" spans="1:19" ht="34">
       <c r="A77" s="7" t="s">
         <v>276</v>
       </c>
@@ -7327,7 +7319,7 @@
       </c>
       <c r="G77" s="14"/>
       <c r="H77" s="7" t="s">
-        <v>406</v>
+        <v>440</v>
       </c>
       <c r="I77" s="7" t="e">
         <f>VLOOKUP(C77,OBJECT!A:C,3,FALSE)</f>
@@ -7374,7 +7366,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_IsSecureBootEnabled: &lt;/b&gt;Indicates if Secure Boot mode is enabled. Secure Boot is a security measure to protect against malware during early system startup..  </v>
       </c>
     </row>
-    <row r="78" spans="1:19" ht="45">
+    <row r="78" spans="1:19" ht="51">
       <c r="A78" s="7" t="s">
         <v>275</v>
       </c>
@@ -7445,7 +7437,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_IsWIMBootEnabled: &lt;/b&gt;wimboot is a boot loader for Windows Imaging Format .wim files. It enables you to boot into a Windows PE (WinPE) deployment or recovery environment..  </v>
       </c>
     </row>
-    <row r="79" spans="1:19" ht="60">
+    <row r="79" spans="1:19" ht="68">
       <c r="A79" s="7" t="s">
         <v>270</v>
       </c>
@@ -7466,10 +7458,10 @@
         <v>1.802E-3</v>
       </c>
       <c r="G79" s="14" t="s">
+        <v>403</v>
+      </c>
+      <c r="H79" s="7" t="s">
         <v>404</v>
-      </c>
-      <c r="H79" s="7" t="s">
-        <v>405</v>
       </c>
       <c r="I79" s="7" t="e">
         <f>VLOOKUP(C79,OBJECT!A:C,3,FALSE)</f>
@@ -7516,7 +7508,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_IsVirtualDevice: &lt;/b&gt;Identifies a Virtual Machine (machine learning model).  </v>
       </c>
     </row>
-    <row r="80" spans="1:19" ht="30">
+    <row r="80" spans="1:19" ht="34">
       <c r="A80" s="7" t="s">
         <v>271</v>
       </c>
@@ -7538,7 +7530,7 @@
       </c>
       <c r="G80" s="14"/>
       <c r="H80" s="7" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="I80" s="7" t="e">
         <f>VLOOKUP(C80,OBJECT!A:C,3,FALSE)</f>
@@ -7585,7 +7577,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_IsTouchEnabled: &lt;/b&gt;Is this a touch device ?.  </v>
       </c>
     </row>
-    <row r="81" spans="1:19" ht="30">
+    <row r="81" spans="1:19" ht="34">
       <c r="A81" s="7" t="s">
         <v>272</v>
       </c>
@@ -7607,7 +7599,7 @@
       </c>
       <c r="G81" s="14"/>
       <c r="H81" s="7" t="s">
-        <v>402</v>
+        <v>441</v>
       </c>
       <c r="I81" s="7" t="e">
         <f>VLOOKUP(C81,OBJECT!A:C,3,FALSE)</f>
@@ -7654,7 +7646,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_IsPenCapable: &lt;/b&gt;Is the device capable of pen input ?.  </v>
       </c>
     </row>
-    <row r="82" spans="1:19" ht="45">
+    <row r="82" spans="1:19" ht="68">
       <c r="A82" s="7" t="s">
         <v>273</v>
       </c>
@@ -7725,7 +7717,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_IsAlwaysOnAlwaysConnectedCapable: &lt;/b&gt;Retreives information about whether the battery enables the device to be AlwaysOnAlwaysConnected.  </v>
       </c>
     </row>
-    <row r="83" spans="1:19" ht="45">
+    <row r="83" spans="1:19" ht="68">
       <c r="A83" s="7" t="s">
         <v>274</v>
       </c>
@@ -7796,7 +7788,7 @@
         <v xml:space="preserve">- &lt;b&gt;Wdft_IsGamer: &lt;/b&gt;Indicates whether the device is a gamer device or not based on its hardware combination..  </v>
       </c>
     </row>
-    <row r="84" spans="1:19" ht="60">
+    <row r="84" spans="1:19" ht="68">
       <c r="A84" s="7" t="s">
         <v>312</v>
       </c>
@@ -7867,7 +7859,7 @@
         <v xml:space="preserve">- &lt;b&gt;Wdft_RegionIdentifier: &lt;/b&gt;Region id code.  </v>
       </c>
     </row>
-    <row r="85" spans="1:19" ht="15.75">
+    <row r="85" spans="1:19" ht="17">
       <c r="A85" s="10" t="s">
         <v>213</v>
       </c>
@@ -7951,7 +7943,7 @@
       <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7966,11 +7958,11 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="20.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="43" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -8105,13 +8097,13 @@
       <selection activeCell="C74" sqref="C74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="51.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="51.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -9724,10 +9716,10 @@
       <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="39.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">

</xml_diff>

<commit_message>
limpieza nulos y etc
</commit_message>
<xml_diff>
--- a/mmp_info.xlsx
+++ b/mmp_info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alinaoganesyan/Desktop/Master Data Science/Entregables/Trabajos/Repositorio entregable 2/Entregable_MMP/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\DataScience\Material didáctico\Ejercicios\Modelo_supervisado\Entregable_MMP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9293642-DF77-B54D-A126-CD5D887A7777}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45F19F66-3974-42CF-8654-634B24694E7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{16D500F6-5AD7-764E-8C39-1ED26FBE09BA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="2" xr2:uid="{16D500F6-5AD7-764E-8C39-1ED26FBE09BA}"/>
   </bookViews>
   <sheets>
     <sheet name="INFO" sheetId="1" r:id="rId1"/>
@@ -22,17 +22,28 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">INFO!$A$1:$T$85</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="776" uniqueCount="442">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="781" uniqueCount="443">
   <si>
     <t>TIPO DATOS</t>
   </si>
@@ -913,9 +924,6 @@
   </si>
   <si>
     <t>Limpieza de atributos y transformación de variables</t>
-  </si>
-  <si>
-    <t>Númericas a categóricas</t>
   </si>
   <si>
     <t>Imputación de nulos</t>
@@ -1207,9 +1215,6 @@
     <t>Se correlaciona con OsBuild en 0.93. Eliminamos ya que vemos un comportamiento distinto en la distribución de registros extremos.</t>
   </si>
   <si>
-    <t>Se correlaciona -0.88 con SxSPassiveMode, se podría considerar eliminar aunque mejor no, porque no es tan alto. Los valores se concentran en 7 y 0. Los demas se podrían agrupar. El valor de 35 es claramente un outlier</t>
-  </si>
-  <si>
     <t>Eliminar. Bool con todos los valores 0 excepto 1 valor (=1). Debido a la distribución del violin plot, solo un valor negativo de in beta te dice que está infectado x malware, por lo que no tiene sentido mantenerla.</t>
   </si>
   <si>
@@ -1292,9 +1297,6 @@
   </si>
   <si>
     <t>Transformar NaN a un valor random, pe -1</t>
-  </si>
-  <si>
-    <t>Transformar NaN a valor -1 o qualquier random, solo tiene 7 Trues… quizás eliminar ya que podría aprender?</t>
   </si>
   <si>
     <t xml:space="preserve">Bool, la ayoria son False o cero. </t>
@@ -1394,6 +1396,18 @@
   </si>
   <si>
     <t>Debería ser bool. Predomina el 0. Distribución bastante equiparable del target</t>
+  </si>
+  <si>
+    <t>Se correlaciona -0.88 con SxSPassiveMode, se podría considerar eliminar aunque mejor no, porque no es tan alto. Los valores se concentran en 7 y 0. Los demas se podrían agrupar. El valor de 35 es claramente un outlier. Si vale la pena en var categoricas agrupar las que son minoritarias.</t>
+  </si>
+  <si>
+    <t>Tiene demasiados valores únicos como para ser analizado con gráfico de barras. Habrá que analizarlo aparte.  Engine, App y AvSig se refieren a lo mismo.</t>
+  </si>
+  <si>
+    <t>Eliminar columnas</t>
+  </si>
+  <si>
+    <t>NúmericasID a categóricas</t>
   </si>
 </sst>
 </file>
@@ -1454,7 +1468,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1470,6 +1484,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1502,7 +1522,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1542,10 +1562,13 @@
     <xf numFmtId="11" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="10" fontId="5" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1972,30 +1995,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1355D624-ACBD-7B41-A30E-75FD1558C62F}">
   <dimension ref="A1:S85"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H82" sqref="H82"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="85.1640625" style="7" customWidth="1"/>
-    <col min="2" max="2" width="18.33203125" style="7" customWidth="1"/>
+    <col min="1" max="1" width="85.125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="18.375" style="7" customWidth="1"/>
     <col min="3" max="3" width="46" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="13.1640625" style="7" customWidth="1"/>
-    <col min="7" max="7" width="14.1640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="61.33203125" style="7" customWidth="1"/>
+    <col min="4" max="6" width="13.125" style="7" customWidth="1"/>
+    <col min="7" max="7" width="14.125" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="61.375" style="7" customWidth="1"/>
     <col min="9" max="9" width="20" style="7" customWidth="1"/>
-    <col min="10" max="10" width="10.83203125" style="7"/>
-    <col min="11" max="11" width="16.83203125" style="15" customWidth="1"/>
-    <col min="12" max="12" width="19.33203125" style="16" customWidth="1"/>
-    <col min="13" max="13" width="22.83203125" style="7" customWidth="1"/>
-    <col min="14" max="18" width="10.83203125" style="7"/>
-    <col min="19" max="19" width="87.83203125" style="7" customWidth="1"/>
-    <col min="20" max="16384" width="10.83203125" style="7"/>
+    <col min="10" max="10" width="10.875" style="7"/>
+    <col min="11" max="11" width="16.875" style="15" customWidth="1"/>
+    <col min="12" max="12" width="19.375" style="16" customWidth="1"/>
+    <col min="13" max="13" width="22.875" style="7" customWidth="1"/>
+    <col min="14" max="18" width="10.875" style="7"/>
+    <col min="19" max="19" width="87.875" style="7" customWidth="1"/>
+    <col min="20" max="16384" width="10.875" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="13" customFormat="1" ht="17">
+    <row r="1" spans="1:19" s="13" customFormat="1" ht="15.75">
       <c r="A1" s="6" t="s">
         <v>211</v>
       </c>
@@ -2015,7 +2038,7 @@
         <v>98</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H1" s="6" t="s">
         <v>3</v>
@@ -2051,7 +2074,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="51">
+    <row r="2" spans="1:19" ht="30">
       <c r="A2" s="7" t="s">
         <v>212</v>
       </c>
@@ -2071,8 +2094,8 @@
         <f xml:space="preserve"> E2/500000</f>
         <v>0</v>
       </c>
-      <c r="G2" s="14" t="s">
-        <v>350</v>
+      <c r="G2" s="17" t="s">
+        <v>349</v>
       </c>
       <c r="H2" s="7" t="s">
         <v>278</v>
@@ -2122,7 +2145,7 @@
         <v xml:space="preserve">- &lt;b&gt;Unnamed: 0: &lt;/b&gt;index.  </v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="68">
+    <row r="3" spans="1:19" ht="60">
       <c r="A3" s="7" t="s">
         <v>218</v>
       </c>
@@ -2142,9 +2165,11 @@
         <f t="shared" ref="F3:F66" si="0" xml:space="preserve"> E3/500000</f>
         <v>0</v>
       </c>
-      <c r="G3" s="14"/>
+      <c r="G3" s="17" t="s">
+        <v>349</v>
+      </c>
       <c r="H3" s="8" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="I3" s="7">
         <f>VLOOKUP(C3,OBJECT!A:C,3,FALSE)</f>
@@ -2191,7 +2216,7 @@
         <v xml:space="preserve">- &lt;b&gt;MachineIdentifier: &lt;/b&gt;Individual machine ID.  </v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="119">
+    <row r="4" spans="1:19" ht="90">
       <c r="B4" s="7" t="s">
         <v>95</v>
       </c>
@@ -2210,7 +2235,7 @@
       </c>
       <c r="G4" s="14"/>
       <c r="H4" s="8" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="I4" s="7">
         <f>VLOOKUP(C4,OBJECT!A:C,3,FALSE)</f>
@@ -2257,7 +2282,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="68">
+    <row r="5" spans="1:19" ht="60">
       <c r="A5" s="7" t="s">
         <v>219</v>
       </c>
@@ -2279,7 +2304,7 @@
       </c>
       <c r="G5" s="14"/>
       <c r="H5" s="7" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="I5" s="7">
         <f>VLOOKUP(C5,OBJECT!A:C,3,FALSE)</f>
@@ -2326,7 +2351,7 @@
         <v xml:space="preserve">- &lt;b&gt;EngineVersion: &lt;/b&gt;Defender state information e.g. 1.1.12603.0.  </v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="51">
+    <row r="6" spans="1:19" ht="30">
       <c r="A6" s="7" t="s">
         <v>220</v>
       </c>
@@ -2346,9 +2371,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G6" s="14"/>
+      <c r="G6" s="17" t="s">
+        <v>349</v>
+      </c>
       <c r="H6" s="7" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="I6" s="7">
         <f>VLOOKUP(C6,OBJECT!A:C,3,FALSE)</f>
@@ -2395,7 +2422,7 @@
         <v xml:space="preserve">- &lt;b&gt;AppVersion: &lt;/b&gt;Defender state information e.g. 4.9.10586.0.  </v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="34">
+    <row r="7" spans="1:19" ht="45">
       <c r="A7" s="7" t="s">
         <v>221</v>
       </c>
@@ -2415,9 +2442,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G7" s="14"/>
+      <c r="G7" s="17" t="s">
+        <v>349</v>
+      </c>
       <c r="H7" s="8" t="s">
-        <v>353</v>
+        <v>440</v>
       </c>
       <c r="I7" s="7">
         <f>VLOOKUP(C7,OBJECT!A:C,3,FALSE)</f>
@@ -2464,7 +2493,7 @@
         <v xml:space="preserve">- &lt;b&gt;AvSigVersion: &lt;/b&gt;Defender state information e.g. 1.217.1014.0.  </v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="68">
+    <row r="8" spans="1:19" ht="60">
       <c r="A8" s="7" t="s">
         <v>222</v>
       </c>
@@ -2484,11 +2513,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G8" s="14" t="s">
-        <v>350</v>
+      <c r="G8" s="17" t="s">
+        <v>349</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="I8" s="7" t="e">
         <f>VLOOKUP(C8,OBJECT!A:C,3,FALSE)</f>
@@ -2535,16 +2564,14 @@
         <v xml:space="preserve">- &lt;b&gt;IsBeta: &lt;/b&gt;Defender state information e.g. false.  </v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="119">
+    <row r="9" spans="1:19" ht="105">
       <c r="A9" s="7" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="C9" s="10" t="s">
-        <v>17</v>
-      </c>
+      <c r="C9" s="10"/>
       <c r="D9" s="7">
         <v>498168</v>
       </c>
@@ -2556,10 +2583,10 @@
         <v>3.6640000000000002E-3</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>380</v>
+        <v>439</v>
       </c>
       <c r="I9" s="7" t="e">
         <f>VLOOKUP(C9,OBJECT!A:C,3,FALSE)</f>
@@ -2573,42 +2600,42 @@
         <f>VLOOKUP(C9,OBJECT!$A$2:$E$31,5,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="L9" s="16">
+      <c r="L9" s="16" t="e">
         <f>VLOOKUP(C9,STATS!$A$2:$I$55,3,0)</f>
-        <v>6846207</v>
-      </c>
-      <c r="M9" s="16">
+        <v>#N/A</v>
+      </c>
+      <c r="M9" s="16" t="e">
         <f>VLOOKUP(C9,STATS!$A$1:$I$55,4,0)</f>
-        <v>1023049</v>
-      </c>
-      <c r="N9" s="16" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="N9" s="16" t="e">
         <f>VLOOKUP(C9,STATS!$A$1:$I$55,5,0)</f>
-        <v>0.0</v>
-      </c>
-      <c r="O9" s="16" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="O9" s="16" t="e">
         <f>VLOOKUP(C9,STATS!$A$1:$I$55,6,0)</f>
-        <v>7.00</v>
-      </c>
-      <c r="P9" s="16" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="P9" s="16" t="e">
         <f>VLOOKUP(C9,STATS!$A$1:$I$55,7,0)</f>
-        <v>7.0</v>
-      </c>
-      <c r="Q9" s="16">
+        <v>#N/A</v>
+      </c>
+      <c r="Q9" s="16" t="e">
         <f>VLOOKUP(C9,STATS!$A$1:$I$55,8,0)</f>
-        <v>7000000</v>
-      </c>
-      <c r="R9" s="16">
+        <v>#N/A</v>
+      </c>
+      <c r="R9" s="16" t="e">
         <f>VLOOKUP(C9,STATS!$A$1:$I$55,9,0)</f>
-        <v>35000000</v>
+        <v>#N/A</v>
       </c>
       <c r="S9" s="7" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">- &lt;b&gt;RtpStateBitfield: &lt;/b&gt;RTP state: Realtime protection state (Enabled or Disabled).  </v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" ht="170">
+        <v xml:space="preserve">- &lt;b&gt;: &lt;/b&gt;RTP state: Realtime protection state (Enabled or Disabled).  </v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="150">
       <c r="A10" s="7" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>94</v>
@@ -2627,10 +2654,10 @@
         <v>0</v>
       </c>
       <c r="G10" s="14" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="I10" s="7" t="e">
         <f>VLOOKUP(C10,OBJECT!A:C,3,FALSE)</f>
@@ -2677,7 +2704,7 @@
         <v xml:space="preserve">- &lt;b&gt;IsSxsPassiveMode: &lt;/b&gt;active/passive mode of operation for Windows Defender. If another third party primary antivirus exists on the system, the Defender enters Passive mode. Passive mode obviously offers reduced functionality.  </v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="17">
+    <row r="11" spans="1:19" ht="15.75">
       <c r="A11" s="7" t="s">
         <v>224</v>
       </c>
@@ -2697,11 +2724,11 @@
         <f t="shared" si="0"/>
         <v>0.951878</v>
       </c>
-      <c r="G11" s="14" t="s">
-        <v>350</v>
+      <c r="G11" s="17" t="s">
+        <v>349</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="I11" s="7" t="e">
         <f>VLOOKUP(C11,OBJECT!A:C,3,FALSE)</f>
@@ -2748,7 +2775,7 @@
         <v xml:space="preserve">- &lt;b&gt;DefaultBrowsersIdentifier: &lt;/b&gt;ID for the machine's default browser.  </v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="102">
+    <row r="12" spans="1:19" ht="75">
       <c r="A12" s="7" t="s">
         <v>225</v>
       </c>
@@ -2769,10 +2796,10 @@
         <v>3.8760000000000001E-3</v>
       </c>
       <c r="G12" s="14" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="I12" s="7" t="e">
         <f>VLOOKUP(C12,OBJECT!A:C,3,FALSE)</f>
@@ -2819,9 +2846,9 @@
         <v xml:space="preserve">- &lt;b&gt;AVProductStatesIdentifier: &lt;/b&gt;ID for the specific configuration of a user's antivirus software.  </v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="68">
+    <row r="13" spans="1:19" ht="60">
       <c r="A13" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>96</v>
@@ -2840,10 +2867,10 @@
         <v>3.8760000000000001E-3</v>
       </c>
       <c r="G13" s="14" t="s">
+        <v>384</v>
+      </c>
+      <c r="H13" s="7" t="s">
         <v>386</v>
-      </c>
-      <c r="H13" s="7" t="s">
-        <v>388</v>
       </c>
       <c r="I13" s="7" t="e">
         <f>VLOOKUP(C13,OBJECT!A:C,3,FALSE)</f>
@@ -2890,9 +2917,9 @@
         <v xml:space="preserve">- &lt;b&gt;AVProductsInstalled: &lt;/b&gt;Active anti-virus of the total installed.  </v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="68">
+    <row r="14" spans="1:19" ht="60">
       <c r="A14" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>96</v>
@@ -2911,10 +2938,10 @@
         <v>3.8760000000000001E-3</v>
       </c>
       <c r="G14" s="14" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="I14" s="7" t="e">
         <f>VLOOKUP(C14,OBJECT!A:C,3,FALSE)</f>
@@ -2961,7 +2988,7 @@
         <v xml:space="preserve">- &lt;b&gt;AVProductsEnabled: &lt;/b&gt;Of the installed antiviruses, those that are active.  </v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="34">
+    <row r="15" spans="1:19" ht="30">
       <c r="A15" s="7" t="s">
         <v>226</v>
       </c>
@@ -2983,7 +3010,7 @@
       </c>
       <c r="G15" s="14"/>
       <c r="H15" s="7" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="I15" s="7" t="e">
         <f>VLOOKUP(C15,OBJECT!A:C,3,FALSE)</f>
@@ -3030,7 +3057,7 @@
         <v xml:space="preserve">- &lt;b&gt;HasTpm: &lt;/b&gt;True if machine has tpm.  </v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="85">
+    <row r="16" spans="1:19" ht="75">
       <c r="A16" s="7" t="s">
         <v>227</v>
       </c>
@@ -3050,11 +3077,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G16" s="14" t="s">
-        <v>350</v>
+      <c r="G16" s="17" t="s">
+        <v>349</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="I16" s="7" t="e">
         <f>VLOOKUP(C16,OBJECT!A:C,3,FALSE)</f>
@@ -3101,7 +3128,7 @@
         <v xml:space="preserve">- &lt;b&gt;CountryIdentifier: &lt;/b&gt;ID for the country the machine is located in.  </v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="85">
+    <row r="17" spans="1:19" ht="75">
       <c r="A17" s="7" t="s">
         <v>228</v>
       </c>
@@ -3121,11 +3148,11 @@
         <f t="shared" si="0"/>
         <v>3.6479999999999999E-2</v>
       </c>
-      <c r="G17" s="14" t="s">
-        <v>392</v>
+      <c r="G17" s="17" t="s">
+        <v>390</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="I17" s="7" t="e">
         <f>VLOOKUP(C17,OBJECT!A:C,3,FALSE)</f>
@@ -3172,7 +3199,7 @@
         <v xml:space="preserve">- &lt;b&gt;CityIdentifier: &lt;/b&gt;ID for the city the machine is located in.  </v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="68">
+    <row r="18" spans="1:19" ht="60">
       <c r="A18" s="7" t="s">
         <v>229</v>
       </c>
@@ -3193,10 +3220,10 @@
         <v>0.30912600000000001</v>
       </c>
       <c r="G18" s="14" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="I18" s="7" t="e">
         <f>VLOOKUP(C18,OBJECT!A:C,3,FALSE)</f>
@@ -3243,7 +3270,7 @@
         <v xml:space="preserve">- &lt;b&gt;OrganizationIdentifier: &lt;/b&gt;ID for the organization the machine belongs in, organization ID is mapped to both specific companies and broad industries.  </v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="51">
+    <row r="19" spans="1:19" ht="45">
       <c r="A19" s="7" t="s">
         <v>230</v>
       </c>
@@ -3264,10 +3291,10 @@
         <v>3.1999999999999999E-5</v>
       </c>
       <c r="G19" s="14" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="I19" s="7" t="e">
         <f>VLOOKUP(C19,OBJECT!A:C,3,FALSE)</f>
@@ -3314,7 +3341,7 @@
         <v xml:space="preserve">- &lt;b&gt;GeoNameIdentifier: &lt;/b&gt;ID for the geographic region a machine is located in.  </v>
       </c>
     </row>
-    <row r="20" spans="1:19" ht="51">
+    <row r="20" spans="1:19" ht="15.75">
       <c r="A20" s="7" t="s">
         <v>231</v>
       </c>
@@ -3334,11 +3361,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G20" s="14" t="s">
+      <c r="G20" s="17" t="s">
+        <v>349</v>
+      </c>
+      <c r="H20" s="7" t="s">
         <v>394</v>
-      </c>
-      <c r="H20" s="7" t="s">
-        <v>396</v>
       </c>
       <c r="I20" s="7" t="e">
         <f>VLOOKUP(C20,OBJECT!A:C,3,FALSE)</f>
@@ -3385,7 +3412,7 @@
         <v xml:space="preserve">- &lt;b&gt;LocaleEnglishNameIdentifier: &lt;/b&gt;English name of Locale ID of the current user.  </v>
       </c>
     </row>
-    <row r="21" spans="1:19" ht="68">
+    <row r="21" spans="1:19" ht="45">
       <c r="A21" s="7" t="s">
         <v>232</v>
       </c>
@@ -3407,7 +3434,7 @@
       </c>
       <c r="G21" s="14"/>
       <c r="H21" s="8" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I21" s="7">
         <f>VLOOKUP(C21,OBJECT!A:C,3,FALSE)</f>
@@ -3454,7 +3481,7 @@
         <v xml:space="preserve">- &lt;b&gt;Platform: &lt;/b&gt;Calculates platform name (of OS related properties and processor property).  </v>
       </c>
     </row>
-    <row r="22" spans="1:19" ht="102">
+    <row r="22" spans="1:19" ht="90">
       <c r="A22" s="7" t="s">
         <v>233</v>
       </c>
@@ -3476,7 +3503,7 @@
       </c>
       <c r="G22" s="14"/>
       <c r="H22" s="8" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I22" s="7">
         <f>VLOOKUP(C22,OBJECT!A:C,3,FALSE)</f>
@@ -3523,7 +3550,7 @@
         <v xml:space="preserve">- &lt;b&gt;Processor: &lt;/b&gt;This is the process architecture of the installed operating system.  </v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="51">
+    <row r="23" spans="1:19" ht="45">
       <c r="A23" s="7" t="s">
         <v>234</v>
       </c>
@@ -3545,7 +3572,7 @@
       </c>
       <c r="G23" s="14"/>
       <c r="H23" s="8" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="I23" s="7">
         <f>VLOOKUP(C23,OBJECT!A:C,3,FALSE)</f>
@@ -3592,7 +3619,7 @@
         <v xml:space="preserve">- &lt;b&gt;OsVer: &lt;/b&gt;Version of the current operating system.  </v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="68">
+    <row r="24" spans="1:19" ht="60">
       <c r="A24" s="7" t="s">
         <v>235</v>
       </c>
@@ -3614,7 +3641,7 @@
       </c>
       <c r="G24" s="14"/>
       <c r="H24" s="7" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="I24" s="7" t="e">
         <f>VLOOKUP(C24,OBJECT!A:C,3,FALSE)</f>
@@ -3661,7 +3688,7 @@
         <v xml:space="preserve">- &lt;b&gt;OsBuild: &lt;/b&gt;Build of the current operating system.  </v>
       </c>
     </row>
-    <row r="25" spans="1:19" ht="17">
+    <row r="25" spans="1:19" ht="15.75">
       <c r="A25" s="7" t="s">
         <v>236</v>
       </c>
@@ -3682,10 +3709,10 @@
         <v>0</v>
       </c>
       <c r="G25" s="14" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I25" s="7" t="e">
         <f>VLOOKUP(C25,OBJECT!A:C,3,FALSE)</f>
@@ -3732,7 +3759,7 @@
         <v xml:space="preserve">- &lt;b&gt;OsSuite: &lt;/b&gt;Product suite mask for the current operating system..  </v>
       </c>
     </row>
-    <row r="26" spans="1:19" ht="85">
+    <row r="26" spans="1:19" ht="60">
       <c r="A26" s="7" t="s">
         <v>237</v>
       </c>
@@ -3754,7 +3781,7 @@
       </c>
       <c r="G26" s="14"/>
       <c r="H26" s="7" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="I26" s="7">
         <f>VLOOKUP(C26,OBJECT!A:C,3,FALSE)</f>
@@ -3801,7 +3828,7 @@
         <v xml:space="preserve">- &lt;b&gt;OsPlatformSubRelease: &lt;/b&gt;Returns the OS Platform sub.  </v>
       </c>
     </row>
-    <row r="27" spans="1:19" ht="85">
+    <row r="27" spans="1:19" ht="75">
       <c r="A27" s="7" t="s">
         <v>238</v>
       </c>
@@ -3823,7 +3850,7 @@
       </c>
       <c r="G27" s="14"/>
       <c r="H27" s="8" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="I27" s="7">
         <f>VLOOKUP(C27,OBJECT!A:C,3,FALSE)</f>
@@ -3870,7 +3897,7 @@
         <v xml:space="preserve">- &lt;b&gt;OsBuildLab: &lt;/b&gt;Build lab that generated the current OS. Example: 9600.17630.amd64fre.winblue_r7.150109.  </v>
       </c>
     </row>
-    <row r="28" spans="1:19" ht="90">
+    <row r="28" spans="1:19" ht="82.5">
       <c r="A28" s="7" t="s">
         <v>277</v>
       </c>
@@ -3892,7 +3919,7 @@
       </c>
       <c r="G28" s="14"/>
       <c r="H28" s="9" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="I28" s="7">
         <f>VLOOKUP(C28,OBJECT!A:C,3,FALSE)</f>
@@ -3939,7 +3966,7 @@
         <v xml:space="preserve">- &lt;b&gt;SkuEdition: &lt;/b&gt;The goal of this feature is to use the Product Type defined in the MSDN (Microsoft Developer Network) to map to a SKU (Stock Keeping Unit).  </v>
       </c>
     </row>
-    <row r="29" spans="1:19" ht="34">
+    <row r="29" spans="1:19" ht="30">
       <c r="A29" s="7" t="s">
         <v>239</v>
       </c>
@@ -3960,10 +3987,10 @@
         <v>3.852E-3</v>
       </c>
       <c r="G29" s="14" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="H29" s="7" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="I29" s="7" t="e">
         <f>VLOOKUP(C29,OBJECT!A:C,3,FALSE)</f>
@@ -4010,7 +4037,7 @@
         <v xml:space="preserve">- &lt;b&gt;IsProtected: &lt;/b&gt;This is a calculated field derived from the Spynet Report's AV Products field. Returns: a. TRUE if there is at least one active and up.  </v>
       </c>
     </row>
-    <row r="30" spans="1:19" ht="34">
+    <row r="30" spans="1:19" ht="30">
       <c r="A30" s="7" t="s">
         <v>240</v>
       </c>
@@ -4030,9 +4057,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G30" s="14"/>
+      <c r="G30" s="17" t="s">
+        <v>349</v>
+      </c>
       <c r="H30" s="7" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="I30" s="7" t="e">
         <f>VLOOKUP(C30,OBJECT!A:C,3,FALSE)</f>
@@ -4079,7 +4108,7 @@
         <v xml:space="preserve">- &lt;b&gt;AutoSampleOptIn: &lt;/b&gt;This is the SubmitSamplesConsent value passed in from the service, available on CAMP 9+.  </v>
       </c>
     </row>
-    <row r="31" spans="1:19" ht="17">
+    <row r="31" spans="1:19" ht="15.75">
       <c r="A31" s="7" t="s">
         <v>241</v>
       </c>
@@ -4099,11 +4128,11 @@
         <f t="shared" si="0"/>
         <v>0.99974799999999997</v>
       </c>
-      <c r="G31" s="14" t="s">
-        <v>350</v>
+      <c r="G31" s="17" t="s">
+        <v>349</v>
       </c>
       <c r="H31" s="7" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="I31" s="7">
         <f>VLOOKUP(C31,OBJECT!A:C,3,FALSE)</f>
@@ -4150,7 +4179,7 @@
         <v xml:space="preserve">- &lt;b&gt;PuaMode: &lt;/b&gt;Pua Enabled mode from the service.  </v>
       </c>
     </row>
-    <row r="32" spans="1:19" ht="51">
+    <row r="32" spans="1:19" ht="45">
       <c r="A32" s="7" t="s">
         <v>242</v>
       </c>
@@ -4170,11 +4199,11 @@
         <f t="shared" si="0"/>
         <v>5.9695999999999999E-2</v>
       </c>
-      <c r="G32" s="14" t="s">
-        <v>429</v>
+      <c r="G32" s="17" t="s">
+        <v>349</v>
       </c>
       <c r="H32" s="7" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="I32" s="7" t="e">
         <f>VLOOKUP(C32,OBJECT!A:C,3,FALSE)</f>
@@ -4221,9 +4250,9 @@
         <v xml:space="preserve">- &lt;b&gt;SMode: &lt;/b&gt;This field is set to true when the device is known to be in 'S Mode', as in, Windows 10 S mode, where only Microsoft Store apps can be installed.  </v>
       </c>
     </row>
-    <row r="33" spans="1:19" ht="34">
+    <row r="33" spans="1:19" ht="30">
       <c r="A33" s="7" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B33" s="7" t="s">
         <v>96</v>
@@ -4242,10 +4271,10 @@
         <v>6.4180000000000001E-3</v>
       </c>
       <c r="G33" s="14" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="H33" s="7" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="I33" s="7" t="e">
         <f>VLOOKUP(C33,OBJECT!A:C,3,FALSE)</f>
@@ -4292,7 +4321,7 @@
         <v xml:space="preserve">- &lt;b&gt;IeVerIdentifier: &lt;/b&gt;Retrieves which version of Internet Explorer is running on this device.  </v>
       </c>
     </row>
-    <row r="34" spans="1:19" ht="136">
+    <row r="34" spans="1:19" ht="121.5">
       <c r="A34" s="7" t="s">
         <v>243</v>
       </c>
@@ -4313,10 +4342,10 @@
         <v>0.35719200000000001</v>
       </c>
       <c r="G34" s="14" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="H34" s="8" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="I34" s="7">
         <f>VLOOKUP(C34,OBJECT!A:C,3,FALSE)</f>
@@ -4363,7 +4392,7 @@
         <v xml:space="preserve">- &lt;b&gt;SmartScreen: &lt;/b&gt;This is the SmartScreen enabled string value from registry. This is obtained by checking in order, HKLM\SOFTWARE\Policies\Microsoft\Windows\System\SmartScreenEnabled and HKLM\SOFTWARE\Microsoft\Windows\CurrentVersion\Explorer\SmartScreenEnabled. If the value exists but is blank, the value "ExistsNotSet" is sent in telemetry..  </v>
       </c>
     </row>
-    <row r="35" spans="1:19" ht="34">
+    <row r="35" spans="1:19" ht="30">
       <c r="A35" s="7" t="s">
         <v>244</v>
       </c>
@@ -4384,10 +4413,10 @@
         <v>1.0324E-2</v>
       </c>
       <c r="G35" s="14" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="H35" s="7" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="I35" s="7" t="e">
         <f>VLOOKUP(C35,OBJECT!A:C,3,FALSE)</f>
@@ -4434,7 +4463,7 @@
         <v xml:space="preserve">- &lt;b&gt;Firewall: &lt;/b&gt;This attribute is true (1) for Windows 8.1 and above if windows firewall is enabled, as reported by the service..  </v>
       </c>
     </row>
-    <row r="36" spans="1:19" ht="68">
+    <row r="36" spans="1:19" ht="60">
       <c r="A36" s="7" t="s">
         <v>245</v>
       </c>
@@ -4456,7 +4485,7 @@
       </c>
       <c r="G36" s="14"/>
       <c r="H36" s="7" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="I36" s="7" t="e">
         <f>VLOOKUP(C36,OBJECT!A:C,3,FALSE)</f>
@@ -4503,7 +4532,7 @@
         <v xml:space="preserve">- &lt;b&gt;UacLuaenable: &lt;/b&gt;This attribute reports whether or not the "administrator in Admin Approval Mode" user type is disabled or enabled in UAC. The value reported is obtained by reading the regkey HKLM\SOFTWARE\Microsoft\Windows\CurrentVersion\Policies\System\EnableLUA..  </v>
       </c>
     </row>
-    <row r="37" spans="1:19" ht="85">
+    <row r="37" spans="1:19" ht="75">
       <c r="A37" s="7" t="s">
         <v>246</v>
       </c>
@@ -4525,7 +4554,7 @@
       </c>
       <c r="G37" s="14"/>
       <c r="H37" s="8" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="I37" s="7">
         <f>VLOOKUP(C37,OBJECT!A:C,3,FALSE)</f>
@@ -4572,7 +4601,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_MDC2FormFactor: &lt;/b&gt;A grouping based on a combination of Device Census level hardware characteristics. The logic used to define Form Factor is rooted in business and industry standards and aligns with how people think about their device. (Examples: Smartphone, Small Tablet, All in One, Convertible...).  </v>
       </c>
     </row>
-    <row r="38" spans="1:19" ht="68">
+    <row r="38" spans="1:19" ht="60">
       <c r="A38" s="7" t="s">
         <v>247</v>
       </c>
@@ -4594,7 +4623,7 @@
       </c>
       <c r="G38" s="14"/>
       <c r="H38" s="8" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="I38" s="7">
         <f>VLOOKUP(C38,OBJECT!A:C,3,FALSE)</f>
@@ -4641,7 +4670,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_DeviceFamily: &lt;/b&gt;AKA DeviceClass. Indicates the type of device that an edition of the OS is intended for. Example values: Windows.Desktop, Windows.Mobile, and iOS.Phone.  </v>
       </c>
     </row>
-    <row r="39" spans="1:19" ht="34">
+    <row r="39" spans="1:19" ht="15.75">
       <c r="A39" s="7" t="s">
         <v>223</v>
       </c>
@@ -4662,10 +4691,10 @@
         <v>1.0762000000000001E-2</v>
       </c>
       <c r="G39" s="14" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="H39" s="7" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="I39" s="7" t="e">
         <f>VLOOKUP(C39,OBJECT!A:C,3,FALSE)</f>
@@ -4712,7 +4741,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_OEMNameIdentifier: &lt;/b&gt;NA.  </v>
       </c>
     </row>
-    <row r="40" spans="1:19" ht="34">
+    <row r="40" spans="1:19" ht="15.75">
       <c r="A40" s="7" t="s">
         <v>223</v>
       </c>
@@ -4733,10 +4762,10 @@
         <v>1.1528E-2</v>
       </c>
       <c r="G40" s="14" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="H40" s="7" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="I40" s="7" t="e">
         <f>VLOOKUP(C40,OBJECT!A:C,3,FALSE)</f>
@@ -4783,7 +4812,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_OEMModelIdentifier: &lt;/b&gt;NA.  </v>
       </c>
     </row>
-    <row r="41" spans="1:19" ht="68">
+    <row r="41" spans="1:19" ht="45">
       <c r="A41" s="7" t="s">
         <v>248</v>
       </c>
@@ -4804,10 +4833,10 @@
         <v>4.6940000000000003E-3</v>
       </c>
       <c r="G41" s="14" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="H41" s="7" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="I41" s="7" t="e">
         <f>VLOOKUP(C41,OBJECT!A:C,3,FALSE)</f>
@@ -4854,7 +4883,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_ProcessorCoreCount: &lt;/b&gt;Number of logical cores in the processor.  </v>
       </c>
     </row>
-    <row r="42" spans="1:19" ht="68">
+    <row r="42" spans="1:19" ht="60">
       <c r="A42" s="7" t="s">
         <v>223</v>
       </c>
@@ -4875,10 +4904,10 @@
         <v>4.6940000000000003E-3</v>
       </c>
       <c r="G42" s="14" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="H42" s="7" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="I42" s="7" t="e">
         <f>VLOOKUP(C42,OBJECT!A:C,3,FALSE)</f>
@@ -4925,7 +4954,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_ProcessorManufacturerIdentifier: &lt;/b&gt;NA.  </v>
       </c>
     </row>
-    <row r="43" spans="1:19" ht="17">
+    <row r="43" spans="1:19" ht="15.75">
       <c r="A43" s="7" t="s">
         <v>223</v>
       </c>
@@ -4946,10 +4975,10 @@
         <v>4.6979999999999999E-3</v>
       </c>
       <c r="G43" s="14" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="H43" s="7" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="I43" s="7" t="e">
         <f>VLOOKUP(C43,OBJECT!A:C,3,FALSE)</f>
@@ -4996,7 +5025,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_ProcessorModelIdentifier: &lt;/b&gt;NA.  </v>
       </c>
     </row>
-    <row r="44" spans="1:19" ht="34">
+    <row r="44" spans="1:19" ht="30">
       <c r="A44" s="7" t="s">
         <v>249</v>
       </c>
@@ -5016,11 +5045,11 @@
         <f t="shared" si="0"/>
         <v>0.99583600000000005</v>
       </c>
-      <c r="G44" s="14" t="s">
-        <v>350</v>
+      <c r="G44" s="17" t="s">
+        <v>349</v>
       </c>
       <c r="H44" s="7" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="I44" s="7">
         <f>VLOOKUP(C44,OBJECT!A:C,3,FALSE)</f>
@@ -5067,7 +5096,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_ProcessorClass: &lt;/b&gt;A classification of processors into high/medium/low. Initially used for Pricing Level SKU. No longer maintained and updated.  </v>
       </c>
     </row>
-    <row r="45" spans="1:19" ht="34">
+    <row r="45" spans="1:19" ht="30">
       <c r="A45" s="7" t="s">
         <v>215</v>
       </c>
@@ -5089,7 +5118,7 @@
       </c>
       <c r="G45" s="14"/>
       <c r="H45" s="7" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="I45" s="7" t="e">
         <f>VLOOKUP(C45,OBJECT!A:C,3,FALSE)</f>
@@ -5136,7 +5165,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_PrimaryDiskTotalCapacity: &lt;/b&gt;Amount of disk space on primary disk of the machine in MB.  </v>
       </c>
     </row>
-    <row r="46" spans="1:19" ht="51">
+    <row r="46" spans="1:19" ht="45">
       <c r="A46" s="7" t="s">
         <v>216</v>
       </c>
@@ -5158,7 +5187,7 @@
       </c>
       <c r="G46" s="14"/>
       <c r="H46" s="7" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="I46" s="7">
         <f>VLOOKUP(C46,OBJECT!A:C,3,FALSE)</f>
@@ -5205,7 +5234,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_PrimaryDiskTypeName: &lt;/b&gt;Friendly name of Primary Disk Type .  </v>
       </c>
     </row>
-    <row r="47" spans="1:19" ht="68">
+    <row r="47" spans="1:19" ht="60">
       <c r="A47" s="7" t="s">
         <v>217</v>
       </c>
@@ -5226,10 +5255,10 @@
         <v>5.9519999999999998E-3</v>
       </c>
       <c r="G47" s="14" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="H47" s="7" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="I47" s="7" t="e">
         <f>VLOOKUP(C47,OBJECT!A:C,3,FALSE)</f>
@@ -5276,7 +5305,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_SystemVolumeTotalCapacity: &lt;/b&gt;The size of the partition that the System volume is installed on in MB.  </v>
       </c>
     </row>
-    <row r="48" spans="1:19" ht="34">
+    <row r="48" spans="1:19" ht="30">
       <c r="A48" s="7" t="s">
         <v>250</v>
       </c>
@@ -5298,7 +5327,7 @@
       </c>
       <c r="G48" s="14"/>
       <c r="H48" s="7" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="I48" s="7" t="e">
         <f>VLOOKUP(C48,OBJECT!A:C,3,FALSE)</f>
@@ -5345,7 +5374,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_HasOpticalDiskDrive: &lt;/b&gt;True indicates that the machine has an optical disk drive (CD/DVD).  </v>
       </c>
     </row>
-    <row r="49" spans="1:19" ht="51">
+    <row r="49" spans="1:19" ht="45">
       <c r="A49" s="7" t="s">
         <v>251</v>
       </c>
@@ -5366,10 +5395,10 @@
         <v>9.1120000000000003E-3</v>
       </c>
       <c r="G49" s="14" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="H49" s="7" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="I49" s="7" t="e">
         <f>VLOOKUP(C49,OBJECT!A:C,3,FALSE)</f>
@@ -5416,7 +5445,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_TotalPhysicalRAM: &lt;/b&gt;Retrieves the physical RAM in MB.  </v>
       </c>
     </row>
-    <row r="50" spans="1:19" ht="51">
+    <row r="50" spans="1:19" ht="45">
       <c r="A50" s="7" t="s">
         <v>252</v>
       </c>
@@ -5438,7 +5467,7 @@
       </c>
       <c r="G50" s="14"/>
       <c r="H50" s="8" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="I50" s="7">
         <f>VLOOKUP(C50,OBJECT!A:C,3,FALSE)</f>
@@ -5485,7 +5514,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_ChassisTypeName: &lt;/b&gt;Retrieves a numeric representation of what type of chassis the machine has. A value of 0 means xx.  </v>
       </c>
     </row>
-    <row r="51" spans="1:19" ht="68">
+    <row r="51" spans="1:19" ht="60">
       <c r="A51" s="7" t="s">
         <v>253</v>
       </c>
@@ -5506,10 +5535,10 @@
         <v>5.3080000000000002E-3</v>
       </c>
       <c r="G51" s="14" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="H51" s="7" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="I51" s="7" t="e">
         <f>VLOOKUP(C51,OBJECT!A:C,3,FALSE)</f>
@@ -5556,7 +5585,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_InternalPrimaryDiagonalDisplaySizeInInches: &lt;/b&gt;Retrieves the physical diagonal length in inches of the primary display.  </v>
       </c>
     </row>
-    <row r="52" spans="1:19" ht="68">
+    <row r="52" spans="1:19" ht="60">
       <c r="A52" s="7" t="s">
         <v>254</v>
       </c>
@@ -5578,7 +5607,7 @@
       </c>
       <c r="G52" s="14"/>
       <c r="H52" s="7" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="I52" s="7" t="e">
         <f>VLOOKUP(C52,OBJECT!A:C,3,FALSE)</f>
@@ -5625,7 +5654,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_InternalPrimaryDisplayResolutionHorizontal: &lt;/b&gt;Retrieves the number of pixels in the horizontal direction of the internal display..  </v>
       </c>
     </row>
-    <row r="53" spans="1:19" ht="68">
+    <row r="53" spans="1:19" ht="60">
       <c r="A53" s="7" t="s">
         <v>255</v>
       </c>
@@ -5647,7 +5676,7 @@
       </c>
       <c r="G53" s="14"/>
       <c r="H53" s="7" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="I53" s="7" t="e">
         <f>VLOOKUP(C53,OBJECT!A:C,3,FALSE)</f>
@@ -5694,7 +5723,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_InternalPrimaryDisplayResolutionVertical: &lt;/b&gt;Retrieves the number of pixels in the vertical direction of the internal display.  </v>
       </c>
     </row>
-    <row r="54" spans="1:19" ht="51">
+    <row r="54" spans="1:19" ht="45">
       <c r="A54" s="7" t="s">
         <v>214</v>
       </c>
@@ -5716,7 +5745,7 @@
       </c>
       <c r="G54" s="14"/>
       <c r="H54" s="8" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="I54" s="7">
         <f>VLOOKUP(C54,OBJECT!A:C,3,FALSE)</f>
@@ -5763,7 +5792,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_PowerPlatformRoleName: &lt;/b&gt;Indicates the OEM preferred power management profile. This value helps identify the basic form factor of the device.  </v>
       </c>
     </row>
-    <row r="55" spans="1:19" ht="68">
+    <row r="55" spans="1:19" ht="60">
       <c r="A55" s="7" t="s">
         <v>223</v>
       </c>
@@ -5785,7 +5814,7 @@
       </c>
       <c r="G55" s="14"/>
       <c r="H55" s="8" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="I55" s="7">
         <f>VLOOKUP(C55,OBJECT!A:C,3,FALSE)</f>
@@ -5832,7 +5861,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_InternalBatteryType: &lt;/b&gt;NA.  </v>
       </c>
     </row>
-    <row r="56" spans="1:19" ht="102">
+    <row r="56" spans="1:19" ht="90">
       <c r="A56" s="7" t="s">
         <v>223</v>
       </c>
@@ -5854,7 +5883,7 @@
       </c>
       <c r="G56" s="14"/>
       <c r="H56" s="7" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="I56" s="7" t="e">
         <f>VLOOKUP(C56,OBJECT!A:C,3,FALSE)</f>
@@ -5901,7 +5930,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_InternalBatteryNumberOfCharges: &lt;/b&gt;NA.  </v>
       </c>
     </row>
-    <row r="57" spans="1:19" ht="34">
+    <row r="57" spans="1:19" ht="30">
       <c r="A57" s="7" t="s">
         <v>256</v>
       </c>
@@ -5923,7 +5952,7 @@
       </c>
       <c r="G57" s="14"/>
       <c r="H57" s="8" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="I57" s="7">
         <f>VLOOKUP(C57,OBJECT!A:C,3,FALSE)</f>
@@ -5970,7 +5999,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_OSVersion: &lt;/b&gt;Numeric OS version Example .  </v>
       </c>
     </row>
-    <row r="58" spans="1:19" ht="85">
+    <row r="58" spans="1:19" ht="75">
       <c r="A58" s="7" t="s">
         <v>257</v>
       </c>
@@ -5992,7 +6021,7 @@
       </c>
       <c r="G58" s="14"/>
       <c r="H58" s="8" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="I58" s="7">
         <f>VLOOKUP(C58,OBJECT!A:C,3,FALSE)</f>
@@ -6039,7 +6068,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_OSArchitecture: &lt;/b&gt;Architecture on which the OS is based. Derived from OSVersionFull. Example .  </v>
       </c>
     </row>
-    <row r="59" spans="1:19" ht="85">
+    <row r="59" spans="1:19" ht="75">
       <c r="A59" s="7" t="s">
         <v>258</v>
       </c>
@@ -6061,7 +6090,7 @@
       </c>
       <c r="G59" s="14"/>
       <c r="H59" s="8" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="I59" s="7">
         <f>VLOOKUP(C59,OBJECT!A:C,3,FALSE)</f>
@@ -6108,7 +6137,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_OSBranch: &lt;/b&gt;Branch of the OS extracted from the OsVersionFull. Example .  </v>
       </c>
     </row>
-    <row r="60" spans="1:19" ht="51">
+    <row r="60" spans="1:19" ht="30">
       <c r="A60" s="7" t="s">
         <v>259</v>
       </c>
@@ -6128,9 +6157,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G60" s="14"/>
+      <c r="G60" s="17" t="s">
+        <v>349</v>
+      </c>
       <c r="H60" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="I60" s="7" t="e">
         <f>VLOOKUP(C60,OBJECT!A:C,3,FALSE)</f>
@@ -6177,7 +6208,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_OSBuildNumber: &lt;/b&gt;OS Build number extracted from the OsVersionFull. Example .  </v>
       </c>
     </row>
-    <row r="61" spans="1:19" ht="51">
+    <row r="61" spans="1:19" ht="45">
       <c r="A61" s="7" t="s">
         <v>260</v>
       </c>
@@ -6198,10 +6229,10 @@
         <v>0</v>
       </c>
       <c r="G61" s="14" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="H61" s="7" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="I61" s="7" t="e">
         <f>VLOOKUP(C61,OBJECT!A:C,3,FALSE)</f>
@@ -6248,7 +6279,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_OSBuildRevision: &lt;/b&gt;OS Build revision extracted from the OsVersionFull. Example .  </v>
       </c>
     </row>
-    <row r="62" spans="1:19" ht="68">
+    <row r="62" spans="1:19" ht="60">
       <c r="A62" s="7" t="s">
         <v>261</v>
       </c>
@@ -6270,7 +6301,7 @@
       </c>
       <c r="G62" s="14"/>
       <c r="H62" s="8" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="I62" s="7">
         <f>VLOOKUP(C62,OBJECT!A:C,3,FALSE)</f>
@@ -6317,7 +6348,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_OSEdition: &lt;/b&gt;Edition of the current OS. Sourced from HKLM\Software\Microsoft\Windows NT\CurrentVersion@EditionID in registry. Example: Enterprise.  </v>
       </c>
     </row>
-    <row r="63" spans="1:19" ht="51">
+    <row r="63" spans="1:19" ht="45">
       <c r="A63" s="7" t="s">
         <v>262</v>
       </c>
@@ -6339,7 +6370,7 @@
       </c>
       <c r="G63" s="14"/>
       <c r="H63" s="8" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="I63" s="7">
         <f>VLOOKUP(C63,OBJECT!A:C,3,FALSE)</f>
@@ -6386,7 +6417,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_OSSkuName: &lt;/b&gt;OS edition friendly name (currently Windows only).  </v>
       </c>
     </row>
-    <row r="64" spans="1:19" ht="51">
+    <row r="64" spans="1:19" ht="45">
       <c r="A64" s="7" t="s">
         <v>263</v>
       </c>
@@ -6408,7 +6439,7 @@
       </c>
       <c r="G64" s="14"/>
       <c r="H64" s="7" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="I64" s="7">
         <f>VLOOKUP(C64,OBJECT!A:C,3,FALSE)</f>
@@ -6455,7 +6486,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_OSInstallTypeName: &lt;/b&gt;Friendly description of what install was used on the machine i.e. clean.  </v>
       </c>
     </row>
-    <row r="65" spans="1:19" ht="34">
+    <row r="65" spans="1:19" ht="30">
       <c r="A65" s="7" t="s">
         <v>223</v>
       </c>
@@ -6475,11 +6506,11 @@
         <f t="shared" si="0"/>
         <v>6.6639999999999998E-3</v>
       </c>
-      <c r="G65" s="14" t="s">
-        <v>350</v>
+      <c r="G65" s="17" t="s">
+        <v>349</v>
       </c>
       <c r="H65" s="7" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="I65" s="7" t="e">
         <f>VLOOKUP(C65,OBJECT!A:C,3,FALSE)</f>
@@ -6526,7 +6557,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_OSInstallLanguageIdentifier: &lt;/b&gt;NA.  </v>
       </c>
     </row>
-    <row r="66" spans="1:19" ht="68">
+    <row r="66" spans="1:19" ht="60">
       <c r="A66" s="7" t="s">
         <v>223</v>
       </c>
@@ -6547,10 +6578,10 @@
         <v>0</v>
       </c>
       <c r="G66" s="14" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="H66" s="7" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="I66" s="7" t="e">
         <f>VLOOKUP(C66,OBJECT!A:C,3,FALSE)</f>
@@ -6597,7 +6628,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_OSUILocaleIdentifier: &lt;/b&gt;NA.  </v>
       </c>
     </row>
-    <row r="67" spans="1:19" ht="68">
+    <row r="67" spans="1:19" ht="60">
       <c r="A67" s="7" t="s">
         <v>264</v>
       </c>
@@ -6619,7 +6650,7 @@
       </c>
       <c r="G67" s="14"/>
       <c r="H67" s="8" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="I67" s="7">
         <f>VLOOKUP(C67,OBJECT!A:C,3,FALSE)</f>
@@ -6666,7 +6697,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_OSWUAutoUpdateOptionsName: &lt;/b&gt;Friendly name of the WindowsUpdate auto.  </v>
       </c>
     </row>
-    <row r="68" spans="1:19" ht="34">
+    <row r="68" spans="1:19" ht="30">
       <c r="A68" s="7" t="s">
         <v>265</v>
       </c>
@@ -6688,7 +6719,7 @@
       </c>
       <c r="G68" s="14"/>
       <c r="H68" s="7" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="I68" s="7" t="e">
         <f>VLOOKUP(C68,OBJECT!A:C,3,FALSE)</f>
@@ -6735,7 +6766,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_IsPortableOperatingSystem: &lt;/b&gt;Indicates whether OS is booted up and running via Windows.  </v>
       </c>
     </row>
-    <row r="69" spans="1:19" ht="34">
+    <row r="69" spans="1:19" ht="30">
       <c r="A69" s="7" t="s">
         <v>266</v>
       </c>
@@ -6757,7 +6788,7 @@
       </c>
       <c r="G69" s="14"/>
       <c r="H69" s="8" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="I69" s="7">
         <f>VLOOKUP(C69,OBJECT!A:C,3,FALSE)</f>
@@ -6804,7 +6835,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_GenuineStateName: &lt;/b&gt;Friendly name of OSGenuineStateID. 0 = Genuine.  </v>
       </c>
     </row>
-    <row r="70" spans="1:19" ht="51">
+    <row r="70" spans="1:19" ht="45">
       <c r="A70" s="7" t="s">
         <v>267</v>
       </c>
@@ -6826,7 +6857,7 @@
       </c>
       <c r="G70" s="14"/>
       <c r="H70" s="8" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="I70" s="7">
         <f>VLOOKUP(C70,OBJECT!A:C,3,FALSE)</f>
@@ -6873,9 +6904,9 @@
         <v xml:space="preserve">- &lt;b&gt;Census_ActivationChannel: &lt;/b&gt;Retail license key or Volume license key for a machine..  </v>
       </c>
     </row>
-    <row r="71" spans="1:19" ht="68">
+    <row r="71" spans="1:19" ht="45">
       <c r="A71" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B71" s="7" t="s">
         <v>96</v>
@@ -6893,11 +6924,11 @@
         <f t="shared" si="2"/>
         <v>0.83045000000000002</v>
       </c>
-      <c r="G71" s="14" t="s">
-        <v>350</v>
+      <c r="G71" s="17" t="s">
+        <v>349</v>
       </c>
       <c r="H71" s="7" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="I71" s="7" t="e">
         <f>VLOOKUP(C71,OBJECT!A:C,3,FALSE)</f>
@@ -6944,7 +6975,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_IsFlightingInternal: &lt;/b&gt;Flighting' in Windows Defender context means making new development features available as soon as possible, during the development cycle. This does not refer to a public release. The 'internal' most likely means the Window Insider community.  </v>
       </c>
     </row>
-    <row r="72" spans="1:19" ht="170">
+    <row r="72" spans="1:19" ht="45">
       <c r="A72" s="7" t="s">
         <v>268</v>
       </c>
@@ -6964,11 +6995,11 @@
         <f t="shared" si="2"/>
         <v>1.7866E-2</v>
       </c>
-      <c r="G72" s="14" t="s">
-        <v>409</v>
+      <c r="G72" s="17" t="s">
+        <v>349</v>
       </c>
       <c r="H72" s="7" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="I72" s="7" t="e">
         <f>VLOOKUP(C72,OBJECT!A:C,3,FALSE)</f>
@@ -7015,7 +7046,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_IsFlightsDisabled: &lt;/b&gt;Indicates if the machine is participating in flighting..  </v>
       </c>
     </row>
-    <row r="73" spans="1:19" ht="51">
+    <row r="73" spans="1:19" ht="45">
       <c r="A73" s="7" t="s">
         <v>269</v>
       </c>
@@ -7037,7 +7068,7 @@
       </c>
       <c r="G73" s="14"/>
       <c r="H73" s="8" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="I73" s="7">
         <f>VLOOKUP(C73,OBJECT!A:C,3,FALSE)</f>
@@ -7084,7 +7115,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_FlightRing: &lt;/b&gt;The ring that the device user would like to receive flights for. This might be different from the ring of the OS which is currently installed if the user changes the ring after getting a flight from a different ring..  </v>
       </c>
     </row>
-    <row r="74" spans="1:19" ht="68">
+    <row r="74" spans="1:19" ht="45">
       <c r="A74" s="7" t="s">
         <v>223</v>
       </c>
@@ -7105,10 +7136,10 @@
         <v>0.636208</v>
       </c>
       <c r="G74" s="14" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="H74" s="7" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="I74" s="7" t="e">
         <f>VLOOKUP(C74,OBJECT!A:C,3,FALSE)</f>
@@ -7155,7 +7186,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_ThresholdOptIn: &lt;/b&gt;NA.  </v>
       </c>
     </row>
-    <row r="75" spans="1:19" ht="34">
+    <row r="75" spans="1:19" ht="30">
       <c r="A75" s="7" t="s">
         <v>223</v>
       </c>
@@ -7176,10 +7207,10 @@
         <v>2.0698000000000001E-2</v>
       </c>
       <c r="G75" s="14" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H75" s="7" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="I75" s="7" t="e">
         <f>VLOOKUP(C75,OBJECT!A:C,3,FALSE)</f>
@@ -7226,7 +7257,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_FirmwareManufacturerIdentifier: &lt;/b&gt;NA.  </v>
       </c>
     </row>
-    <row r="76" spans="1:19" ht="34">
+    <row r="76" spans="1:19" ht="30">
       <c r="A76" s="7" t="s">
         <v>223</v>
       </c>
@@ -7247,10 +7278,10 @@
         <v>1.8121999999999999E-2</v>
       </c>
       <c r="G76" s="14" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H76" s="7" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="I76" s="7" t="e">
         <f>VLOOKUP(C76,OBJECT!A:C,3,FALSE)</f>
@@ -7297,7 +7328,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_FirmwareVersionIdentifier: &lt;/b&gt;NA.  </v>
       </c>
     </row>
-    <row r="77" spans="1:19" ht="34">
+    <row r="77" spans="1:19" ht="30">
       <c r="A77" s="7" t="s">
         <v>276</v>
       </c>
@@ -7319,7 +7350,7 @@
       </c>
       <c r="G77" s="14"/>
       <c r="H77" s="7" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="I77" s="7" t="e">
         <f>VLOOKUP(C77,OBJECT!A:C,3,FALSE)</f>
@@ -7366,7 +7397,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_IsSecureBootEnabled: &lt;/b&gt;Indicates if Secure Boot mode is enabled. Secure Boot is a security measure to protect against malware during early system startup..  </v>
       </c>
     </row>
-    <row r="78" spans="1:19" ht="51">
+    <row r="78" spans="1:19" ht="45">
       <c r="A78" s="7" t="s">
         <v>275</v>
       </c>
@@ -7386,11 +7417,11 @@
         <f t="shared" si="2"/>
         <v>0.63533200000000001</v>
       </c>
-      <c r="G78" s="14" t="s">
-        <v>350</v>
+      <c r="G78" s="17" t="s">
+        <v>349</v>
       </c>
       <c r="H78" s="7" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="I78" s="7" t="e">
         <f>VLOOKUP(C78,OBJECT!A:C,3,FALSE)</f>
@@ -7437,7 +7468,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_IsWIMBootEnabled: &lt;/b&gt;wimboot is a boot loader for Windows Imaging Format .wim files. It enables you to boot into a Windows PE (WinPE) deployment or recovery environment..  </v>
       </c>
     </row>
-    <row r="79" spans="1:19" ht="68">
+    <row r="79" spans="1:19" ht="60">
       <c r="A79" s="7" t="s">
         <v>270</v>
       </c>
@@ -7458,10 +7489,10 @@
         <v>1.802E-3</v>
       </c>
       <c r="G79" s="14" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="H79" s="7" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="I79" s="7" t="e">
         <f>VLOOKUP(C79,OBJECT!A:C,3,FALSE)</f>
@@ -7508,7 +7539,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_IsVirtualDevice: &lt;/b&gt;Identifies a Virtual Machine (machine learning model).  </v>
       </c>
     </row>
-    <row r="80" spans="1:19" ht="34">
+    <row r="80" spans="1:19" ht="30">
       <c r="A80" s="7" t="s">
         <v>271</v>
       </c>
@@ -7530,7 +7561,7 @@
       </c>
       <c r="G80" s="14"/>
       <c r="H80" s="7" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="I80" s="7" t="e">
         <f>VLOOKUP(C80,OBJECT!A:C,3,FALSE)</f>
@@ -7577,7 +7608,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_IsTouchEnabled: &lt;/b&gt;Is this a touch device ?.  </v>
       </c>
     </row>
-    <row r="81" spans="1:19" ht="34">
+    <row r="81" spans="1:19" ht="30">
       <c r="A81" s="7" t="s">
         <v>272</v>
       </c>
@@ -7599,7 +7630,7 @@
       </c>
       <c r="G81" s="14"/>
       <c r="H81" s="7" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="I81" s="7" t="e">
         <f>VLOOKUP(C81,OBJECT!A:C,3,FALSE)</f>
@@ -7646,7 +7677,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_IsPenCapable: &lt;/b&gt;Is the device capable of pen input ?.  </v>
       </c>
     </row>
-    <row r="82" spans="1:19" ht="68">
+    <row r="82" spans="1:19" ht="45">
       <c r="A82" s="7" t="s">
         <v>273</v>
       </c>
@@ -7667,10 +7698,10 @@
         <v>8.0800000000000004E-3</v>
       </c>
       <c r="G82" s="14" t="s">
+        <v>397</v>
+      </c>
+      <c r="H82" s="7" t="s">
         <v>399</v>
-      </c>
-      <c r="H82" s="7" t="s">
-        <v>401</v>
       </c>
       <c r="I82" s="7" t="e">
         <f>VLOOKUP(C82,OBJECT!A:C,3,FALSE)</f>
@@ -7717,7 +7748,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_IsAlwaysOnAlwaysConnectedCapable: &lt;/b&gt;Retreives information about whether the battery enables the device to be AlwaysOnAlwaysConnected.  </v>
       </c>
     </row>
-    <row r="83" spans="1:19" ht="68">
+    <row r="83" spans="1:19" ht="45">
       <c r="A83" s="7" t="s">
         <v>274</v>
       </c>
@@ -7738,10 +7769,10 @@
         <v>3.39E-2</v>
       </c>
       <c r="G83" s="14" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="H83" s="7" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="I83" s="7" t="e">
         <f>VLOOKUP(C83,OBJECT!A:C,3,FALSE)</f>
@@ -7788,9 +7819,9 @@
         <v xml:space="preserve">- &lt;b&gt;Wdft_IsGamer: &lt;/b&gt;Indicates whether the device is a gamer device or not based on its hardware combination..  </v>
       </c>
     </row>
-    <row r="84" spans="1:19" ht="68">
+    <row r="84" spans="1:19" ht="60">
       <c r="A84" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B84" s="7" t="s">
         <v>96</v>
@@ -7809,10 +7840,10 @@
         <v>3.39E-2</v>
       </c>
       <c r="G84" s="14" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="H84" s="7" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="I84" s="7" t="e">
         <f>VLOOKUP(C84,OBJECT!A:C,3,FALSE)</f>
@@ -7859,7 +7890,7 @@
         <v xml:space="preserve">- &lt;b&gt;Wdft_RegionIdentifier: &lt;/b&gt;Region id code.  </v>
       </c>
     </row>
-    <row r="85" spans="1:19" ht="17">
+    <row r="85" spans="1:19" ht="15.75">
       <c r="A85" s="10" t="s">
         <v>213</v>
       </c>
@@ -7881,7 +7912,7 @@
       </c>
       <c r="G85" s="14"/>
       <c r="H85" s="10" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="I85" s="7" t="e">
         <f>VLOOKUP(C85,OBJECT!A:C,3,FALSE)</f>
@@ -7943,7 +7974,7 @@
       <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7954,15 +7985,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63F36F59-B644-4A4B-A18E-D4BF69C056EB}">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="20.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="43" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -8002,8 +8033,13 @@
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="C7" t="s">
+      <c r="C7" s="5" t="s">
         <v>287</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="C8" s="5" t="s">
+        <v>441</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -8013,75 +8049,75 @@
       <c r="B9" t="s">
         <v>289</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="5" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="C10" s="5" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
-      <c r="C10" t="s">
+    <row r="11" spans="1:3">
+      <c r="C11" s="5" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
-      <c r="C11" t="s">
+    <row r="12" spans="1:3">
+      <c r="C12" s="5" t="s">
         <v>292</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="C12" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="C13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
+        <v>294</v>
+      </c>
+      <c r="B15" t="s">
         <v>295</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>296</v>
-      </c>
-      <c r="C15" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="17" spans="2:3">
       <c r="B17" t="s">
+        <v>297</v>
+      </c>
+      <c r="C17" t="s">
         <v>298</v>
-      </c>
-      <c r="C17" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="19" spans="2:3">
       <c r="B19" t="s">
+        <v>299</v>
+      </c>
+      <c r="C19" t="s">
         <v>300</v>
-      </c>
-      <c r="C19" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="20" spans="2:3">
       <c r="C20" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="21" spans="2:3">
       <c r="C21" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="22" spans="2:3">
       <c r="C22" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="23" spans="2:3">
       <c r="C23" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
   </sheetData>
@@ -8097,13 +8133,13 @@
       <selection activeCell="C74" sqref="C74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="51.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="51.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.875" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -9716,10 +9752,10 @@
       <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="39.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -9727,13 +9763,13 @@
         <v>99</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>314</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -9747,7 +9783,7 @@
         <v>500000</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E2" s="3">
         <v>1</v>
@@ -9764,7 +9800,7 @@
         <v>3</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E3" s="3">
         <v>494604</v>
@@ -9781,7 +9817,7 @@
         <v>53</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E4" s="3">
         <v>216491</v>
@@ -9798,7 +9834,7 @@
         <v>95</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E5" s="3">
         <v>288809</v>
@@ -9815,7 +9851,7 @@
         <v>6455</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E6" s="3">
         <v>5771</v>
@@ -9832,7 +9868,7 @@
         <v>4</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E7" s="3">
         <v>483048</v>
@@ -9849,7 +9885,7 @@
         <v>3</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E8" s="3">
         <v>454423</v>
@@ -9866,7 +9902,7 @@
         <v>21</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E9" s="3">
         <v>483830</v>
@@ -9883,7 +9919,7 @@
         <v>9</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E10" s="3">
         <v>220779</v>
@@ -9900,7 +9936,7 @@
         <v>453</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E11" s="3">
         <v>206436</v>
@@ -9917,7 +9953,7 @@
         <v>8</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E12" s="3">
         <v>308567</v>
@@ -9934,7 +9970,7 @@
         <v>1</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E13" s="3">
         <v>126</v>
@@ -9951,7 +9987,7 @@
         <v>12</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E14" s="3">
         <v>241594</v>
@@ -9968,7 +10004,7 @@
         <v>12</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E15" s="3">
         <v>320948</v>
@@ -9985,7 +10021,7 @@
         <v>3</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E16" s="3">
         <v>499183</v>
@@ -10002,7 +10038,7 @@
         <v>3</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E17" s="3">
         <v>1196</v>
@@ -10019,7 +10055,7 @@
         <v>4</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E18" s="3">
         <v>325429</v>
@@ -10036,7 +10072,7 @@
         <v>34</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E19" s="3">
         <v>294232</v>
@@ -10053,7 +10089,7 @@
         <v>9</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E20" s="3">
         <v>346378</v>
@@ -10070,7 +10106,7 @@
         <v>28</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E21" s="3">
         <v>113500</v>
@@ -10087,7 +10123,7 @@
         <v>305</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E22" s="3">
         <v>79975</v>
@@ -10104,7 +10140,7 @@
         <v>3</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E23" s="3">
         <v>454435</v>
@@ -10121,7 +10157,7 @@
         <v>15</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E24" s="3">
         <v>226001</v>
@@ -10138,7 +10174,7 @@
         <v>22</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E25" s="3">
         <v>194469</v>
@@ -10155,7 +10191,7 @@
         <v>21</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E26" s="3">
         <v>194464</v>
@@ -10172,7 +10208,7 @@
         <v>9</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E27" s="3">
         <v>146780</v>
@@ -10189,7 +10225,7 @@
         <v>6</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E28" s="3">
         <v>222482</v>
@@ -10206,7 +10242,7 @@
         <v>4</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E29" s="3">
         <v>441402</v>
@@ -10223,7 +10259,7 @@
         <v>6</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E30" s="3">
         <v>264932</v>
@@ -10240,7 +10276,7 @@
         <v>8</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E31" s="3">
         <v>468299</v>

</xml_diff>

<commit_message>
Preparación del OHE y frequency encoding
</commit_message>
<xml_diff>
--- a/mmp_info.xlsx
+++ b/mmp_info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\DataScience\Material didáctico\Ejercicios\Modelo_supervisado\Entregable_MMP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45F19F66-3974-42CF-8654-634B24694E7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C152E0A-2318-428A-8BEA-FA71692C5585}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="2" xr2:uid="{16D500F6-5AD7-764E-8C39-1ED26FBE09BA}"/>
+    <workbookView xWindow="23880" yWindow="-7695" windowWidth="29040" windowHeight="15840" xr2:uid="{16D500F6-5AD7-764E-8C39-1ED26FBE09BA}"/>
   </bookViews>
   <sheets>
     <sheet name="INFO" sheetId="1" r:id="rId1"/>
@@ -1995,9 +1995,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1355D624-ACBD-7B41-A30E-75FD1558C62F}">
   <dimension ref="A1:S85"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A73" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G50" sqref="G50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15"/>
@@ -4670,7 +4670,7 @@
         <v xml:space="preserve">- &lt;b&gt;Census_DeviceFamily: &lt;/b&gt;AKA DeviceClass. Indicates the type of device that an edition of the OS is intended for. Example values: Windows.Desktop, Windows.Mobile, and iOS.Phone.  </v>
       </c>
     </row>
-    <row r="39" spans="1:19" ht="15.75">
+    <row r="39" spans="1:19" ht="24" customHeight="1">
       <c r="A39" s="7" t="s">
         <v>223</v>
       </c>
@@ -7985,7 +7985,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63F36F59-B644-4A4B-A18E-D4BF69C056EB}">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update excel hasta tratamiento cat
</commit_message>
<xml_diff>
--- a/mmp_info.xlsx
+++ b/mmp_info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\DataScience\Material didáctico\Ejercicios\Modelo_supervisado\Entregable_MMP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C152E0A-2318-428A-8BEA-FA71692C5585}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{252470B9-62E2-451B-B83C-FD40D2C39AB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23880" yWindow="-7695" windowWidth="29040" windowHeight="15840" xr2:uid="{16D500F6-5AD7-764E-8C39-1ED26FBE09BA}"/>
+    <workbookView xWindow="23880" yWindow="-7695" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{16D500F6-5AD7-764E-8C39-1ED26FBE09BA}"/>
   </bookViews>
   <sheets>
     <sheet name="INFO" sheetId="1" r:id="rId1"/>
@@ -1414,7 +1414,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1466,6 +1466,14 @@
       <color theme="1"/>
       <name val="Helvetica Neue"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1522,7 +1530,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1565,6 +1573,7 @@
     <xf numFmtId="10" fontId="5" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1995,9 +2004,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1355D624-ACBD-7B41-A30E-75FD1558C62F}">
   <dimension ref="A1:S85"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A73" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G50" sqref="G50"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A72" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O28" sqref="O28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15"/>
@@ -7985,8 +7994,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63F36F59-B644-4A4B-A18E-D4BF69C056EB}">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
@@ -8069,7 +8078,7 @@
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="C13" t="s">
+      <c r="C13" s="18" t="s">
         <v>293</v>
       </c>
     </row>
@@ -8122,6 +8131,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
update excel hasta model definition
</commit_message>
<xml_diff>
--- a/mmp_info.xlsx
+++ b/mmp_info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\DataScience\Material didáctico\Ejercicios\Modelo_supervisado\Entregable_MMP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{252470B9-62E2-451B-B83C-FD40D2C39AB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D0BE1D2-C568-47CA-8A86-01E138FA6836}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="23880" yWindow="-7695" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{16D500F6-5AD7-764E-8C39-1ED26FBE09BA}"/>
   </bookViews>
@@ -7995,7 +7995,7 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
@@ -8089,7 +8089,7 @@
       <c r="B15" t="s">
         <v>295</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="5" t="s">
         <v>296</v>
       </c>
     </row>

</xml_diff>